<commit_message>
feat: enhance test result logging and failure handling in Excel updates
</commit_message>
<xml_diff>
--- a/data/BigCommerceData/BigC_Ecomm_TestCases_AutomationMasterSheet.xlsx
+++ b/data/BigCommerceData/BigC_Ecomm_TestCases_AutomationMasterSheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D21C48D-F6CA-4590-B747-B06F4A20D043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC089AE-2690-4CC3-BF04-29B2C64948C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19128" uniqueCount="3187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19138" uniqueCount="3197">
   <si>
     <t>Global Test Case ID</t>
   </si>
@@ -9535,7 +9535,7 @@
     <t>Order_Id</t>
   </si>
   <si>
-    <t>Test_Results</t>
+    <t>Test_Result</t>
   </si>
   <si>
     <t>Execution_Notes</t>
@@ -9568,7 +9568,11 @@
     <t>Standard product order for existing customer</t>
   </si>
   <si>
-    <t>All steps completed successfully</t>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>All steps completed successfully
+[Last updated: 2025-09-10T17:31:58.631Z]</t>
   </si>
   <si>
     <t>USD $20.00</t>
@@ -9577,9 +9581,21 @@
     <t>USD $132.15</t>
   </si>
   <si>
+    <t>All steps completed successfully
+[Last updated: 2025-09-10T17:32:39.439Z]</t>
+  </si>
+  <si>
     <t>Customer transfers money directly to the seller's bank account.</t>
   </si>
   <si>
+    <t>All steps completed successfully
+[Last updated: 2025-09-10T17:33:14.462Z]</t>
+  </si>
+  <si>
+    <t>All steps completed successfully
+[Last updated: 2025-09-10T17:33:55.170Z]</t>
+  </si>
+  <si>
     <t>A real payment gateway/service provider (owned by Visa).</t>
   </si>
   <si>
@@ -9587,6 +9603,26 @@
   </si>
   <si>
     <t>American Express</t>
+  </si>
+  <si>
+    <t>All steps completed successfully
+[Last updated: 2025-09-10T17:34:32.483Z]</t>
+  </si>
+  <si>
+    <t>All steps completed successfully
+[Last updated: 2025-09-10T17:35:14.140Z]</t>
+  </si>
+  <si>
+    <t>Manual payment</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-10T18:03:47.478Z\nScreenshot: test-results/screenshots/TC0247.png","Status: Passed","Last Updated: 2025-09-10T18:03:47.625Z","---"]</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>["=== Test Failure Details ===","Failed Step: Verify Summary and Add Comments","Error Message: Grand Total mismatch. Expected: USD $132.15, Found: USD $152.15","Failure Timestamp: 2025-09-10T18:05:20.590Z","Failure Screenshot: test-results/screenshots/failure_TC0256_1757527520300.png","","=== Additional Notes ===","Test failed during: Verify Summary and Add Comments\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-10T18:05:21.061Z","---"]</t>
   </si>
 </sst>
 </file>
@@ -47127,8 +47163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AN73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="AI20" sqref="AI20"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="AN47" sqref="AN47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -47171,7 +47207,7 @@
     <col min="37" max="37" width="14.33203125" style="3" customWidth="1"/>
     <col min="38" max="38" width="12.5546875" style="3" customWidth="1"/>
     <col min="39" max="39" width="13.77734375" style="3" customWidth="1"/>
-    <col min="40" max="40" width="38.21875" style="3" customWidth="1"/>
+    <col min="40" max="40" width="75.44140625" style="3" customWidth="1"/>
     <col min="41" max="41" width="9.109375" style="3" customWidth="1"/>
     <col min="42" max="16384" width="9.109375" style="3"/>
   </cols>
@@ -47410,8 +47446,11 @@
       <c r="AK2" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="AM2" s="3" t="s">
+        <v>3180</v>
+      </c>
       <c r="AN2" s="3" t="s">
-        <v>3180</v>
+        <v>3181</v>
       </c>
     </row>
     <row r="3" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -47840,7 +47879,7 @@
         <v>3176</v>
       </c>
       <c r="Y11" s="3" t="s">
-        <v>3181</v>
+        <v>3182</v>
       </c>
       <c r="Z11" s="3" t="s">
         <v>3172</v>
@@ -47849,7 +47888,7 @@
         <v>3177</v>
       </c>
       <c r="AB11" s="8" t="s">
-        <v>3182</v>
+        <v>3183</v>
       </c>
       <c r="AC11" s="9">
         <v>0</v>
@@ -47878,8 +47917,11 @@
       <c r="AK11" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="AM11" s="3" t="s">
+        <v>3180</v>
+      </c>
       <c r="AN11" s="3" t="s">
-        <v>3180</v>
+        <v>3184</v>
       </c>
     </row>
     <row r="12" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -48302,7 +48344,7 @@
         <v>123</v>
       </c>
       <c r="W20" s="3" t="s">
-        <v>3183</v>
+        <v>3185</v>
       </c>
       <c r="X20" s="3" t="s">
         <v>3176</v>
@@ -48346,8 +48388,11 @@
       <c r="AK20" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="AM20" s="3" t="s">
+        <v>3180</v>
+      </c>
       <c r="AN20" s="3" t="s">
-        <v>3180</v>
+        <v>3186</v>
       </c>
     </row>
     <row r="21" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -48770,13 +48815,13 @@
         <v>123</v>
       </c>
       <c r="W29" s="3" t="s">
-        <v>3183</v>
+        <v>3185</v>
       </c>
       <c r="X29" s="3" t="s">
         <v>3176</v>
       </c>
       <c r="Y29" s="3" t="s">
-        <v>3181</v>
+        <v>3182</v>
       </c>
       <c r="Z29" s="3" t="s">
         <v>3172</v>
@@ -48785,7 +48830,7 @@
         <v>3177</v>
       </c>
       <c r="AB29" s="8" t="s">
-        <v>3182</v>
+        <v>3183</v>
       </c>
       <c r="AC29" s="9">
         <v>0</v>
@@ -48814,8 +48859,11 @@
       <c r="AK29" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="AM29" s="3" t="s">
+        <v>3180</v>
+      </c>
       <c r="AN29" s="3" t="s">
-        <v>3180</v>
+        <v>3187</v>
       </c>
     </row>
     <row r="30" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -49238,7 +49286,7 @@
         <v>214</v>
       </c>
       <c r="W38" s="3" t="s">
-        <v>3184</v>
+        <v>3188</v>
       </c>
       <c r="X38" s="3" t="s">
         <v>3176</v>
@@ -49265,10 +49313,10 @@
         <v>3179</v>
       </c>
       <c r="AF38" s="3" t="s">
-        <v>3185</v>
+        <v>3189</v>
       </c>
       <c r="AG38" s="3" t="s">
-        <v>3186</v>
+        <v>3190</v>
       </c>
       <c r="AH38" s="3">
         <v>234234523</v>
@@ -49282,8 +49330,11 @@
       <c r="AK38" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="AM38" s="3" t="s">
+        <v>3180</v>
+      </c>
       <c r="AN38" s="3" t="s">
-        <v>3180</v>
+        <v>3191</v>
       </c>
     </row>
     <row r="39" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -49706,13 +49757,13 @@
         <v>214</v>
       </c>
       <c r="W47" s="3" t="s">
-        <v>3184</v>
+        <v>3188</v>
       </c>
       <c r="X47" s="3" t="s">
         <v>3176</v>
       </c>
       <c r="Y47" s="3" t="s">
-        <v>3181</v>
+        <v>3182</v>
       </c>
       <c r="Z47" s="3" t="s">
         <v>3172</v>
@@ -49721,7 +49772,7 @@
         <v>3177</v>
       </c>
       <c r="AB47" s="8" t="s">
-        <v>3182</v>
+        <v>3183</v>
       </c>
       <c r="AC47" s="9">
         <v>0</v>
@@ -49733,10 +49784,10 @@
         <v>3179</v>
       </c>
       <c r="AF47" s="3" t="s">
-        <v>3185</v>
+        <v>3189</v>
       </c>
       <c r="AG47" s="3" t="s">
-        <v>3186</v>
+        <v>3190</v>
       </c>
       <c r="AH47" s="3">
         <v>234234523</v>
@@ -49750,8 +49801,11 @@
       <c r="AK47" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="AM47" s="3" t="s">
+        <v>3180</v>
+      </c>
       <c r="AN47" s="3" t="s">
-        <v>3180</v>
+        <v>3192</v>
       </c>
     </row>
     <row r="48" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -49798,7 +49852,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="49" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>267</v>
       </c>
@@ -49842,7 +49896,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="50" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>272</v>
       </c>
@@ -49886,7 +49940,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="51" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>277</v>
       </c>
@@ -49930,7 +49984,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="52" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>282</v>
       </c>
@@ -49974,7 +50028,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="53" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>287</v>
       </c>
@@ -50018,7 +50072,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="54" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>292</v>
       </c>
@@ -50062,7 +50116,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="55" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>297</v>
       </c>
@@ -50106,7 +50160,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="56" spans="1:37" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:40" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>302</v>
       </c>
@@ -50171,7 +50225,7 @@
         <v>3173</v>
       </c>
       <c r="V56" s="3" t="s">
-        <v>305</v>
+        <v>3193</v>
       </c>
       <c r="W56" s="3" t="s">
         <v>3175</v>
@@ -50218,8 +50272,14 @@
       <c r="AK56" s="3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM56" s="3" t="s">
+        <v>3180</v>
+      </c>
+      <c r="AN56" s="3" t="s">
+        <v>3194</v>
+      </c>
+    </row>
+    <row r="57" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>308</v>
       </c>
@@ -50263,7 +50323,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="58" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>313</v>
       </c>
@@ -50307,7 +50367,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="59" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>318</v>
       </c>
@@ -50351,7 +50411,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="60" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>323</v>
       </c>
@@ -50395,7 +50455,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="61" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>328</v>
       </c>
@@ -50439,7 +50499,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="62" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>333</v>
       </c>
@@ -50483,7 +50543,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="63" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>338</v>
       </c>
@@ -50527,7 +50587,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="64" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>343</v>
       </c>
@@ -50571,7 +50631,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="65" spans="1:37" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:40" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>348</v>
       </c>
@@ -50636,7 +50696,7 @@
         <v>3173</v>
       </c>
       <c r="V65" s="3" t="s">
-        <v>305</v>
+        <v>3193</v>
       </c>
       <c r="W65" s="3" t="s">
         <v>3175</v>
@@ -50645,7 +50705,7 @@
         <v>3176</v>
       </c>
       <c r="Y65" s="3" t="s">
-        <v>3181</v>
+        <v>3182</v>
       </c>
       <c r="Z65" s="3" t="s">
         <v>3172</v>
@@ -50654,7 +50714,7 @@
         <v>3177</v>
       </c>
       <c r="AB65" s="8" t="s">
-        <v>3182</v>
+        <v>3183</v>
       </c>
       <c r="AC65" s="9">
         <v>0</v>
@@ -50683,8 +50743,14 @@
       <c r="AK65" s="3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM65" s="3" t="s">
+        <v>3195</v>
+      </c>
+      <c r="AN65" s="3" t="s">
+        <v>3196</v>
+      </c>
+    </row>
+    <row r="66" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>353</v>
       </c>
@@ -50728,7 +50794,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="67" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>358</v>
       </c>
@@ -50772,7 +50838,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="68" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>363</v>
       </c>
@@ -50816,7 +50882,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="69" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>368</v>
       </c>
@@ -50860,7 +50926,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="70" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>373</v>
       </c>
@@ -50904,7 +50970,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="71" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>378</v>
       </c>
@@ -50948,7 +51014,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="72" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>383</v>
       </c>
@@ -50992,7 +51058,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="73" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>388</v>
       </c>

</xml_diff>

<commit_message>
feat: update step description to clarify payment summary verification process
</commit_message>
<xml_diff>
--- a/data/BigCommerceData/BigC_Ecomm_TestCases_AutomationMasterSheet.xlsx
+++ b/data/BigCommerceData/BigC_Ecomm_TestCases_AutomationMasterSheet.xlsx
@@ -9570,7 +9570,7 @@
     <t>Passed</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-10T20:19:44.897Z\nScreenshot: test-results/screenshots/TC0193.png","Status: Passed","Last Updated: 2025-09-10T20:19:45.059Z","---"]</t>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-10T20:43:23.097Z\nScreenshot: test-results/screenshots/TC0193.png","Status: Passed","Last Updated: 2025-09-10T20:43:23.246Z","---"]</t>
   </si>
   <si>
     <t>USD $20.00</t>
@@ -9579,16 +9579,16 @@
     <t>USD $132.15</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-10T20:20:26.999Z\nScreenshot: test-results/screenshots/TC0202.png","Status: Passed","Last Updated: 2025-09-10T20:20:27.113Z","---"]</t>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-10T20:44:08.906Z\nScreenshot: test-results/screenshots/TC0202.png","Status: Passed","Last Updated: 2025-09-10T20:44:08.981Z","---"]</t>
   </si>
   <si>
     <t>Customer transfers money directly to the seller's bank account.</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-10T20:21:03.342Z\nScreenshot: test-results/screenshots/TC0211.png","Status: Passed","Last Updated: 2025-09-10T20:21:03.418Z","---"]</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-10T20:21:44.893Z\nScreenshot: test-results/screenshots/TC0220.png","Status: Passed","Last Updated: 2025-09-10T20:21:44.973Z","---"]</t>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-10T20:44:44.644Z\nScreenshot: test-results/screenshots/TC0211.png","Status: Passed","Last Updated: 2025-09-10T20:44:44.764Z","---"]</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-10T20:45:27.318Z\nScreenshot: test-results/screenshots/TC0220.png","Status: Passed","Last Updated: 2025-09-10T20:45:27.404Z","---"]</t>
   </si>
   <si>
     <t>A real payment gateway/service provider (owned by Visa).</t>
@@ -9600,19 +9600,19 @@
     <t>American Express</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-10T20:22:22.217Z\nScreenshot: test-results/screenshots/TC0229.png","Status: Passed","Last Updated: 2025-09-10T20:22:22.358Z","---"]</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-10T20:23:05.822Z\nScreenshot: test-results/screenshots/TC0238.png","Status: Passed","Last Updated: 2025-09-10T20:23:05.968Z","---"]</t>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-10T20:46:06.545Z\nScreenshot: test-results/screenshots/TC0229.png","Status: Passed","Last Updated: 2025-09-10T20:46:06.632Z","---"]</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-10T20:46:50.189Z\nScreenshot: test-results/screenshots/TC0238.png","Status: Passed","Last Updated: 2025-09-10T20:46:50.261Z","---"]</t>
   </si>
   <si>
     <t>Manual payment</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-10T20:23:41.933Z\nScreenshot: test-results/screenshots/TC0247.png","Status: Passed","Last Updated: 2025-09-10T20:23:42.066Z","---"]</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-10T20:24:23.748Z\nScreenshot: test-results/screenshots/TC0256.png","Status: Passed","Last Updated: 2025-09-10T20:24:23.896Z","---"]</t>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-10T20:47:27.398Z\nScreenshot: test-results/screenshots/TC0247.png","Status: Passed","Last Updated: 2025-09-10T20:47:27.548Z","---"]</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-10T20:48:10.121Z\nScreenshot: test-results/screenshots/TC0256.png","Status: Passed","Last Updated: 2025-09-10T20:48:10.210Z","---"]</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Refactor Order Tests to Support Grouped Test Cases and Enhanced Scenario Handling
- Updated the test configuration to allow scenarios to include multiple test cases.
- Modified the test execution logic to iterate over test cases defined within each scenario.
- Removed redundant scenario matching checks in the test execution flow.
- Enhanced the shipping address filling logic to conditionally execute based on scenario names.
- Improved the default scenario setup to include test cases for both fulfillment methods.
</commit_message>
<xml_diff>
--- a/data/BigCommerceData/BigC_Ecomm_TestCases_AutomationMasterSheet.xlsx
+++ b/data/BigCommerceData/BigC_Ecomm_TestCases_AutomationMasterSheet.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19138" uniqueCount="3196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19308" uniqueCount="3204">
   <si>
     <t>Global Test Case ID</t>
   </si>
@@ -9570,7 +9570,10 @@
     <t>Passed</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-10T20:43:23.097Z\nScreenshot: test-results/screenshots/TC0193.png","Status: Passed","Last Updated: 2025-09-10T20:43:23.246Z","---"]</t>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:36:19.376Z\nScreenshot: test-results/screenshots/TC0193.png","Status: Passed","Last Updated: 2025-09-11T10:36:19.546Z","---"]</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:41:24.411Z\nScreenshot: test-results/screenshots/TC0194.png","Status: Passed","Last Updated: 2025-09-11T10:41:24.521Z","---"]</t>
   </si>
   <si>
     <t>USD $20.00</t>
@@ -9579,16 +9582,25 @@
     <t>USD $132.15</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-10T20:44:08.906Z\nScreenshot: test-results/screenshots/TC0202.png","Status: Passed","Last Updated: 2025-09-10T20:44:08.981Z","---"]</t>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:36:59.352Z\nScreenshot: test-results/screenshots/TC0202.png","Status: Passed","Last Updated: 2025-09-11T10:36:59.495Z","---"]</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:42:09.849Z\nScreenshot: test-results/screenshots/TC0203.png","Status: Passed","Last Updated: 2025-09-11T10:42:09.993Z","---"]</t>
   </si>
   <si>
     <t>Customer transfers money directly to the seller's bank account.</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-10T20:44:44.644Z\nScreenshot: test-results/screenshots/TC0211.png","Status: Passed","Last Updated: 2025-09-10T20:44:44.764Z","---"]</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-10T20:45:27.318Z\nScreenshot: test-results/screenshots/TC0220.png","Status: Passed","Last Updated: 2025-09-10T20:45:27.404Z","---"]</t>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:37:34.171Z\nScreenshot: test-results/screenshots/TC0211.png","Status: Passed","Last Updated: 2025-09-11T10:37:34.256Z","---"]</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:42:50.174Z\nScreenshot: test-results/screenshots/TC0212.png","Status: Passed","Last Updated: 2025-09-11T10:42:50.285Z","---"]</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:38:13.457Z\nScreenshot: test-results/screenshots/TC0220.png","Status: Passed","Last Updated: 2025-09-11T10:38:13.550Z","---"]</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:43:36.117Z\nScreenshot: test-results/screenshots/TC0221.png","Status: Passed","Last Updated: 2025-09-11T10:43:36.235Z","---"]</t>
   </si>
   <si>
     <t>A real payment gateway/service provider (owned by Visa).</t>
@@ -9600,19 +9612,31 @@
     <t>American Express</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-10T20:46:06.545Z\nScreenshot: test-results/screenshots/TC0229.png","Status: Passed","Last Updated: 2025-09-10T20:46:06.632Z","---"]</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-10T20:46:50.189Z\nScreenshot: test-results/screenshots/TC0238.png","Status: Passed","Last Updated: 2025-09-10T20:46:50.261Z","---"]</t>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:38:49.562Z\nScreenshot: test-results/screenshots/TC0229.png","Status: Passed","Last Updated: 2025-09-11T10:38:49.655Z","---"]</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:44:18.338Z\nScreenshot: test-results/screenshots/TC0230.png","Status: Passed","Last Updated: 2025-09-11T10:44:18.412Z","---"]</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:39:30.952Z\nScreenshot: test-results/screenshots/TC0238.png","Status: Passed","Last Updated: 2025-09-11T10:39:31.037Z","---"]</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:45:05.415Z\nScreenshot: test-results/screenshots/TC0239.png","Status: Passed","Last Updated: 2025-09-11T10:45:05.549Z","---"]</t>
   </si>
   <si>
     <t>Manual payment</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-10T20:47:27.398Z\nScreenshot: test-results/screenshots/TC0247.png","Status: Passed","Last Updated: 2025-09-10T20:47:27.548Z","---"]</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-10T20:48:10.121Z\nScreenshot: test-results/screenshots/TC0256.png","Status: Passed","Last Updated: 2025-09-10T20:48:10.210Z","---"]</t>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:40:04.874Z\nScreenshot: test-results/screenshots/TC0247.png","Status: Passed","Last Updated: 2025-09-11T10:40:04.950Z","---"]</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:45:46.913Z\nScreenshot: test-results/screenshots/TC0248.png","Status: Passed","Last Updated: 2025-09-11T10:45:47.032Z","---"]</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:40:44.769Z\nScreenshot: test-results/screenshots/TC0256.png","Status: Passed","Last Updated: 2025-09-11T10:40:44.844Z","---"]</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:46:37.793Z\nScreenshot: test-results/screenshots/TC0257.png","Status: Passed","Last Updated: 2025-09-11T10:46:37.932Z","---"]</t>
   </si>
 </sst>
 </file>
@@ -47144,7 +47168,7 @@
   <dimension ref="A1:AN73"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="86" zoomScaleNormal="86">
-      <selection activeCell="AN47" sqref="AN47"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" defaultColWidth="9.109375" customHeight="1"/>
@@ -47152,7 +47176,7 @@
     <col min="1" max="1" width="12.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="12.88671875" style="3" customWidth="1"/>
     <col min="3" max="3" width="14" style="3" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="36.6640625" style="3" customWidth="1"/>
     <col min="5" max="5" width="26.33203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" style="3" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" style="3" customWidth="1"/>
@@ -47432,7 +47456,7 @@
         <v>3181</v>
       </c>
     </row>
-    <row r="3" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
@@ -47474,6 +47498,81 @@
       </c>
       <c r="N3" s="3" t="s">
         <v>34</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>3171</v>
+      </c>
+      <c r="P3" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>3174</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>3175</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>3176</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>3172</v>
+      </c>
+      <c r="AA3" s="7" t="s">
+        <v>3177</v>
+      </c>
+      <c r="AB3" s="7" t="s">
+        <v>3172</v>
+      </c>
+      <c r="AC3" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AK3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM3" s="3" t="s">
+        <v>3180</v>
+      </c>
+      <c r="AN3" s="3" t="s">
+        <v>3182</v>
       </c>
     </row>
     <row r="4" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -47858,7 +47957,7 @@
         <v>3176</v>
       </c>
       <c r="Y11" s="3" t="s">
-        <v>3182</v>
+        <v>3183</v>
       </c>
       <c r="Z11" s="3" t="s">
         <v>3172</v>
@@ -47867,7 +47966,7 @@
         <v>3177</v>
       </c>
       <c r="AB11" s="8" t="s">
-        <v>3183</v>
+        <v>3184</v>
       </c>
       <c r="AC11" s="9">
         <v>0</v>
@@ -47900,10 +47999,10 @@
         <v>3180</v>
       </c>
       <c r="AN11" s="3" t="s">
-        <v>3184</v>
-      </c>
-    </row>
-    <row r="12" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
+        <v>3185</v>
+      </c>
+    </row>
+    <row r="12" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>80</v>
       </c>
@@ -47945,6 +48044,81 @@
       </c>
       <c r="N12" s="3" t="s">
         <v>84</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>3171</v>
+      </c>
+      <c r="P12" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>3174</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>3175</v>
+      </c>
+      <c r="X12" s="3" t="s">
+        <v>3176</v>
+      </c>
+      <c r="Y12" s="3" t="s">
+        <v>3183</v>
+      </c>
+      <c r="Z12" s="3" t="s">
+        <v>3172</v>
+      </c>
+      <c r="AA12" s="7" t="s">
+        <v>3177</v>
+      </c>
+      <c r="AB12" s="8" t="s">
+        <v>3184</v>
+      </c>
+      <c r="AC12" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="3" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AE12" s="3" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AF12" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AG12" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AH12" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AI12" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AJ12" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AK12" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM12" s="3" t="s">
+        <v>3180</v>
+      </c>
+      <c r="AN12" s="3" t="s">
+        <v>3186</v>
       </c>
     </row>
     <row r="13" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -48323,7 +48497,7 @@
         <v>123</v>
       </c>
       <c r="W20" s="3" t="s">
-        <v>3185</v>
+        <v>3187</v>
       </c>
       <c r="X20" s="3" t="s">
         <v>3176</v>
@@ -48371,10 +48545,10 @@
         <v>3180</v>
       </c>
       <c r="AN20" s="3" t="s">
-        <v>3186</v>
-      </c>
-    </row>
-    <row r="21" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
+        <v>3188</v>
+      </c>
+    </row>
+    <row r="21" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>126</v>
       </c>
@@ -48416,6 +48590,81 @@
       </c>
       <c r="N21" s="3" t="s">
         <v>130</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>3171</v>
+      </c>
+      <c r="P21" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="R21" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="S21" s="3" t="s">
+        <v>3174</v>
+      </c>
+      <c r="T21" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="U21" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="V21" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="W21" s="3" t="s">
+        <v>3175</v>
+      </c>
+      <c r="X21" s="3" t="s">
+        <v>3176</v>
+      </c>
+      <c r="Y21" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="Z21" s="3" t="s">
+        <v>3172</v>
+      </c>
+      <c r="AA21" s="7" t="s">
+        <v>3177</v>
+      </c>
+      <c r="AB21" s="7" t="s">
+        <v>3172</v>
+      </c>
+      <c r="AC21" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="3" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AE21" s="3" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AF21" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AG21" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AH21" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AI21" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AJ21" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AK21" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM21" s="3" t="s">
+        <v>3180</v>
+      </c>
+      <c r="AN21" s="3" t="s">
+        <v>3189</v>
       </c>
     </row>
     <row r="22" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -48794,13 +49043,13 @@
         <v>123</v>
       </c>
       <c r="W29" s="3" t="s">
-        <v>3185</v>
+        <v>3187</v>
       </c>
       <c r="X29" s="3" t="s">
         <v>3176</v>
       </c>
       <c r="Y29" s="3" t="s">
-        <v>3182</v>
+        <v>3183</v>
       </c>
       <c r="Z29" s="3" t="s">
         <v>3172</v>
@@ -48809,7 +49058,7 @@
         <v>3177</v>
       </c>
       <c r="AB29" s="8" t="s">
-        <v>3183</v>
+        <v>3184</v>
       </c>
       <c r="AC29" s="9">
         <v>0</v>
@@ -48842,10 +49091,10 @@
         <v>3180</v>
       </c>
       <c r="AN29" s="3" t="s">
-        <v>3187</v>
-      </c>
-    </row>
-    <row r="30" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
+        <v>3190</v>
+      </c>
+    </row>
+    <row r="30" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>171</v>
       </c>
@@ -48887,6 +49136,81 @@
       </c>
       <c r="N30" s="3" t="s">
         <v>175</v>
+      </c>
+      <c r="O30" s="3" t="s">
+        <v>3171</v>
+      </c>
+      <c r="P30" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="R30" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="S30" s="3" t="s">
+        <v>3174</v>
+      </c>
+      <c r="T30" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="U30" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="V30" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="W30" s="3" t="s">
+        <v>3175</v>
+      </c>
+      <c r="X30" s="3" t="s">
+        <v>3176</v>
+      </c>
+      <c r="Y30" s="3" t="s">
+        <v>3183</v>
+      </c>
+      <c r="Z30" s="3" t="s">
+        <v>3172</v>
+      </c>
+      <c r="AA30" s="7" t="s">
+        <v>3177</v>
+      </c>
+      <c r="AB30" s="8" t="s">
+        <v>3184</v>
+      </c>
+      <c r="AC30" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD30" s="3" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AE30" s="3" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AF30" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AG30" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AH30" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AI30" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AJ30" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AK30" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM30" s="3" t="s">
+        <v>3180</v>
+      </c>
+      <c r="AN30" s="3" t="s">
+        <v>3191</v>
       </c>
     </row>
     <row r="31" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -49265,7 +49589,7 @@
         <v>214</v>
       </c>
       <c r="W38" s="3" t="s">
-        <v>3188</v>
+        <v>3192</v>
       </c>
       <c r="X38" s="3" t="s">
         <v>3176</v>
@@ -49292,10 +49616,10 @@
         <v>3179</v>
       </c>
       <c r="AF38" s="3" t="s">
-        <v>3189</v>
+        <v>3193</v>
       </c>
       <c r="AG38" s="3" t="s">
-        <v>3190</v>
+        <v>3194</v>
       </c>
       <c r="AH38" s="3">
         <v>234234523</v>
@@ -49313,10 +49637,10 @@
         <v>3180</v>
       </c>
       <c r="AN38" s="3" t="s">
-        <v>3191</v>
-      </c>
-    </row>
-    <row r="39" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
+        <v>3195</v>
+      </c>
+    </row>
+    <row r="39" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>217</v>
       </c>
@@ -49358,6 +49682,81 @@
       </c>
       <c r="N39" s="3" t="s">
         <v>221</v>
+      </c>
+      <c r="O39" s="3" t="s">
+        <v>3171</v>
+      </c>
+      <c r="P39" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="R39" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="S39" s="3" t="s">
+        <v>3174</v>
+      </c>
+      <c r="T39" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="U39" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="V39" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="W39" s="3" t="s">
+        <v>3175</v>
+      </c>
+      <c r="X39" s="3" t="s">
+        <v>3176</v>
+      </c>
+      <c r="Y39" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="Z39" s="3" t="s">
+        <v>3172</v>
+      </c>
+      <c r="AA39" s="7" t="s">
+        <v>3177</v>
+      </c>
+      <c r="AB39" s="7" t="s">
+        <v>3172</v>
+      </c>
+      <c r="AC39" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD39" s="3" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AE39" s="3" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AF39" s="3" t="s">
+        <v>3193</v>
+      </c>
+      <c r="AG39" s="3" t="s">
+        <v>3194</v>
+      </c>
+      <c r="AH39" s="3">
+        <v>234234523</v>
+      </c>
+      <c r="AI39" s="3">
+        <v>445</v>
+      </c>
+      <c r="AJ39" s="10">
+        <v>47209</v>
+      </c>
+      <c r="AK39" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM39" s="3" t="s">
+        <v>3180</v>
+      </c>
+      <c r="AN39" s="3" t="s">
+        <v>3196</v>
       </c>
     </row>
     <row r="40" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -49736,13 +50135,13 @@
         <v>214</v>
       </c>
       <c r="W47" s="3" t="s">
-        <v>3188</v>
+        <v>3192</v>
       </c>
       <c r="X47" s="3" t="s">
         <v>3176</v>
       </c>
       <c r="Y47" s="3" t="s">
-        <v>3182</v>
+        <v>3183</v>
       </c>
       <c r="Z47" s="3" t="s">
         <v>3172</v>
@@ -49751,7 +50150,7 @@
         <v>3177</v>
       </c>
       <c r="AB47" s="8" t="s">
-        <v>3183</v>
+        <v>3184</v>
       </c>
       <c r="AC47" s="9">
         <v>0</v>
@@ -49763,10 +50162,10 @@
         <v>3179</v>
       </c>
       <c r="AF47" s="3" t="s">
-        <v>3189</v>
+        <v>3193</v>
       </c>
       <c r="AG47" s="3" t="s">
-        <v>3190</v>
+        <v>3194</v>
       </c>
       <c r="AH47" s="3">
         <v>234234523</v>
@@ -49784,10 +50183,10 @@
         <v>3180</v>
       </c>
       <c r="AN47" s="3" t="s">
-        <v>3192</v>
-      </c>
-    </row>
-    <row r="48" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
+        <v>3197</v>
+      </c>
+    </row>
+    <row r="48" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>262</v>
       </c>
@@ -49829,6 +50228,81 @@
       </c>
       <c r="N48" s="3" t="s">
         <v>266</v>
+      </c>
+      <c r="O48" s="3" t="s">
+        <v>3171</v>
+      </c>
+      <c r="P48" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q48" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="R48" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="S48" s="3" t="s">
+        <v>3174</v>
+      </c>
+      <c r="T48" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="U48" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="V48" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="W48" s="3" t="s">
+        <v>3175</v>
+      </c>
+      <c r="X48" s="3" t="s">
+        <v>3176</v>
+      </c>
+      <c r="Y48" s="3" t="s">
+        <v>3183</v>
+      </c>
+      <c r="Z48" s="3" t="s">
+        <v>3172</v>
+      </c>
+      <c r="AA48" s="7" t="s">
+        <v>3177</v>
+      </c>
+      <c r="AB48" s="8" t="s">
+        <v>3184</v>
+      </c>
+      <c r="AC48" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD48" s="3" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AE48" s="3" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AF48" s="3" t="s">
+        <v>3193</v>
+      </c>
+      <c r="AG48" s="3" t="s">
+        <v>3194</v>
+      </c>
+      <c r="AH48" s="3">
+        <v>234234523</v>
+      </c>
+      <c r="AI48" s="3">
+        <v>332</v>
+      </c>
+      <c r="AJ48" s="10">
+        <v>47209</v>
+      </c>
+      <c r="AK48" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM48" s="3" t="s">
+        <v>3180</v>
+      </c>
+      <c r="AN48" s="3" t="s">
+        <v>3198</v>
       </c>
     </row>
     <row r="49" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -50204,7 +50678,7 @@
         <v>3173</v>
       </c>
       <c r="V56" s="3" t="s">
-        <v>3193</v>
+        <v>3199</v>
       </c>
       <c r="W56" s="3" t="s">
         <v>3175</v>
@@ -50255,10 +50729,10 @@
         <v>3180</v>
       </c>
       <c r="AN56" s="3" t="s">
-        <v>3194</v>
-      </c>
-    </row>
-    <row r="57" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="57" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>308</v>
       </c>
@@ -50300,6 +50774,81 @@
       </c>
       <c r="N57" s="3" t="s">
         <v>312</v>
+      </c>
+      <c r="O57" s="3" t="s">
+        <v>3171</v>
+      </c>
+      <c r="P57" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q57" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="R57" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="S57" s="3" t="s">
+        <v>3174</v>
+      </c>
+      <c r="T57" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="U57" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="V57" s="3" t="s">
+        <v>3199</v>
+      </c>
+      <c r="W57" s="3" t="s">
+        <v>3175</v>
+      </c>
+      <c r="X57" s="3" t="s">
+        <v>3176</v>
+      </c>
+      <c r="Y57" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="Z57" s="3" t="s">
+        <v>3172</v>
+      </c>
+      <c r="AA57" s="7" t="s">
+        <v>3177</v>
+      </c>
+      <c r="AB57" s="7" t="s">
+        <v>3172</v>
+      </c>
+      <c r="AC57" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD57" s="3" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AE57" s="3" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AF57" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AG57" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AH57" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AI57" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AJ57" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AK57" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM57" s="3" t="s">
+        <v>3180</v>
+      </c>
+      <c r="AN57" s="3" t="s">
+        <v>3201</v>
       </c>
     </row>
     <row r="58" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -50675,7 +51224,7 @@
         <v>3173</v>
       </c>
       <c r="V65" s="3" t="s">
-        <v>3193</v>
+        <v>3199</v>
       </c>
       <c r="W65" s="3" t="s">
         <v>3175</v>
@@ -50684,7 +51233,7 @@
         <v>3176</v>
       </c>
       <c r="Y65" s="3" t="s">
-        <v>3182</v>
+        <v>3183</v>
       </c>
       <c r="Z65" s="3" t="s">
         <v>3172</v>
@@ -50693,7 +51242,7 @@
         <v>3177</v>
       </c>
       <c r="AB65" s="8" t="s">
-        <v>3183</v>
+        <v>3184</v>
       </c>
       <c r="AC65" s="9">
         <v>0</v>
@@ -50726,10 +51275,10 @@
         <v>3180</v>
       </c>
       <c r="AN65" s="3" t="s">
-        <v>3195</v>
-      </c>
-    </row>
-    <row r="66" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
+        <v>3202</v>
+      </c>
+    </row>
+    <row r="66" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>353</v>
       </c>
@@ -50771,6 +51320,81 @@
       </c>
       <c r="N66" s="3" t="s">
         <v>357</v>
+      </c>
+      <c r="O66" s="3" t="s">
+        <v>3171</v>
+      </c>
+      <c r="P66" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q66" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="R66" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="S66" s="3" t="s">
+        <v>3174</v>
+      </c>
+      <c r="T66" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="U66" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="V66" s="3" t="s">
+        <v>3199</v>
+      </c>
+      <c r="W66" s="3" t="s">
+        <v>3175</v>
+      </c>
+      <c r="X66" s="3" t="s">
+        <v>3176</v>
+      </c>
+      <c r="Y66" s="3" t="s">
+        <v>3183</v>
+      </c>
+      <c r="Z66" s="3" t="s">
+        <v>3172</v>
+      </c>
+      <c r="AA66" s="7" t="s">
+        <v>3177</v>
+      </c>
+      <c r="AB66" s="8" t="s">
+        <v>3184</v>
+      </c>
+      <c r="AC66" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD66" s="3" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AE66" s="3" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AF66" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AG66" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AH66" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AI66" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AJ66" s="3" t="s">
+        <v>3173</v>
+      </c>
+      <c r="AK66" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM66" s="3" t="s">
+        <v>3180</v>
+      </c>
+      <c r="AN66" s="3" t="s">
+        <v>3203</v>
       </c>
     </row>
     <row r="67" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -51082,7 +51706,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AL73"/>
+  <autoFilter ref="A1:AN73"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
@@ -51093,7 +51717,7 @@
   <dimension ref="A1:N73"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" defaultColWidth="9.109375" customHeight="1"/>
@@ -54324,6 +54948,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="D1:D73"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
feat: enhance order processing by adding order success alert handling and refactoring address management
</commit_message>
<xml_diff>
--- a/data/BigCommerceData/BigC_Ecomm_TestCases_AutomationMasterSheet.xlsx
+++ b/data/BigCommerceData/BigC_Ecomm_TestCases_AutomationMasterSheet.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19308" uniqueCount="3204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19320" uniqueCount="3217">
   <si>
     <t>Global Test Case ID</t>
   </si>
@@ -9567,13 +9567,19 @@
     <t>Standard product order for existing customer</t>
   </si>
   <si>
+    <t>356989</t>
+  </si>
+  <si>
     <t>Passed</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:36:19.376Z\nScreenshot: test-results/screenshots/TC0193.png","Status: Passed","Last Updated: 2025-09-11T10:36:19.546Z","---"]</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:41:24.411Z\nScreenshot: test-results/screenshots/TC0194.png","Status: Passed","Last Updated: 2025-09-11T10:41:24.521Z","---"]</t>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-12T09:18:53.199Z\nScreenshot: test-results/screenshots/TC0193.png","Status: Passed","Last Updated: 2025-09-12T09:18:53.292Z","---"]</t>
+  </si>
+  <si>
+    <t>356995</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-12T09:29:14.821Z\nScreenshot: test-results/screenshots/TC0194.png","Status: Passed","Last Updated: 2025-09-12T09:29:14.926Z","---"]</t>
   </si>
   <si>
     <t>USD $20.00</t>
@@ -9582,25 +9588,43 @@
     <t>USD $132.15</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:36:59.352Z\nScreenshot: test-results/screenshots/TC0202.png","Status: Passed","Last Updated: 2025-09-11T10:36:59.495Z","---"]</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:42:09.849Z\nScreenshot: test-results/screenshots/TC0203.png","Status: Passed","Last Updated: 2025-09-11T10:42:09.993Z","---"]</t>
+    <t>356990</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-12T09:19:37.499Z\nScreenshot: test-results/screenshots/TC0202.png","Status: Passed","Last Updated: 2025-09-12T09:19:37.605Z","---"]</t>
+  </si>
+  <si>
+    <t>356996</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-12T09:30:09.873Z\nScreenshot: test-results/screenshots/TC0203.png","Status: Passed","Last Updated: 2025-09-12T09:30:09.990Z","---"]</t>
   </si>
   <si>
     <t>Customer transfers money directly to the seller's bank account.</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:37:34.171Z\nScreenshot: test-results/screenshots/TC0211.png","Status: Passed","Last Updated: 2025-09-11T10:37:34.256Z","---"]</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:42:50.174Z\nScreenshot: test-results/screenshots/TC0212.png","Status: Passed","Last Updated: 2025-09-11T10:42:50.285Z","---"]</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:38:13.457Z\nScreenshot: test-results/screenshots/TC0220.png","Status: Passed","Last Updated: 2025-09-11T10:38:13.550Z","---"]</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:43:36.117Z\nScreenshot: test-results/screenshots/TC0221.png","Status: Passed","Last Updated: 2025-09-11T10:43:36.235Z","---"]</t>
+    <t>356991</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-12T09:20:17.659Z\nScreenshot: test-results/screenshots/TC0211.png","Status: Passed","Last Updated: 2025-09-12T09:20:17.761Z","---"]</t>
+  </si>
+  <si>
+    <t>356997</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-12T09:30:56.613Z\nScreenshot: test-results/screenshots/TC0212.png","Status: Passed","Last Updated: 2025-09-12T09:30:56.705Z","---"]</t>
+  </si>
+  <si>
+    <t>356992</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-12T09:21:01.665Z\nScreenshot: test-results/screenshots/TC0220.png","Status: Passed","Last Updated: 2025-09-12T09:21:01.760Z","---"]</t>
+  </si>
+  <si>
+    <t>356998</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-12T09:31:47.989Z\nScreenshot: test-results/screenshots/TC0221.png","Status: Passed","Last Updated: 2025-09-12T09:31:48.067Z","---"]</t>
   </si>
   <si>
     <t>A real payment gateway/service provider (owned by Visa).</t>
@@ -9612,31 +9636,46 @@
     <t>American Express</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:38:49.562Z\nScreenshot: test-results/screenshots/TC0229.png","Status: Passed","Last Updated: 2025-09-11T10:38:49.655Z","---"]</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:44:18.338Z\nScreenshot: test-results/screenshots/TC0230.png","Status: Passed","Last Updated: 2025-09-11T10:44:18.412Z","---"]</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:39:30.952Z\nScreenshot: test-results/screenshots/TC0238.png","Status: Passed","Last Updated: 2025-09-11T10:39:31.037Z","---"]</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:45:05.415Z\nScreenshot: test-results/screenshots/TC0239.png","Status: Passed","Last Updated: 2025-09-11T10:45:05.549Z","---"]</t>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>["=== Test Failure Details ===","Failed Step: Verify Order Creation in All Orders Page","Error Message: locator.waitFor: Timeout 10000ms exceeded.\nCall log:\n\u001b[2m  - waiting for locator('#content-iframe').contentFrame().locator('//div[@id=\"orderStatus\"]//p') to be visible\u001b[22m\n","Failure Timestamp: 2025-09-12T09:26:35.072Z","Failure Screenshot: test-results/screenshots/failure_TC0229_1757669194852.png","","=== Additional Notes ===","Test failed during: Verify Order Creation in All Orders Page\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T09:26:35.731Z","---"]</t>
+  </si>
+  <si>
+    <t>["=== Test Failure Details ===","Failed Step: Verify Order Creation in All Orders Page","Error Message: locator.waitFor: Timeout 10000ms exceeded.\nCall log:\n\u001b[2m  - waiting for locator('#content-iframe').contentFrame().locator('//div[@id=\"orderStatus\"]//p') to be visible\u001b[22m\n","Failure Timestamp: 2025-09-12T09:32:39.304Z","Failure Screenshot: test-results/screenshots/failure_TC0230_1757669559009.png","","=== Additional Notes ===","Test failed during: Verify Order Creation in All Orders Page\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T09:32:39.483Z","---"]</t>
+  </si>
+  <si>
+    <t>["=== Test Failure Details ===","Failed Step: Verify Order Creation in All Orders Page","Error Message: locator.waitFor: Timeout 10000ms exceeded.\nCall log:\n\u001b[2m  - waiting for locator('#content-iframe').contentFrame().locator('//div[@id=\"orderStatus\"]//p') to be visible\u001b[22m\n","Failure Timestamp: 2025-09-12T09:22:42.501Z","Failure Screenshot: test-results/screenshots/failure_TC0238_1757668962229.png","","=== Additional Notes ===","Test failed during: Verify Order Creation in All Orders Page\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T09:22:42.657Z","---"]</t>
+  </si>
+  <si>
+    <t>["=== Test Failure Details ===","Failed Step: Verify Order Creation in All Orders Page","Error Message: locator.waitFor: Timeout 10000ms exceeded.\nCall log:\n\u001b[2m  - waiting for locator('#content-iframe').contentFrame().locator('//div[@id=\"orderStatus\"]//p') to be visible\u001b[22m\n","Failure Timestamp: 2025-09-12T09:33:40.042Z","Failure Screenshot: test-results/screenshots/failure_TC0239_1757669619789.png","","=== Additional Notes ===","Test failed during: Verify Order Creation in All Orders Page\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T09:33:40.159Z","---"]</t>
   </si>
   <si>
     <t>Manual payment</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:40:04.874Z\nScreenshot: test-results/screenshots/TC0247.png","Status: Passed","Last Updated: 2025-09-11T10:40:04.950Z","---"]</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:45:46.913Z\nScreenshot: test-results/screenshots/TC0248.png","Status: Passed","Last Updated: 2025-09-11T10:45:47.032Z","---"]</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:40:44.769Z\nScreenshot: test-results/screenshots/TC0256.png","Status: Passed","Last Updated: 2025-09-11T10:40:44.844Z","---"]</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-11T10:46:37.793Z\nScreenshot: test-results/screenshots/TC0257.png","Status: Passed","Last Updated: 2025-09-11T10:46:37.932Z","---"]</t>
+    <t>356993</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-12T09:23:24.073Z\nScreenshot: test-results/screenshots/TC0247.png","Status: Passed","Last Updated: 2025-09-12T09:23:24.548Z","---"]</t>
+  </si>
+  <si>
+    <t>356999</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-12T09:34:28.313Z\nScreenshot: test-results/screenshots/TC0248.png","Status: Passed","Last Updated: 2025-09-12T09:34:28.421Z","---"]</t>
+  </si>
+  <si>
+    <t>356994</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-12T09:24:10.195Z\nScreenshot: test-results/screenshots/TC0256.png","Status: Passed","Last Updated: 2025-09-12T09:24:10.603Z","---"]</t>
+  </si>
+  <si>
+    <t>357000</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-12T09:35:18.814Z\nScreenshot: test-results/screenshots/TC0257.png","Status: Passed","Last Updated: 2025-09-12T09:35:18.920Z","---"]</t>
   </si>
 </sst>
 </file>
@@ -47449,11 +47488,14 @@
       <c r="AK2" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="AL2" s="3" t="s">
+        <v>3180</v>
+      </c>
       <c r="AM2" s="3" t="s">
-        <v>3180</v>
+        <v>3181</v>
       </c>
       <c r="AN2" s="3" t="s">
-        <v>3181</v>
+        <v>3182</v>
       </c>
     </row>
     <row r="3" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
@@ -47568,11 +47610,14 @@
       <c r="AK3" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="AL3" s="3" t="s">
+        <v>3183</v>
+      </c>
       <c r="AM3" s="3" t="s">
-        <v>3180</v>
+        <v>3181</v>
       </c>
       <c r="AN3" s="3" t="s">
-        <v>3182</v>
+        <v>3184</v>
       </c>
     </row>
     <row r="4" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -47957,7 +48002,7 @@
         <v>3176</v>
       </c>
       <c r="Y11" s="3" t="s">
-        <v>3183</v>
+        <v>3185</v>
       </c>
       <c r="Z11" s="3" t="s">
         <v>3172</v>
@@ -47966,7 +48011,7 @@
         <v>3177</v>
       </c>
       <c r="AB11" s="8" t="s">
-        <v>3184</v>
+        <v>3186</v>
       </c>
       <c r="AC11" s="9">
         <v>0</v>
@@ -47995,11 +48040,14 @@
       <c r="AK11" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="AL11" s="3" t="s">
+        <v>3187</v>
+      </c>
       <c r="AM11" s="3" t="s">
-        <v>3180</v>
+        <v>3181</v>
       </c>
       <c r="AN11" s="3" t="s">
-        <v>3185</v>
+        <v>3188</v>
       </c>
     </row>
     <row r="12" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
@@ -48076,7 +48124,7 @@
         <v>3176</v>
       </c>
       <c r="Y12" s="3" t="s">
-        <v>3183</v>
+        <v>3185</v>
       </c>
       <c r="Z12" s="3" t="s">
         <v>3172</v>
@@ -48085,7 +48133,7 @@
         <v>3177</v>
       </c>
       <c r="AB12" s="8" t="s">
-        <v>3184</v>
+        <v>3186</v>
       </c>
       <c r="AC12" s="9">
         <v>0</v>
@@ -48114,11 +48162,14 @@
       <c r="AK12" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="AL12" s="3" t="s">
+        <v>3189</v>
+      </c>
       <c r="AM12" s="3" t="s">
-        <v>3180</v>
+        <v>3181</v>
       </c>
       <c r="AN12" s="3" t="s">
-        <v>3186</v>
+        <v>3190</v>
       </c>
     </row>
     <row r="13" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -48497,7 +48548,7 @@
         <v>123</v>
       </c>
       <c r="W20" s="3" t="s">
-        <v>3187</v>
+        <v>3191</v>
       </c>
       <c r="X20" s="3" t="s">
         <v>3176</v>
@@ -48541,11 +48592,14 @@
       <c r="AK20" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="AL20" s="3" t="s">
+        <v>3192</v>
+      </c>
       <c r="AM20" s="3" t="s">
-        <v>3180</v>
+        <v>3181</v>
       </c>
       <c r="AN20" s="3" t="s">
-        <v>3188</v>
+        <v>3193</v>
       </c>
     </row>
     <row r="21" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
@@ -48660,11 +48714,14 @@
       <c r="AK21" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="AL21" s="3" t="s">
+        <v>3194</v>
+      </c>
       <c r="AM21" s="3" t="s">
-        <v>3180</v>
+        <v>3181</v>
       </c>
       <c r="AN21" s="3" t="s">
-        <v>3189</v>
+        <v>3195</v>
       </c>
     </row>
     <row r="22" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -49043,13 +49100,13 @@
         <v>123</v>
       </c>
       <c r="W29" s="3" t="s">
-        <v>3187</v>
+        <v>3191</v>
       </c>
       <c r="X29" s="3" t="s">
         <v>3176</v>
       </c>
       <c r="Y29" s="3" t="s">
-        <v>3183</v>
+        <v>3185</v>
       </c>
       <c r="Z29" s="3" t="s">
         <v>3172</v>
@@ -49058,7 +49115,7 @@
         <v>3177</v>
       </c>
       <c r="AB29" s="8" t="s">
-        <v>3184</v>
+        <v>3186</v>
       </c>
       <c r="AC29" s="9">
         <v>0</v>
@@ -49087,11 +49144,14 @@
       <c r="AK29" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="AL29" s="3" t="s">
+        <v>3196</v>
+      </c>
       <c r="AM29" s="3" t="s">
-        <v>3180</v>
+        <v>3181</v>
       </c>
       <c r="AN29" s="3" t="s">
-        <v>3190</v>
+        <v>3197</v>
       </c>
     </row>
     <row r="30" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
@@ -49168,7 +49228,7 @@
         <v>3176</v>
       </c>
       <c r="Y30" s="3" t="s">
-        <v>3183</v>
+        <v>3185</v>
       </c>
       <c r="Z30" s="3" t="s">
         <v>3172</v>
@@ -49177,7 +49237,7 @@
         <v>3177</v>
       </c>
       <c r="AB30" s="8" t="s">
-        <v>3184</v>
+        <v>3186</v>
       </c>
       <c r="AC30" s="9">
         <v>0</v>
@@ -49206,11 +49266,14 @@
       <c r="AK30" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="AL30" s="3" t="s">
+        <v>3198</v>
+      </c>
       <c r="AM30" s="3" t="s">
-        <v>3180</v>
+        <v>3181</v>
       </c>
       <c r="AN30" s="3" t="s">
-        <v>3191</v>
+        <v>3199</v>
       </c>
     </row>
     <row r="31" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -49589,7 +49652,7 @@
         <v>214</v>
       </c>
       <c r="W38" s="3" t="s">
-        <v>3192</v>
+        <v>3200</v>
       </c>
       <c r="X38" s="3" t="s">
         <v>3176</v>
@@ -49616,10 +49679,10 @@
         <v>3179</v>
       </c>
       <c r="AF38" s="3" t="s">
-        <v>3193</v>
+        <v>3201</v>
       </c>
       <c r="AG38" s="3" t="s">
-        <v>3194</v>
+        <v>3202</v>
       </c>
       <c r="AH38" s="3">
         <v>234234523</v>
@@ -49634,10 +49697,10 @@
         <v>1</v>
       </c>
       <c r="AM38" s="3" t="s">
-        <v>3180</v>
+        <v>3203</v>
       </c>
       <c r="AN38" s="3" t="s">
-        <v>3195</v>
+        <v>3204</v>
       </c>
     </row>
     <row r="39" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
@@ -49735,10 +49798,10 @@
         <v>3179</v>
       </c>
       <c r="AF39" s="3" t="s">
-        <v>3193</v>
+        <v>3201</v>
       </c>
       <c r="AG39" s="3" t="s">
-        <v>3194</v>
+        <v>3202</v>
       </c>
       <c r="AH39" s="3">
         <v>234234523</v>
@@ -49753,10 +49816,10 @@
         <v>1</v>
       </c>
       <c r="AM39" s="3" t="s">
-        <v>3180</v>
+        <v>3203</v>
       </c>
       <c r="AN39" s="3" t="s">
-        <v>3196</v>
+        <v>3205</v>
       </c>
     </row>
     <row r="40" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -50135,13 +50198,13 @@
         <v>214</v>
       </c>
       <c r="W47" s="3" t="s">
-        <v>3192</v>
+        <v>3200</v>
       </c>
       <c r="X47" s="3" t="s">
         <v>3176</v>
       </c>
       <c r="Y47" s="3" t="s">
-        <v>3183</v>
+        <v>3185</v>
       </c>
       <c r="Z47" s="3" t="s">
         <v>3172</v>
@@ -50150,7 +50213,7 @@
         <v>3177</v>
       </c>
       <c r="AB47" s="8" t="s">
-        <v>3184</v>
+        <v>3186</v>
       </c>
       <c r="AC47" s="9">
         <v>0</v>
@@ -50162,10 +50225,10 @@
         <v>3179</v>
       </c>
       <c r="AF47" s="3" t="s">
-        <v>3193</v>
+        <v>3201</v>
       </c>
       <c r="AG47" s="3" t="s">
-        <v>3194</v>
+        <v>3202</v>
       </c>
       <c r="AH47" s="3">
         <v>234234523</v>
@@ -50180,10 +50243,10 @@
         <v>1</v>
       </c>
       <c r="AM47" s="3" t="s">
-        <v>3180</v>
+        <v>3203</v>
       </c>
       <c r="AN47" s="3" t="s">
-        <v>3197</v>
+        <v>3206</v>
       </c>
     </row>
     <row r="48" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
@@ -50260,7 +50323,7 @@
         <v>3176</v>
       </c>
       <c r="Y48" s="3" t="s">
-        <v>3183</v>
+        <v>3185</v>
       </c>
       <c r="Z48" s="3" t="s">
         <v>3172</v>
@@ -50269,7 +50332,7 @@
         <v>3177</v>
       </c>
       <c r="AB48" s="8" t="s">
-        <v>3184</v>
+        <v>3186</v>
       </c>
       <c r="AC48" s="9">
         <v>0</v>
@@ -50281,10 +50344,10 @@
         <v>3179</v>
       </c>
       <c r="AF48" s="3" t="s">
-        <v>3193</v>
+        <v>3201</v>
       </c>
       <c r="AG48" s="3" t="s">
-        <v>3194</v>
+        <v>3202</v>
       </c>
       <c r="AH48" s="3">
         <v>234234523</v>
@@ -50299,10 +50362,10 @@
         <v>1</v>
       </c>
       <c r="AM48" s="3" t="s">
-        <v>3180</v>
+        <v>3203</v>
       </c>
       <c r="AN48" s="3" t="s">
-        <v>3198</v>
+        <v>3207</v>
       </c>
     </row>
     <row r="49" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -50678,7 +50741,7 @@
         <v>3173</v>
       </c>
       <c r="V56" s="3" t="s">
-        <v>3199</v>
+        <v>3208</v>
       </c>
       <c r="W56" s="3" t="s">
         <v>3175</v>
@@ -50725,11 +50788,14 @@
       <c r="AK56" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="AL56" s="3" t="s">
+        <v>3209</v>
+      </c>
       <c r="AM56" s="3" t="s">
-        <v>3180</v>
+        <v>3181</v>
       </c>
       <c r="AN56" s="3" t="s">
-        <v>3200</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="57" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
@@ -50797,7 +50863,7 @@
         <v>3173</v>
       </c>
       <c r="V57" s="3" t="s">
-        <v>3199</v>
+        <v>3208</v>
       </c>
       <c r="W57" s="3" t="s">
         <v>3175</v>
@@ -50844,11 +50910,14 @@
       <c r="AK57" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="AL57" s="3" t="s">
+        <v>3211</v>
+      </c>
       <c r="AM57" s="3" t="s">
-        <v>3180</v>
+        <v>3181</v>
       </c>
       <c r="AN57" s="3" t="s">
-        <v>3201</v>
+        <v>3212</v>
       </c>
     </row>
     <row r="58" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -51224,7 +51293,7 @@
         <v>3173</v>
       </c>
       <c r="V65" s="3" t="s">
-        <v>3199</v>
+        <v>3208</v>
       </c>
       <c r="W65" s="3" t="s">
         <v>3175</v>
@@ -51233,7 +51302,7 @@
         <v>3176</v>
       </c>
       <c r="Y65" s="3" t="s">
-        <v>3183</v>
+        <v>3185</v>
       </c>
       <c r="Z65" s="3" t="s">
         <v>3172</v>
@@ -51242,7 +51311,7 @@
         <v>3177</v>
       </c>
       <c r="AB65" s="8" t="s">
-        <v>3184</v>
+        <v>3186</v>
       </c>
       <c r="AC65" s="9">
         <v>0</v>
@@ -51271,11 +51340,14 @@
       <c r="AK65" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="AL65" s="3" t="s">
+        <v>3213</v>
+      </c>
       <c r="AM65" s="3" t="s">
-        <v>3180</v>
+        <v>3181</v>
       </c>
       <c r="AN65" s="3" t="s">
-        <v>3202</v>
+        <v>3214</v>
       </c>
     </row>
     <row r="66" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
@@ -51343,7 +51415,7 @@
         <v>3173</v>
       </c>
       <c r="V66" s="3" t="s">
-        <v>3199</v>
+        <v>3208</v>
       </c>
       <c r="W66" s="3" t="s">
         <v>3175</v>
@@ -51352,7 +51424,7 @@
         <v>3176</v>
       </c>
       <c r="Y66" s="3" t="s">
-        <v>3183</v>
+        <v>3185</v>
       </c>
       <c r="Z66" s="3" t="s">
         <v>3172</v>
@@ -51361,7 +51433,7 @@
         <v>3177</v>
       </c>
       <c r="AB66" s="8" t="s">
-        <v>3184</v>
+        <v>3186</v>
       </c>
       <c r="AC66" s="9">
         <v>0</v>
@@ -51390,11 +51462,14 @@
       <c r="AK66" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="AL66" s="3" t="s">
+        <v>3215</v>
+      </c>
       <c r="AM66" s="3" t="s">
-        <v>3180</v>
+        <v>3181</v>
       </c>
       <c r="AN66" s="3" t="s">
-        <v>3203</v>
+        <v>3216</v>
       </c>
     </row>
     <row r="67" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat: implement comprehensive database verification for BigCommerce orders with query management and testing framework
</commit_message>
<xml_diff>
--- a/data/BigCommerceData/BigC_Ecomm_TestCases_AutomationMasterSheet.xlsx
+++ b/data/BigCommerceData/BigC_Ecomm_TestCases_AutomationMasterSheet.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19320" uniqueCount="3217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19320" uniqueCount="3216">
   <si>
     <t>Global Test Case ID</t>
   </si>
@@ -9570,16 +9570,16 @@
     <t>356989</t>
   </si>
   <si>
-    <t>Passed</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-12T09:18:53.199Z\nScreenshot: test-results/screenshots/TC0193.png","Status: Passed","Last Updated: 2025-09-12T09:18:53.292Z","---"]</t>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.59.8.144' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-12T10:40:57.492Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:40:57.600Z","---"]</t>
   </si>
   <si>
     <t>356995</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-12T09:29:14.821Z\nScreenshot: test-results/screenshots/TC0194.png","Status: Passed","Last Updated: 2025-09-12T09:29:14.926Z","---"]</t>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.59.8.144' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-12T10:41:31.494Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:31.606Z","---"]</t>
   </si>
   <si>
     <t>USD $20.00</t>
@@ -9591,13 +9591,13 @@
     <t>356990</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-12T09:19:37.499Z\nScreenshot: test-results/screenshots/TC0202.png","Status: Passed","Last Updated: 2025-09-12T09:19:37.605Z","---"]</t>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.59.8.144' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-12T10:41:01.947Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:02.077Z","---"]</t>
   </si>
   <si>
     <t>356996</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-12T09:30:09.873Z\nScreenshot: test-results/screenshots/TC0203.png","Status: Passed","Last Updated: 2025-09-12T09:30:09.990Z","---"]</t>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.59.8.144' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-12T10:41:35.837Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:35.945Z","---"]</t>
   </si>
   <si>
     <t>Customer transfers money directly to the seller's bank account.</t>
@@ -9606,25 +9606,25 @@
     <t>356991</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-12T09:20:17.659Z\nScreenshot: test-results/screenshots/TC0211.png","Status: Passed","Last Updated: 2025-09-12T09:20:17.761Z","---"]</t>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.59.8.144' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-12T10:41:06.455Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:06.590Z","---"]</t>
   </si>
   <si>
     <t>356997</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-12T09:30:56.613Z\nScreenshot: test-results/screenshots/TC0212.png","Status: Passed","Last Updated: 2025-09-12T09:30:56.705Z","---"]</t>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.59.8.144' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-12T10:41:40.257Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:40.365Z","---"]</t>
   </si>
   <si>
     <t>356992</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-12T09:21:01.665Z\nScreenshot: test-results/screenshots/TC0220.png","Status: Passed","Last Updated: 2025-09-12T09:21:01.760Z","---"]</t>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.59.8.144' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-12T10:41:11.144Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:11.262Z","---"]</t>
   </si>
   <si>
     <t>356998</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-12T09:31:47.989Z\nScreenshot: test-results/screenshots/TC0221.png","Status: Passed","Last Updated: 2025-09-12T09:31:48.067Z","---"]</t>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.59.8.144' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-12T10:41:44.860Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:44.985Z","---"]</t>
   </si>
   <si>
     <t>A real payment gateway/service provider (owned by Visa).</t>
@@ -9636,19 +9636,16 @@
     <t>American Express</t>
   </si>
   <si>
-    <t>Failed</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Verify Order Creation in All Orders Page","Error Message: locator.waitFor: Timeout 10000ms exceeded.\nCall log:\n\u001b[2m  - waiting for locator('#content-iframe').contentFrame().locator('//div[@id=\"orderStatus\"]//p') to be visible\u001b[22m\n","Failure Timestamp: 2025-09-12T09:26:35.072Z","Failure Screenshot: test-results/screenshots/failure_TC0229_1757669194852.png","","=== Additional Notes ===","Test failed during: Verify Order Creation in All Orders Page\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T09:26:35.731Z","---"]</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Verify Order Creation in All Orders Page","Error Message: locator.waitFor: Timeout 10000ms exceeded.\nCall log:\n\u001b[2m  - waiting for locator('#content-iframe').contentFrame().locator('//div[@id=\"orderStatus\"]//p') to be visible\u001b[22m\n","Failure Timestamp: 2025-09-12T09:32:39.304Z","Failure Screenshot: test-results/screenshots/failure_TC0230_1757669559009.png","","=== Additional Notes ===","Test failed during: Verify Order Creation in All Orders Page\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T09:32:39.483Z","---"]</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Verify Order Creation in All Orders Page","Error Message: locator.waitFor: Timeout 10000ms exceeded.\nCall log:\n\u001b[2m  - waiting for locator('#content-iframe').contentFrame().locator('//div[@id=\"orderStatus\"]//p') to be visible\u001b[22m\n","Failure Timestamp: 2025-09-12T09:22:42.501Z","Failure Screenshot: test-results/screenshots/failure_TC0238_1757668962229.png","","=== Additional Notes ===","Test failed during: Verify Order Creation in All Orders Page\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T09:22:42.657Z","---"]</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Verify Order Creation in All Orders Page","Error Message: locator.waitFor: Timeout 10000ms exceeded.\nCall log:\n\u001b[2m  - waiting for locator('#content-iframe').contentFrame().locator('//div[@id=\"orderStatus\"]//p') to be visible\u001b[22m\n","Failure Timestamp: 2025-09-12T09:33:40.042Z","Failure Screenshot: test-results/screenshots/failure_TC0239_1757669619789.png","","=== Additional Notes ===","Test failed during: Verify Order Creation in All Orders Page\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T09:33:40.159Z","---"]</t>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Order_Id not found in Excel sheet. Ensure the order has been created first.","Failure Timestamp: 2025-09-12T10:41:14.289Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:14.410Z","---"]</t>
+  </si>
+  <si>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Order_Id not found in Excel sheet. Ensure the order has been created first.","Failure Timestamp: 2025-09-12T10:41:47.711Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:47.826Z","---"]</t>
+  </si>
+  <si>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Order_Id not found in Excel sheet. Ensure the order has been created first.","Failure Timestamp: 2025-09-12T10:41:17.189Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:17.329Z","---"]</t>
+  </si>
+  <si>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Order_Id not found in Excel sheet. Ensure the order has been created first.","Failure Timestamp: 2025-09-12T10:41:50.540Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:50.655Z","---"]</t>
   </si>
   <si>
     <t>Manual payment</t>
@@ -9657,25 +9654,25 @@
     <t>356993</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-12T09:23:24.073Z\nScreenshot: test-results/screenshots/TC0247.png","Status: Passed","Last Updated: 2025-09-12T09:23:24.548Z","---"]</t>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.59.8.144' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-12T10:41:22.217Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:22.328Z","---"]</t>
   </si>
   <si>
     <t>356999</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-12T09:34:28.313Z\nScreenshot: test-results/screenshots/TC0248.png","Status: Passed","Last Updated: 2025-09-12T09:34:28.421Z","---"]</t>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.59.8.144' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-12T10:41:55.566Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:55.682Z","---"]</t>
   </si>
   <si>
     <t>356994</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-12T09:24:10.195Z\nScreenshot: test-results/screenshots/TC0256.png","Status: Passed","Last Updated: 2025-09-12T09:24:10.603Z","---"]</t>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.59.8.144' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-12T10:41:26.960Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:27.070Z","---"]</t>
   </si>
   <si>
     <t>357000</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-12T09:35:18.814Z\nScreenshot: test-results/screenshots/TC0257.png","Status: Passed","Last Updated: 2025-09-12T09:35:18.920Z","---"]</t>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.59.8.144' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-12T10:42:01.534Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:42:01.651Z","---"]</t>
   </si>
 </sst>
 </file>
@@ -49697,10 +49694,10 @@
         <v>1</v>
       </c>
       <c r="AM38" s="3" t="s">
+        <v>3181</v>
+      </c>
+      <c r="AN38" s="3" t="s">
         <v>3203</v>
-      </c>
-      <c r="AN38" s="3" t="s">
-        <v>3204</v>
       </c>
     </row>
     <row r="39" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
@@ -49816,10 +49813,10 @@
         <v>1</v>
       </c>
       <c r="AM39" s="3" t="s">
-        <v>3203</v>
+        <v>3181</v>
       </c>
       <c r="AN39" s="3" t="s">
-        <v>3205</v>
+        <v>3204</v>
       </c>
     </row>
     <row r="40" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -50243,10 +50240,10 @@
         <v>1</v>
       </c>
       <c r="AM47" s="3" t="s">
-        <v>3203</v>
+        <v>3181</v>
       </c>
       <c r="AN47" s="3" t="s">
-        <v>3206</v>
+        <v>3205</v>
       </c>
     </row>
     <row r="48" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
@@ -50362,10 +50359,10 @@
         <v>1</v>
       </c>
       <c r="AM48" s="3" t="s">
-        <v>3203</v>
+        <v>3181</v>
       </c>
       <c r="AN48" s="3" t="s">
-        <v>3207</v>
+        <v>3206</v>
       </c>
     </row>
     <row r="49" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -50741,7 +50738,7 @@
         <v>3173</v>
       </c>
       <c r="V56" s="3" t="s">
-        <v>3208</v>
+        <v>3207</v>
       </c>
       <c r="W56" s="3" t="s">
         <v>3175</v>
@@ -50789,13 +50786,13 @@
         <v>1</v>
       </c>
       <c r="AL56" s="3" t="s">
-        <v>3209</v>
+        <v>3208</v>
       </c>
       <c r="AM56" s="3" t="s">
         <v>3181</v>
       </c>
       <c r="AN56" s="3" t="s">
-        <v>3210</v>
+        <v>3209</v>
       </c>
     </row>
     <row r="57" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
@@ -50863,7 +50860,7 @@
         <v>3173</v>
       </c>
       <c r="V57" s="3" t="s">
-        <v>3208</v>
+        <v>3207</v>
       </c>
       <c r="W57" s="3" t="s">
         <v>3175</v>
@@ -50911,13 +50908,13 @@
         <v>1</v>
       </c>
       <c r="AL57" s="3" t="s">
-        <v>3211</v>
+        <v>3210</v>
       </c>
       <c r="AM57" s="3" t="s">
         <v>3181</v>
       </c>
       <c r="AN57" s="3" t="s">
-        <v>3212</v>
+        <v>3211</v>
       </c>
     </row>
     <row r="58" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -51293,7 +51290,7 @@
         <v>3173</v>
       </c>
       <c r="V65" s="3" t="s">
-        <v>3208</v>
+        <v>3207</v>
       </c>
       <c r="W65" s="3" t="s">
         <v>3175</v>
@@ -51341,13 +51338,13 @@
         <v>1</v>
       </c>
       <c r="AL65" s="3" t="s">
-        <v>3213</v>
+        <v>3212</v>
       </c>
       <c r="AM65" s="3" t="s">
         <v>3181</v>
       </c>
       <c r="AN65" s="3" t="s">
-        <v>3214</v>
+        <v>3213</v>
       </c>
     </row>
     <row r="66" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
@@ -51415,7 +51412,7 @@
         <v>3173</v>
       </c>
       <c r="V66" s="3" t="s">
-        <v>3208</v>
+        <v>3207</v>
       </c>
       <c r="W66" s="3" t="s">
         <v>3175</v>
@@ -51463,13 +51460,13 @@
         <v>1</v>
       </c>
       <c r="AL66" s="3" t="s">
-        <v>3215</v>
+        <v>3214</v>
       </c>
       <c r="AM66" s="3" t="s">
         <v>3181</v>
       </c>
       <c r="AN66" s="3" t="s">
-        <v>3216</v>
+        <v>3215</v>
       </c>
     </row>
     <row r="67" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat: add IBM Assessment Voucher Bundle modal locators and methods for customization and order addition
</commit_message>
<xml_diff>
--- a/data/BigCommerceData/BigC_Ecomm_TestCases_AutomationMasterSheet.xlsx
+++ b/data/BigCommerceData/BigC_Ecomm_TestCases_AutomationMasterSheet.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19320" uniqueCount="3216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19320" uniqueCount="3217">
   <si>
     <t>Global Test Case ID</t>
   </si>
@@ -9567,19 +9567,22 @@
     <t>Standard product order for existing customer</t>
   </si>
   <si>
-    <t>356989</t>
+    <t>357002</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-15T06:04:22.063Z\nScreenshot: test-results/screenshots/TC0193.png","Status: Passed","Last Updated: 2025-09-15T06:04:22.466Z","---"]</t>
+  </si>
+  <si>
+    <t>356995</t>
   </si>
   <si>
     <t>Failed</t>
   </si>
   <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.59.8.144' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-12T10:40:57.492Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:40:57.600Z","---"]</t>
-  </si>
-  <si>
-    <t>356995</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.59.8.144' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-12T10:41:31.494Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:31.606Z","---"]</t>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Incorrect syntax near ','.","Failure Timestamp: 2025-09-12T11:04:20.886Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:04:21.007Z","---"]</t>
   </si>
   <si>
     <t>USD $20.00</t>
@@ -9588,16 +9591,16 @@
     <t>USD $132.15</t>
   </si>
   <si>
-    <t>356990</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.59.8.144' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-12T10:41:01.947Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:02.077Z","---"]</t>
+    <t>357003</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-15T18:53:54.335Z\nScreenshot: test-results/screenshots/TC0202.png","Status: Passed","Last Updated: 2025-09-15T18:53:54.707Z","---"]</t>
   </si>
   <si>
     <t>356996</t>
   </si>
   <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.59.8.144' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-12T10:41:35.837Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:35.945Z","---"]</t>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Incorrect syntax near ','.","Failure Timestamp: 2025-09-12T11:04:28.316Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:04:28.427Z","---"]</t>
   </si>
   <si>
     <t>Customer transfers money directly to the seller's bank account.</t>
@@ -9606,25 +9609,25 @@
     <t>356991</t>
   </si>
   <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.59.8.144' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-12T10:41:06.455Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:06.590Z","---"]</t>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Incorrect syntax near ','.","Failure Timestamp: 2025-09-12T11:03:45.398Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:03:45.504Z","---"]</t>
   </si>
   <si>
     <t>356997</t>
   </si>
   <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.59.8.144' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-12T10:41:40.257Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:40.365Z","---"]</t>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Incorrect syntax near ','.","Failure Timestamp: 2025-09-12T11:04:35.859Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:04:35.983Z","---"]</t>
   </si>
   <si>
     <t>356992</t>
   </si>
   <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.59.8.144' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-12T10:41:11.144Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:11.262Z","---"]</t>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Incorrect syntax near ','.","Failure Timestamp: 2025-09-12T11:03:52.746Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:03:52.851Z","---"]</t>
   </si>
   <si>
     <t>356998</t>
   </si>
   <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.59.8.144' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-12T10:41:44.860Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:44.985Z","---"]</t>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Incorrect syntax near ','.","Failure Timestamp: 2025-09-12T11:04:43.426Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:04:43.545Z","---"]</t>
   </si>
   <si>
     <t>A real payment gateway/service provider (owned by Visa).</t>
@@ -9636,16 +9639,16 @@
     <t>American Express</t>
   </si>
   <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Order_Id not found in Excel sheet. Ensure the order has been created first.","Failure Timestamp: 2025-09-12T10:41:14.289Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:14.410Z","---"]</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Order_Id not found in Excel sheet. Ensure the order has been created first.","Failure Timestamp: 2025-09-12T10:41:47.711Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:47.826Z","---"]</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Order_Id not found in Excel sheet. Ensure the order has been created first.","Failure Timestamp: 2025-09-12T10:41:17.189Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:17.329Z","---"]</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Order_Id not found in Excel sheet. Ensure the order has been created first.","Failure Timestamp: 2025-09-12T10:41:50.540Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:50.655Z","---"]</t>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Order_Id not found in Excel sheet. Ensure the order has been created first.","Failure Timestamp: 2025-09-12T11:03:55.400Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:03:55.512Z","---"]</t>
+  </si>
+  <si>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Order_Id not found in Excel sheet. Ensure the order has been created first.","Failure Timestamp: 2025-09-12T11:04:46.190Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:04:46.297Z","---"]</t>
+  </si>
+  <si>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Order_Id not found in Excel sheet. Ensure the order has been created first.","Failure Timestamp: 2025-09-12T11:03:57.983Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:03:58.094Z","---"]</t>
+  </si>
+  <si>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Order_Id not found in Excel sheet. Ensure the order has been created first.","Failure Timestamp: 2025-09-12T11:04:48.784Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:04:48.891Z","---"]</t>
   </si>
   <si>
     <t>Manual payment</t>
@@ -9654,25 +9657,25 @@
     <t>356993</t>
   </si>
   <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.59.8.144' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-12T10:41:22.217Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:22.328Z","---"]</t>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Incorrect syntax near ','.","Failure Timestamp: 2025-09-12T11:04:05.520Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:04:05.627Z","---"]</t>
   </si>
   <si>
     <t>356999</t>
   </si>
   <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.59.8.144' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-12T10:41:55.566Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:55.682Z","---"]</t>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Incorrect syntax near ','.","Failure Timestamp: 2025-09-12T11:04:56.375Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:04:56.499Z","---"]</t>
   </si>
   <si>
     <t>356994</t>
   </si>
   <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.59.8.144' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-12T10:41:26.960Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:41:27.070Z","---"]</t>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Incorrect syntax near ','.","Failure Timestamp: 2025-09-12T11:04:13.189Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:04:13.306Z","---"]</t>
   </si>
   <si>
     <t>357000</t>
   </si>
   <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.59.8.144' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-12T10:42:01.534Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T10:42:01.651Z","---"]</t>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Incorrect syntax near ','.","Failure Timestamp: 2025-09-12T11:05:04.126Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:05:04.245Z","---"]</t>
   </si>
 </sst>
 </file>
@@ -47611,10 +47614,10 @@
         <v>3183</v>
       </c>
       <c r="AM3" s="3" t="s">
-        <v>3181</v>
+        <v>3184</v>
       </c>
       <c r="AN3" s="3" t="s">
-        <v>3184</v>
+        <v>3185</v>
       </c>
     </row>
     <row r="4" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -47999,7 +48002,7 @@
         <v>3176</v>
       </c>
       <c r="Y11" s="3" t="s">
-        <v>3185</v>
+        <v>3186</v>
       </c>
       <c r="Z11" s="3" t="s">
         <v>3172</v>
@@ -48008,7 +48011,7 @@
         <v>3177</v>
       </c>
       <c r="AB11" s="8" t="s">
-        <v>3186</v>
+        <v>3187</v>
       </c>
       <c r="AC11" s="9">
         <v>0</v>
@@ -48038,13 +48041,13 @@
         <v>1</v>
       </c>
       <c r="AL11" s="3" t="s">
-        <v>3187</v>
+        <v>3188</v>
       </c>
       <c r="AM11" s="3" t="s">
         <v>3181</v>
       </c>
       <c r="AN11" s="3" t="s">
-        <v>3188</v>
+        <v>3189</v>
       </c>
     </row>
     <row r="12" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
@@ -48121,7 +48124,7 @@
         <v>3176</v>
       </c>
       <c r="Y12" s="3" t="s">
-        <v>3185</v>
+        <v>3186</v>
       </c>
       <c r="Z12" s="3" t="s">
         <v>3172</v>
@@ -48130,7 +48133,7 @@
         <v>3177</v>
       </c>
       <c r="AB12" s="8" t="s">
-        <v>3186</v>
+        <v>3187</v>
       </c>
       <c r="AC12" s="9">
         <v>0</v>
@@ -48160,13 +48163,13 @@
         <v>1</v>
       </c>
       <c r="AL12" s="3" t="s">
-        <v>3189</v>
+        <v>3190</v>
       </c>
       <c r="AM12" s="3" t="s">
-        <v>3181</v>
+        <v>3184</v>
       </c>
       <c r="AN12" s="3" t="s">
-        <v>3190</v>
+        <v>3191</v>
       </c>
     </row>
     <row r="13" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -48545,7 +48548,7 @@
         <v>123</v>
       </c>
       <c r="W20" s="3" t="s">
-        <v>3191</v>
+        <v>3192</v>
       </c>
       <c r="X20" s="3" t="s">
         <v>3176</v>
@@ -48590,13 +48593,13 @@
         <v>1</v>
       </c>
       <c r="AL20" s="3" t="s">
-        <v>3192</v>
+        <v>3193</v>
       </c>
       <c r="AM20" s="3" t="s">
-        <v>3181</v>
+        <v>3184</v>
       </c>
       <c r="AN20" s="3" t="s">
-        <v>3193</v>
+        <v>3194</v>
       </c>
     </row>
     <row r="21" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
@@ -48712,13 +48715,13 @@
         <v>1</v>
       </c>
       <c r="AL21" s="3" t="s">
-        <v>3194</v>
+        <v>3195</v>
       </c>
       <c r="AM21" s="3" t="s">
-        <v>3181</v>
+        <v>3184</v>
       </c>
       <c r="AN21" s="3" t="s">
-        <v>3195</v>
+        <v>3196</v>
       </c>
     </row>
     <row r="22" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -49097,13 +49100,13 @@
         <v>123</v>
       </c>
       <c r="W29" s="3" t="s">
-        <v>3191</v>
+        <v>3192</v>
       </c>
       <c r="X29" s="3" t="s">
         <v>3176</v>
       </c>
       <c r="Y29" s="3" t="s">
-        <v>3185</v>
+        <v>3186</v>
       </c>
       <c r="Z29" s="3" t="s">
         <v>3172</v>
@@ -49112,7 +49115,7 @@
         <v>3177</v>
       </c>
       <c r="AB29" s="8" t="s">
-        <v>3186</v>
+        <v>3187</v>
       </c>
       <c r="AC29" s="9">
         <v>0</v>
@@ -49142,13 +49145,13 @@
         <v>1</v>
       </c>
       <c r="AL29" s="3" t="s">
-        <v>3196</v>
+        <v>3197</v>
       </c>
       <c r="AM29" s="3" t="s">
-        <v>3181</v>
+        <v>3184</v>
       </c>
       <c r="AN29" s="3" t="s">
-        <v>3197</v>
+        <v>3198</v>
       </c>
     </row>
     <row r="30" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
@@ -49225,7 +49228,7 @@
         <v>3176</v>
       </c>
       <c r="Y30" s="3" t="s">
-        <v>3185</v>
+        <v>3186</v>
       </c>
       <c r="Z30" s="3" t="s">
         <v>3172</v>
@@ -49234,7 +49237,7 @@
         <v>3177</v>
       </c>
       <c r="AB30" s="8" t="s">
-        <v>3186</v>
+        <v>3187</v>
       </c>
       <c r="AC30" s="9">
         <v>0</v>
@@ -49264,13 +49267,13 @@
         <v>1</v>
       </c>
       <c r="AL30" s="3" t="s">
-        <v>3198</v>
+        <v>3199</v>
       </c>
       <c r="AM30" s="3" t="s">
-        <v>3181</v>
+        <v>3184</v>
       </c>
       <c r="AN30" s="3" t="s">
-        <v>3199</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="31" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -49649,7 +49652,7 @@
         <v>214</v>
       </c>
       <c r="W38" s="3" t="s">
-        <v>3200</v>
+        <v>3201</v>
       </c>
       <c r="X38" s="3" t="s">
         <v>3176</v>
@@ -49676,10 +49679,10 @@
         <v>3179</v>
       </c>
       <c r="AF38" s="3" t="s">
-        <v>3201</v>
+        <v>3202</v>
       </c>
       <c r="AG38" s="3" t="s">
-        <v>3202</v>
+        <v>3203</v>
       </c>
       <c r="AH38" s="3">
         <v>234234523</v>
@@ -49694,10 +49697,10 @@
         <v>1</v>
       </c>
       <c r="AM38" s="3" t="s">
-        <v>3181</v>
+        <v>3184</v>
       </c>
       <c r="AN38" s="3" t="s">
-        <v>3203</v>
+        <v>3204</v>
       </c>
     </row>
     <row r="39" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
@@ -49795,10 +49798,10 @@
         <v>3179</v>
       </c>
       <c r="AF39" s="3" t="s">
-        <v>3201</v>
+        <v>3202</v>
       </c>
       <c r="AG39" s="3" t="s">
-        <v>3202</v>
+        <v>3203</v>
       </c>
       <c r="AH39" s="3">
         <v>234234523</v>
@@ -49813,10 +49816,10 @@
         <v>1</v>
       </c>
       <c r="AM39" s="3" t="s">
-        <v>3181</v>
+        <v>3184</v>
       </c>
       <c r="AN39" s="3" t="s">
-        <v>3204</v>
+        <v>3205</v>
       </c>
     </row>
     <row r="40" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -50195,13 +50198,13 @@
         <v>214</v>
       </c>
       <c r="W47" s="3" t="s">
-        <v>3200</v>
+        <v>3201</v>
       </c>
       <c r="X47" s="3" t="s">
         <v>3176</v>
       </c>
       <c r="Y47" s="3" t="s">
-        <v>3185</v>
+        <v>3186</v>
       </c>
       <c r="Z47" s="3" t="s">
         <v>3172</v>
@@ -50210,7 +50213,7 @@
         <v>3177</v>
       </c>
       <c r="AB47" s="8" t="s">
-        <v>3186</v>
+        <v>3187</v>
       </c>
       <c r="AC47" s="9">
         <v>0</v>
@@ -50222,10 +50225,10 @@
         <v>3179</v>
       </c>
       <c r="AF47" s="3" t="s">
-        <v>3201</v>
+        <v>3202</v>
       </c>
       <c r="AG47" s="3" t="s">
-        <v>3202</v>
+        <v>3203</v>
       </c>
       <c r="AH47" s="3">
         <v>234234523</v>
@@ -50240,10 +50243,10 @@
         <v>1</v>
       </c>
       <c r="AM47" s="3" t="s">
-        <v>3181</v>
+        <v>3184</v>
       </c>
       <c r="AN47" s="3" t="s">
-        <v>3205</v>
+        <v>3206</v>
       </c>
     </row>
     <row r="48" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
@@ -50320,7 +50323,7 @@
         <v>3176</v>
       </c>
       <c r="Y48" s="3" t="s">
-        <v>3185</v>
+        <v>3186</v>
       </c>
       <c r="Z48" s="3" t="s">
         <v>3172</v>
@@ -50329,7 +50332,7 @@
         <v>3177</v>
       </c>
       <c r="AB48" s="8" t="s">
-        <v>3186</v>
+        <v>3187</v>
       </c>
       <c r="AC48" s="9">
         <v>0</v>
@@ -50341,10 +50344,10 @@
         <v>3179</v>
       </c>
       <c r="AF48" s="3" t="s">
-        <v>3201</v>
+        <v>3202</v>
       </c>
       <c r="AG48" s="3" t="s">
-        <v>3202</v>
+        <v>3203</v>
       </c>
       <c r="AH48" s="3">
         <v>234234523</v>
@@ -50359,10 +50362,10 @@
         <v>1</v>
       </c>
       <c r="AM48" s="3" t="s">
-        <v>3181</v>
+        <v>3184</v>
       </c>
       <c r="AN48" s="3" t="s">
-        <v>3206</v>
+        <v>3207</v>
       </c>
     </row>
     <row r="49" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -50738,7 +50741,7 @@
         <v>3173</v>
       </c>
       <c r="V56" s="3" t="s">
-        <v>3207</v>
+        <v>3208</v>
       </c>
       <c r="W56" s="3" t="s">
         <v>3175</v>
@@ -50786,13 +50789,13 @@
         <v>1</v>
       </c>
       <c r="AL56" s="3" t="s">
-        <v>3208</v>
+        <v>3209</v>
       </c>
       <c r="AM56" s="3" t="s">
-        <v>3181</v>
+        <v>3184</v>
       </c>
       <c r="AN56" s="3" t="s">
-        <v>3209</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="57" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
@@ -50860,7 +50863,7 @@
         <v>3173</v>
       </c>
       <c r="V57" s="3" t="s">
-        <v>3207</v>
+        <v>3208</v>
       </c>
       <c r="W57" s="3" t="s">
         <v>3175</v>
@@ -50908,13 +50911,13 @@
         <v>1</v>
       </c>
       <c r="AL57" s="3" t="s">
-        <v>3210</v>
+        <v>3211</v>
       </c>
       <c r="AM57" s="3" t="s">
-        <v>3181</v>
+        <v>3184</v>
       </c>
       <c r="AN57" s="3" t="s">
-        <v>3211</v>
+        <v>3212</v>
       </c>
     </row>
     <row r="58" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -51290,7 +51293,7 @@
         <v>3173</v>
       </c>
       <c r="V65" s="3" t="s">
-        <v>3207</v>
+        <v>3208</v>
       </c>
       <c r="W65" s="3" t="s">
         <v>3175</v>
@@ -51299,7 +51302,7 @@
         <v>3176</v>
       </c>
       <c r="Y65" s="3" t="s">
-        <v>3185</v>
+        <v>3186</v>
       </c>
       <c r="Z65" s="3" t="s">
         <v>3172</v>
@@ -51308,7 +51311,7 @@
         <v>3177</v>
       </c>
       <c r="AB65" s="8" t="s">
-        <v>3186</v>
+        <v>3187</v>
       </c>
       <c r="AC65" s="9">
         <v>0</v>
@@ -51338,13 +51341,13 @@
         <v>1</v>
       </c>
       <c r="AL65" s="3" t="s">
-        <v>3212</v>
+        <v>3213</v>
       </c>
       <c r="AM65" s="3" t="s">
-        <v>3181</v>
+        <v>3184</v>
       </c>
       <c r="AN65" s="3" t="s">
-        <v>3213</v>
+        <v>3214</v>
       </c>
     </row>
     <row r="66" ht="43.2" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
@@ -51412,7 +51415,7 @@
         <v>3173</v>
       </c>
       <c r="V66" s="3" t="s">
-        <v>3207</v>
+        <v>3208</v>
       </c>
       <c r="W66" s="3" t="s">
         <v>3175</v>
@@ -51421,7 +51424,7 @@
         <v>3176</v>
       </c>
       <c r="Y66" s="3" t="s">
-        <v>3185</v>
+        <v>3186</v>
       </c>
       <c r="Z66" s="3" t="s">
         <v>3172</v>
@@ -51430,7 +51433,7 @@
         <v>3177</v>
       </c>
       <c r="AB66" s="8" t="s">
-        <v>3186</v>
+        <v>3187</v>
       </c>
       <c r="AC66" s="9">
         <v>0</v>
@@ -51460,13 +51463,13 @@
         <v>1</v>
       </c>
       <c r="AL66" s="3" t="s">
-        <v>3214</v>
+        <v>3215</v>
       </c>
       <c r="AM66" s="3" t="s">
-        <v>3181</v>
+        <v>3184</v>
       </c>
       <c r="AN66" s="3" t="s">
-        <v>3215</v>
+        <v>3216</v>
       </c>
     </row>
     <row r="67" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
chore: update BigC_Ecomm_TestCases_AutomationMasterSheet.xlsx with new test cases
</commit_message>
<xml_diff>
--- a/data/BigCommerceData/BigC_Ecomm_TestCases_AutomationMasterSheet.xlsx
+++ b/data/BigCommerceData/BigC_Ecomm_TestCases_AutomationMasterSheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C65D02A-9969-4891-BF1B-81B6A0322274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47AC47ED-46B1-4381-A640-CC3828D1CC8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20336" uniqueCount="3261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20296" uniqueCount="3239">
   <si>
     <t>Global Test Case ID</t>
   </si>
@@ -9574,69 +9574,18 @@
     <t>Failed</t>
   </si>
   <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Query 'select * from [order] where entityorderid = @OrderNumber' not found","Failure Timestamp: 2025-09-24T09:05:53.200Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-24T09:05:53.324Z","---"]</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Cannot open server 'vue-dv-bpkdb' requested by the login. Client with IP address '152.58.17.69' is not allowed to access the server.  To enable access, use the Azure Management Portal or run sp_set_firewall_rule on the master database to create a firewall rule for this IP address or address range.  It may take up to five minutes for this change to take effect.","Failure Timestamp: 2025-09-24T13:12:22.584Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-24T13:12:22.732Z","---"]</t>
-  </si>
-  <si>
-    <t>356995</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Incorrect syntax near ','.","Failure Timestamp: 2025-09-12T11:04:20.886Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:04:21.007Z","---"]</t>
-  </si>
-  <si>
-    <t>357002</t>
-  </si>
-  <si>
     <t>USD $20.00</t>
   </si>
   <si>
     <t>USD $132.15</t>
   </si>
   <si>
-    <t>357003</t>
-  </si>
-  <si>
     <t>Passed</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-15T18:53:54.335Z\nScreenshot: test-results/screenshots/TC0202.png","Status: Passed","Last Updated: 2025-09-15T18:53:54.707Z","---"]</t>
-  </si>
-  <si>
-    <t>356996</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Incorrect syntax near ','.","Failure Timestamp: 2025-09-12T11:04:28.316Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:04:28.427Z","---"]</t>
-  </si>
-  <si>
     <t>Customer transfers money directly to the seller's bank account.</t>
   </si>
   <si>
-    <t>356991</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Incorrect syntax near ','.","Failure Timestamp: 2025-09-12T11:03:45.398Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:03:45.504Z","---"]</t>
-  </si>
-  <si>
-    <t>356997</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Incorrect syntax near ','.","Failure Timestamp: 2025-09-12T11:04:35.859Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:04:35.983Z","---"]</t>
-  </si>
-  <si>
-    <t>356992</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Incorrect syntax near ','.","Failure Timestamp: 2025-09-12T11:03:52.746Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:03:52.851Z","---"]</t>
-  </si>
-  <si>
-    <t>356998</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Incorrect syntax near ','.","Failure Timestamp: 2025-09-12T11:04:43.426Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:04:43.545Z","---"]</t>
-  </si>
-  <si>
     <t>A real payment gateway/service provider (owned by Visa).</t>
   </si>
   <si>
@@ -9646,45 +9595,9 @@
     <t>American Express</t>
   </si>
   <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Order_Id not found in Excel sheet. Ensure the order has been created first.","Failure Timestamp: 2025-09-12T11:03:55.400Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:03:55.512Z","---"]</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Order_Id not found in Excel sheet. Ensure the order has been created first.","Failure Timestamp: 2025-09-12T11:04:46.190Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:04:46.297Z","---"]</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Order_Id not found in Excel sheet. Ensure the order has been created first.","Failure Timestamp: 2025-09-12T11:03:57.983Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:03:58.094Z","---"]</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Order_Id not found in Excel sheet. Ensure the order has been created first.","Failure Timestamp: 2025-09-12T11:04:48.784Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:04:48.891Z","---"]</t>
-  </si>
-  <si>
     <t>Manual payment</t>
   </si>
   <si>
-    <t>356993</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Incorrect syntax near ','.","Failure Timestamp: 2025-09-12T11:04:05.520Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:04:05.627Z","---"]</t>
-  </si>
-  <si>
-    <t>356999</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Incorrect syntax near ','.","Failure Timestamp: 2025-09-12T11:04:56.375Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:04:56.499Z","---"]</t>
-  </si>
-  <si>
-    <t>356994</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Incorrect syntax near ','.","Failure Timestamp: 2025-09-12T11:04:13.189Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:04:13.306Z","---"]</t>
-  </si>
-  <si>
-    <t>357000</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Database verification failed: Incorrect syntax near ','.","Failure Timestamp: 2025-09-12T11:05:04.126Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-12T11:05:04.245Z","---"]</t>
-  </si>
-  <si>
     <t>Bundle_Name</t>
   </si>
   <si>
@@ -9809,6 +9722,27 @@
   </si>
   <si>
     <t>KIBO_OrderId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execution_Notes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last_Run_Date </t>
+  </si>
+  <si>
+    <t>BigC_Test_Result</t>
+  </si>
+  <si>
+    <t>DB_Execution_Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DB_Test_Result </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pearson_Test_Result </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pearson_Execution_Notes </t>
   </si>
 </sst>
 </file>
@@ -47347,10 +47281,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AQ73"/>
+  <dimension ref="A1:AV73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="AO2" sqref="AO2"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -47392,16 +47326,21 @@
     <col min="36" max="36" width="17.33203125" style="3" customWidth="1"/>
     <col min="37" max="37" width="14.33203125" style="3" customWidth="1"/>
     <col min="38" max="38" width="12.5546875" style="3" customWidth="1"/>
-    <col min="39" max="39" width="13.77734375" style="3" customWidth="1"/>
-    <col min="40" max="40" width="75.44140625" style="3" customWidth="1"/>
-    <col min="41" max="41" width="18.5546875" style="3" customWidth="1"/>
-    <col min="42" max="42" width="18.33203125" style="3" customWidth="1"/>
-    <col min="43" max="43" width="27.5546875" style="3" customWidth="1"/>
-    <col min="44" max="44" width="9.109375" style="3" customWidth="1"/>
-    <col min="45" max="16384" width="9.109375" style="3"/>
+    <col min="39" max="39" width="18.5546875" style="3" customWidth="1"/>
+    <col min="40" max="40" width="13.77734375" style="3" customWidth="1"/>
+    <col min="41" max="41" width="27" style="3" customWidth="1"/>
+    <col min="42" max="42" width="21.88671875" customWidth="1"/>
+    <col min="43" max="43" width="26.33203125" style="3" customWidth="1"/>
+    <col min="44" max="44" width="31.5546875" style="3" customWidth="1"/>
+    <col min="45" max="45" width="39.77734375" style="3" customWidth="1"/>
+    <col min="46" max="46" width="34.5546875" style="3" customWidth="1"/>
+    <col min="47" max="47" width="27.88671875" style="3" customWidth="1"/>
+    <col min="48" max="48" width="26.109375" style="3" customWidth="1"/>
+    <col min="49" max="51" width="18.33203125" style="3" customWidth="1"/>
+    <col min="52" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="4" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:48" s="4" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -47514,25 +47453,40 @@
         <v>3167</v>
       </c>
       <c r="AL1" s="6" t="s">
-        <v>3259</v>
-      </c>
-      <c r="AM1" s="4" t="s">
+        <v>3230</v>
+      </c>
+      <c r="AM1" s="6" t="s">
+        <v>3231</v>
+      </c>
+      <c r="AN1" s="4" t="s">
         <v>3169</v>
       </c>
-      <c r="AN1" s="4" t="s">
-        <v>3170</v>
-      </c>
-      <c r="AO1" s="6" t="s">
-        <v>3260</v>
+      <c r="AO1" s="4" t="s">
+        <v>3232</v>
       </c>
       <c r="AP1" s="4" t="s">
+        <v>3233</v>
+      </c>
+      <c r="AQ1" s="4" t="s">
         <v>3171</v>
       </c>
-      <c r="AQ1" s="4" t="s">
-        <v>3170</v>
-      </c>
-    </row>
-    <row r="2" spans="1:43" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AR1" s="4" t="s">
+        <v>3234</v>
+      </c>
+      <c r="AS1" s="4" t="s">
+        <v>3236</v>
+      </c>
+      <c r="AT1" s="4" t="s">
+        <v>3235</v>
+      </c>
+      <c r="AU1" s="4" t="s">
+        <v>3237</v>
+      </c>
+      <c r="AV1" s="4" t="s">
+        <v>3238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:48" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -47644,23 +47598,8 @@
       <c r="AK2" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="AL2" s="3">
-        <v>433038</v>
-      </c>
-      <c r="AM2" s="3" t="s">
-        <v>3181</v>
-      </c>
-      <c r="AN2" s="3" t="s">
-        <v>3182</v>
-      </c>
-      <c r="AO2" s="3">
-        <v>433038</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
-        <v>3183</v>
-      </c>
-    </row>
-    <row r="3" spans="1:43" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:48" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
@@ -47772,20 +47711,8 @@
       <c r="AK3" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="AL3" s="3" t="s">
-        <v>3184</v>
-      </c>
-      <c r="AM3" s="3" t="s">
-        <v>3181</v>
-      </c>
-      <c r="AN3" s="3" t="s">
-        <v>3185</v>
-      </c>
-      <c r="AO3" s="3" t="s">
-        <v>3186</v>
-      </c>
-    </row>
-    <row r="4" spans="1:43" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:48" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>35</v>
       </c>
@@ -47829,7 +47756,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:43" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>42</v>
       </c>
@@ -47873,7 +47800,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:43" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>48</v>
       </c>
@@ -47917,7 +47844,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:43" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>53</v>
       </c>
@@ -47961,7 +47888,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:43" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>58</v>
       </c>
@@ -48005,7 +47932,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:43" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>64</v>
       </c>
@@ -48049,7 +47976,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:43" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>69</v>
       </c>
@@ -48093,7 +48020,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:43" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:48" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>74</v>
       </c>
@@ -48167,7 +48094,7 @@
         <v>3177</v>
       </c>
       <c r="Y11" s="3" t="s">
-        <v>3187</v>
+        <v>3182</v>
       </c>
       <c r="Z11" s="3" t="s">
         <v>3173</v>
@@ -48176,7 +48103,7 @@
         <v>3178</v>
       </c>
       <c r="AB11" s="8" t="s">
-        <v>3188</v>
+        <v>3183</v>
       </c>
       <c r="AC11" s="9">
         <v>0</v>
@@ -48205,17 +48132,8 @@
       <c r="AK11" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="AL11" s="3" t="s">
-        <v>3189</v>
-      </c>
-      <c r="AM11" s="3" t="s">
-        <v>3190</v>
-      </c>
-      <c r="AN11" s="3" t="s">
-        <v>3191</v>
-      </c>
-    </row>
-    <row r="12" spans="1:43" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:48" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>80</v>
       </c>
@@ -48289,7 +48207,7 @@
         <v>3177</v>
       </c>
       <c r="Y12" s="3" t="s">
-        <v>3187</v>
+        <v>3182</v>
       </c>
       <c r="Z12" s="3" t="s">
         <v>3173</v>
@@ -48298,7 +48216,7 @@
         <v>3178</v>
       </c>
       <c r="AB12" s="8" t="s">
-        <v>3188</v>
+        <v>3183</v>
       </c>
       <c r="AC12" s="9">
         <v>0</v>
@@ -48327,17 +48245,8 @@
       <c r="AK12" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="AL12" s="3" t="s">
-        <v>3192</v>
-      </c>
-      <c r="AM12" s="3" t="s">
-        <v>3181</v>
-      </c>
-      <c r="AN12" s="3" t="s">
-        <v>3193</v>
-      </c>
-    </row>
-    <row r="13" spans="1:43" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:48" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>85</v>
       </c>
@@ -48381,7 +48290,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:43" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>90</v>
       </c>
@@ -48425,7 +48334,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:43" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>95</v>
       </c>
@@ -48469,7 +48378,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:43" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>100</v>
       </c>
@@ -48513,7 +48422,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>105</v>
       </c>
@@ -48557,7 +48466,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>110</v>
       </c>
@@ -48601,7 +48510,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>115</v>
       </c>
@@ -48645,7 +48554,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:40" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>120</v>
       </c>
@@ -48713,7 +48622,7 @@
         <v>123</v>
       </c>
       <c r="W20" s="3" t="s">
-        <v>3194</v>
+        <v>3185</v>
       </c>
       <c r="X20" s="3" t="s">
         <v>3177</v>
@@ -48757,17 +48666,8 @@
       <c r="AK20" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="AL20" s="3" t="s">
-        <v>3195</v>
-      </c>
-      <c r="AM20" s="3" t="s">
-        <v>3181</v>
-      </c>
-      <c r="AN20" s="3" t="s">
-        <v>3196</v>
-      </c>
-    </row>
-    <row r="21" spans="1:40" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:37" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>126</v>
       </c>
@@ -48879,17 +48779,8 @@
       <c r="AK21" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="AL21" s="3" t="s">
-        <v>3197</v>
-      </c>
-      <c r="AM21" s="3" t="s">
-        <v>3181</v>
-      </c>
-      <c r="AN21" s="3" t="s">
-        <v>3198</v>
-      </c>
-    </row>
-    <row r="22" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>131</v>
       </c>
@@ -48933,7 +48824,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>136</v>
       </c>
@@ -48977,7 +48868,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>141</v>
       </c>
@@ -49021,7 +48912,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="25" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>146</v>
       </c>
@@ -49065,7 +48956,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>151</v>
       </c>
@@ -49109,7 +49000,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="27" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>156</v>
       </c>
@@ -49153,7 +49044,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="28" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>161</v>
       </c>
@@ -49197,7 +49088,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="29" spans="1:40" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>166</v>
       </c>
@@ -49265,13 +49156,13 @@
         <v>123</v>
       </c>
       <c r="W29" s="3" t="s">
-        <v>3194</v>
+        <v>3185</v>
       </c>
       <c r="X29" s="3" t="s">
         <v>3177</v>
       </c>
       <c r="Y29" s="3" t="s">
-        <v>3187</v>
+        <v>3182</v>
       </c>
       <c r="Z29" s="3" t="s">
         <v>3173</v>
@@ -49280,7 +49171,7 @@
         <v>3178</v>
       </c>
       <c r="AB29" s="8" t="s">
-        <v>3188</v>
+        <v>3183</v>
       </c>
       <c r="AC29" s="9">
         <v>0</v>
@@ -49309,17 +49200,8 @@
       <c r="AK29" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="AL29" s="3" t="s">
-        <v>3199</v>
-      </c>
-      <c r="AM29" s="3" t="s">
-        <v>3181</v>
-      </c>
-      <c r="AN29" s="3" t="s">
-        <v>3200</v>
-      </c>
-    </row>
-    <row r="30" spans="1:40" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:37" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>171</v>
       </c>
@@ -49393,7 +49275,7 @@
         <v>3177</v>
       </c>
       <c r="Y30" s="3" t="s">
-        <v>3187</v>
+        <v>3182</v>
       </c>
       <c r="Z30" s="3" t="s">
         <v>3173</v>
@@ -49402,7 +49284,7 @@
         <v>3178</v>
       </c>
       <c r="AB30" s="8" t="s">
-        <v>3188</v>
+        <v>3183</v>
       </c>
       <c r="AC30" s="9">
         <v>0</v>
@@ -49431,17 +49313,8 @@
       <c r="AK30" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="AL30" s="3" t="s">
-        <v>3201</v>
-      </c>
-      <c r="AM30" s="3" t="s">
-        <v>3181</v>
-      </c>
-      <c r="AN30" s="3" t="s">
-        <v>3202</v>
-      </c>
-    </row>
-    <row r="31" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>176</v>
       </c>
@@ -49485,7 +49358,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="32" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>181</v>
       </c>
@@ -49529,7 +49402,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="33" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>186</v>
       </c>
@@ -49573,7 +49446,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="34" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>191</v>
       </c>
@@ -49617,7 +49490,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="35" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>196</v>
       </c>
@@ -49661,7 +49534,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="36" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>201</v>
       </c>
@@ -49705,7 +49578,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="37" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>206</v>
       </c>
@@ -49749,7 +49622,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="38" spans="1:40" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:37" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>211</v>
       </c>
@@ -49817,7 +49690,7 @@
         <v>214</v>
       </c>
       <c r="W38" s="3" t="s">
-        <v>3203</v>
+        <v>3186</v>
       </c>
       <c r="X38" s="3" t="s">
         <v>3177</v>
@@ -49844,10 +49717,10 @@
         <v>3180</v>
       </c>
       <c r="AF38" s="3" t="s">
-        <v>3204</v>
+        <v>3187</v>
       </c>
       <c r="AG38" s="3" t="s">
-        <v>3205</v>
+        <v>3188</v>
       </c>
       <c r="AH38" s="3">
         <v>234234523</v>
@@ -49861,14 +49734,8 @@
       <c r="AK38" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="AM38" s="3" t="s">
-        <v>3181</v>
-      </c>
-      <c r="AN38" s="3" t="s">
-        <v>3206</v>
-      </c>
-    </row>
-    <row r="39" spans="1:40" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:37" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>217</v>
       </c>
@@ -49963,10 +49830,10 @@
         <v>3180</v>
       </c>
       <c r="AF39" s="3" t="s">
-        <v>3204</v>
+        <v>3187</v>
       </c>
       <c r="AG39" s="3" t="s">
-        <v>3205</v>
+        <v>3188</v>
       </c>
       <c r="AH39" s="3">
         <v>234234523</v>
@@ -49980,14 +49847,8 @@
       <c r="AK39" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="AM39" s="3" t="s">
-        <v>3181</v>
-      </c>
-      <c r="AN39" s="3" t="s">
-        <v>3207</v>
-      </c>
-    </row>
-    <row r="40" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>222</v>
       </c>
@@ -50031,7 +49892,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="41" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>227</v>
       </c>
@@ -50075,7 +49936,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="42" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>232</v>
       </c>
@@ -50119,7 +49980,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="43" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>237</v>
       </c>
@@ -50163,7 +50024,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="44" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>242</v>
       </c>
@@ -50207,7 +50068,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="45" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>247</v>
       </c>
@@ -50251,7 +50112,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="46" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>252</v>
       </c>
@@ -50295,7 +50156,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="47" spans="1:40" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:37" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>257</v>
       </c>
@@ -50363,13 +50224,13 @@
         <v>214</v>
       </c>
       <c r="W47" s="3" t="s">
-        <v>3203</v>
+        <v>3186</v>
       </c>
       <c r="X47" s="3" t="s">
         <v>3177</v>
       </c>
       <c r="Y47" s="3" t="s">
-        <v>3187</v>
+        <v>3182</v>
       </c>
       <c r="Z47" s="3" t="s">
         <v>3173</v>
@@ -50378,7 +50239,7 @@
         <v>3178</v>
       </c>
       <c r="AB47" s="8" t="s">
-        <v>3188</v>
+        <v>3183</v>
       </c>
       <c r="AC47" s="9">
         <v>0</v>
@@ -50390,10 +50251,10 @@
         <v>3180</v>
       </c>
       <c r="AF47" s="3" t="s">
-        <v>3204</v>
+        <v>3187</v>
       </c>
       <c r="AG47" s="3" t="s">
-        <v>3205</v>
+        <v>3188</v>
       </c>
       <c r="AH47" s="3">
         <v>234234523</v>
@@ -50407,14 +50268,8 @@
       <c r="AK47" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="AM47" s="3" t="s">
-        <v>3181</v>
-      </c>
-      <c r="AN47" s="3" t="s">
-        <v>3208</v>
-      </c>
-    </row>
-    <row r="48" spans="1:40" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:37" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>262</v>
       </c>
@@ -50488,7 +50343,7 @@
         <v>3177</v>
       </c>
       <c r="Y48" s="3" t="s">
-        <v>3187</v>
+        <v>3182</v>
       </c>
       <c r="Z48" s="3" t="s">
         <v>3173</v>
@@ -50497,7 +50352,7 @@
         <v>3178</v>
       </c>
       <c r="AB48" s="8" t="s">
-        <v>3188</v>
+        <v>3183</v>
       </c>
       <c r="AC48" s="9">
         <v>0</v>
@@ -50509,10 +50364,10 @@
         <v>3180</v>
       </c>
       <c r="AF48" s="3" t="s">
-        <v>3204</v>
+        <v>3187</v>
       </c>
       <c r="AG48" s="3" t="s">
-        <v>3205</v>
+        <v>3188</v>
       </c>
       <c r="AH48" s="3">
         <v>234234523</v>
@@ -50526,14 +50381,8 @@
       <c r="AK48" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="AM48" s="3" t="s">
-        <v>3181</v>
-      </c>
-      <c r="AN48" s="3" t="s">
-        <v>3209</v>
-      </c>
-    </row>
-    <row r="49" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>267</v>
       </c>
@@ -50577,7 +50426,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="50" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>272</v>
       </c>
@@ -50621,7 +50470,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="51" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>277</v>
       </c>
@@ -50665,7 +50514,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="52" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>282</v>
       </c>
@@ -50709,7 +50558,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="53" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>287</v>
       </c>
@@ -50753,7 +50602,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="54" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>292</v>
       </c>
@@ -50797,7 +50646,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="55" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>297</v>
       </c>
@@ -50841,7 +50690,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="56" spans="1:40" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:37" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>302</v>
       </c>
@@ -50906,7 +50755,7 @@
         <v>3174</v>
       </c>
       <c r="V56" s="3" t="s">
-        <v>3210</v>
+        <v>3189</v>
       </c>
       <c r="W56" s="3" t="s">
         <v>3176</v>
@@ -50953,17 +50802,8 @@
       <c r="AK56" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="AL56" s="3" t="s">
-        <v>3211</v>
-      </c>
-      <c r="AM56" s="3" t="s">
-        <v>3181</v>
-      </c>
-      <c r="AN56" s="3" t="s">
-        <v>3212</v>
-      </c>
-    </row>
-    <row r="57" spans="1:40" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:37" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>308</v>
       </c>
@@ -51028,7 +50868,7 @@
         <v>3174</v>
       </c>
       <c r="V57" s="3" t="s">
-        <v>3210</v>
+        <v>3189</v>
       </c>
       <c r="W57" s="3" t="s">
         <v>3176</v>
@@ -51075,17 +50915,8 @@
       <c r="AK57" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="AL57" s="3" t="s">
-        <v>3213</v>
-      </c>
-      <c r="AM57" s="3" t="s">
-        <v>3181</v>
-      </c>
-      <c r="AN57" s="3" t="s">
-        <v>3214</v>
-      </c>
-    </row>
-    <row r="58" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>313</v>
       </c>
@@ -51129,7 +50960,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="59" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>318</v>
       </c>
@@ -51173,7 +51004,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="60" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>323</v>
       </c>
@@ -51217,7 +51048,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="61" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>328</v>
       </c>
@@ -51261,7 +51092,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="62" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>333</v>
       </c>
@@ -51305,7 +51136,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="63" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>338</v>
       </c>
@@ -51349,7 +51180,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="64" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>343</v>
       </c>
@@ -51393,7 +51224,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="65" spans="1:40" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:37" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>348</v>
       </c>
@@ -51458,7 +51289,7 @@
         <v>3174</v>
       </c>
       <c r="V65" s="3" t="s">
-        <v>3210</v>
+        <v>3189</v>
       </c>
       <c r="W65" s="3" t="s">
         <v>3176</v>
@@ -51467,7 +51298,7 @@
         <v>3177</v>
       </c>
       <c r="Y65" s="3" t="s">
-        <v>3187</v>
+        <v>3182</v>
       </c>
       <c r="Z65" s="3" t="s">
         <v>3173</v>
@@ -51476,7 +51307,7 @@
         <v>3178</v>
       </c>
       <c r="AB65" s="8" t="s">
-        <v>3188</v>
+        <v>3183</v>
       </c>
       <c r="AC65" s="9">
         <v>0</v>
@@ -51505,17 +51336,8 @@
       <c r="AK65" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="AL65" s="3" t="s">
-        <v>3215</v>
-      </c>
-      <c r="AM65" s="3" t="s">
-        <v>3181</v>
-      </c>
-      <c r="AN65" s="3" t="s">
-        <v>3216</v>
-      </c>
-    </row>
-    <row r="66" spans="1:40" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:37" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>353</v>
       </c>
@@ -51580,7 +51402,7 @@
         <v>3174</v>
       </c>
       <c r="V66" s="3" t="s">
-        <v>3210</v>
+        <v>3189</v>
       </c>
       <c r="W66" s="3" t="s">
         <v>3176</v>
@@ -51589,7 +51411,7 @@
         <v>3177</v>
       </c>
       <c r="Y66" s="3" t="s">
-        <v>3187</v>
+        <v>3182</v>
       </c>
       <c r="Z66" s="3" t="s">
         <v>3173</v>
@@ -51598,7 +51420,7 @@
         <v>3178</v>
       </c>
       <c r="AB66" s="8" t="s">
-        <v>3188</v>
+        <v>3183</v>
       </c>
       <c r="AC66" s="9">
         <v>0</v>
@@ -51627,17 +51449,8 @@
       <c r="AK66" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="AL66" s="3" t="s">
-        <v>3217</v>
-      </c>
-      <c r="AM66" s="3" t="s">
-        <v>3181</v>
-      </c>
-      <c r="AN66" s="3" t="s">
-        <v>3218</v>
-      </c>
-    </row>
-    <row r="67" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>358</v>
       </c>
@@ -51681,7 +51494,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="68" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>363</v>
       </c>
@@ -51725,7 +51538,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="69" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>368</v>
       </c>
@@ -51769,7 +51582,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="70" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>373</v>
       </c>
@@ -51813,7 +51626,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="71" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>378</v>
       </c>
@@ -51857,7 +51670,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="72" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>383</v>
       </c>
@@ -51901,7 +51714,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="73" spans="1:40" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:37" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>388</v>
       </c>
@@ -51946,7 +51759,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AN73" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <autoFilter ref="A1:AO73" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
@@ -52049,25 +51862,25 @@
         <v>13</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>3219</v>
+        <v>3190</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>3220</v>
+        <v>3191</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>3221</v>
+        <v>3192</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>3222</v>
+        <v>3193</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>3223</v>
+        <v>3194</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>3224</v>
+        <v>3195</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>3225</v>
+        <v>3196</v>
       </c>
       <c r="V1" s="4" t="s">
         <v>3149</v>
@@ -52181,16 +51994,16 @@
         <v>399</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S2" s="3">
         <v>1</v>
@@ -52223,13 +52036,13 @@
         <v>3174</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD2" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF2" s="9">
         <v>0</v>
@@ -52259,13 +52072,13 @@
         <v>1</v>
       </c>
       <c r="AO2" s="3" t="s">
-        <v>3230</v>
+        <v>3201</v>
       </c>
       <c r="AP2" s="3" t="s">
-        <v>3190</v>
+        <v>3184</v>
       </c>
       <c r="AQ2" s="3" t="s">
-        <v>3231</v>
+        <v>3202</v>
       </c>
       <c r="AR2" s="3"/>
     </row>
@@ -52313,16 +52126,16 @@
         <v>405</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S3" s="3">
         <v>1</v>
@@ -52355,13 +52168,13 @@
         <v>3174</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD3" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE3" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF3" s="9">
         <v>0</v>
@@ -52391,13 +52204,13 @@
         <v>1</v>
       </c>
       <c r="AO3" s="3" t="s">
-        <v>3232</v>
+        <v>3203</v>
       </c>
       <c r="AP3" s="3" t="s">
-        <v>3190</v>
+        <v>3184</v>
       </c>
       <c r="AQ3" s="3" t="s">
-        <v>3233</v>
+        <v>3204</v>
       </c>
       <c r="AR3" s="3"/>
     </row>
@@ -52445,16 +52258,16 @@
         <v>411</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S4" s="3">
         <v>1</v>
@@ -52531,16 +52344,16 @@
         <v>416</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q5" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S5" s="3">
         <v>1</v>
@@ -52573,13 +52386,13 @@
         <v>3174</v>
       </c>
       <c r="AC5" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD5" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE5" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF5" s="9">
         <v>0</v>
@@ -52641,16 +52454,16 @@
         <v>421</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q6" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S6" s="3">
         <v>1</v>
@@ -52683,13 +52496,13 @@
         <v>3174</v>
       </c>
       <c r="AC6" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD6" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE6" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF6" s="9">
         <v>0</v>
@@ -52751,16 +52564,16 @@
         <v>426</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q7" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S7" s="3">
         <v>1</v>
@@ -52837,16 +52650,16 @@
         <v>431</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q8" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S8" s="3">
         <v>1</v>
@@ -52879,13 +52692,13 @@
         <v>3174</v>
       </c>
       <c r="AC8" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD8" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE8" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF8" s="9">
         <v>0</v>
@@ -52947,16 +52760,16 @@
         <v>436</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q9" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S9" s="3">
         <v>1</v>
@@ -52989,13 +52802,13 @@
         <v>3174</v>
       </c>
       <c r="AC9" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD9" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE9" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF9" s="9">
         <v>0</v>
@@ -53057,16 +52870,16 @@
         <v>441</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q10" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S10" s="3">
         <v>1</v>
@@ -53143,16 +52956,16 @@
         <v>446</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q11" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S11" s="3">
         <v>1</v>
@@ -53182,16 +52995,16 @@
         <v>3177</v>
       </c>
       <c r="AB11" s="3" t="s">
-        <v>3187</v>
+        <v>3182</v>
       </c>
       <c r="AC11" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD11" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE11" s="8" t="s">
-        <v>3234</v>
+        <v>3205</v>
       </c>
       <c r="AF11" s="9">
         <v>0</v>
@@ -53221,13 +53034,13 @@
         <v>1</v>
       </c>
       <c r="AO11" s="3" t="s">
-        <v>3235</v>
+        <v>3206</v>
       </c>
       <c r="AP11" s="3" t="s">
-        <v>3190</v>
+        <v>3184</v>
       </c>
       <c r="AQ11" s="3" t="s">
-        <v>3236</v>
+        <v>3207</v>
       </c>
       <c r="AR11" s="3"/>
     </row>
@@ -53275,16 +53088,16 @@
         <v>451</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q12" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S12" s="3">
         <v>1</v>
@@ -53314,16 +53127,16 @@
         <v>3177</v>
       </c>
       <c r="AB12" s="3" t="s">
-        <v>3187</v>
+        <v>3182</v>
       </c>
       <c r="AC12" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD12" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE12" s="8" t="s">
-        <v>3234</v>
+        <v>3205</v>
       </c>
       <c r="AF12" s="9">
         <v>0</v>
@@ -53353,13 +53166,13 @@
         <v>1</v>
       </c>
       <c r="AO12" s="3" t="s">
-        <v>3237</v>
+        <v>3208</v>
       </c>
       <c r="AP12" s="3" t="s">
-        <v>3190</v>
+        <v>3184</v>
       </c>
       <c r="AQ12" s="3" t="s">
-        <v>3238</v>
+        <v>3209</v>
       </c>
       <c r="AR12" s="3"/>
     </row>
@@ -53407,16 +53220,16 @@
         <v>456</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q13" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S13" s="3">
         <v>1</v>
@@ -53493,16 +53306,16 @@
         <v>461</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q14" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S14" s="3">
         <v>1</v>
@@ -53535,13 +53348,13 @@
         <v>3174</v>
       </c>
       <c r="AC14" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD14" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE14" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF14" s="9">
         <v>0</v>
@@ -53603,16 +53416,16 @@
         <v>466</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q15" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S15" s="3">
         <v>1</v>
@@ -53645,13 +53458,13 @@
         <v>3174</v>
       </c>
       <c r="AC15" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD15" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE15" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF15" s="9">
         <v>0</v>
@@ -53713,16 +53526,16 @@
         <v>471</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q16" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R16" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S16" s="3">
         <v>1</v>
@@ -53799,16 +53612,16 @@
         <v>476</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q17" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S17" s="3">
         <v>1</v>
@@ -53841,13 +53654,13 @@
         <v>3174</v>
       </c>
       <c r="AC17" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD17" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE17" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF17" s="9">
         <v>0</v>
@@ -53909,16 +53722,16 @@
         <v>481</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q18" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S18" s="3">
         <v>1</v>
@@ -53951,13 +53764,13 @@
         <v>3174</v>
       </c>
       <c r="AC18" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD18" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE18" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF18" s="9">
         <v>0</v>
@@ -54019,16 +53832,16 @@
         <v>486</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q19" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S19" s="3">
         <v>1</v>
@@ -54107,16 +53920,16 @@
         <v>491</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q20" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S20" s="3">
         <v>1</v>
@@ -54140,7 +53953,7 @@
         <v>123</v>
       </c>
       <c r="Z20" s="3" t="s">
-        <v>3194</v>
+        <v>3185</v>
       </c>
       <c r="AA20" s="3" t="s">
         <v>3177</v>
@@ -54149,13 +53962,13 @@
         <v>3174</v>
       </c>
       <c r="AC20" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD20" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE20" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF20" s="9">
         <v>0</v>
@@ -54185,13 +53998,13 @@
         <v>1</v>
       </c>
       <c r="AO20" s="3" t="s">
-        <v>3239</v>
+        <v>3210</v>
       </c>
       <c r="AP20" s="3" t="s">
-        <v>3190</v>
+        <v>3184</v>
       </c>
       <c r="AQ20" s="3" t="s">
-        <v>3240</v>
+        <v>3211</v>
       </c>
       <c r="AR20" s="3"/>
     </row>
@@ -54239,16 +54052,16 @@
         <v>496</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q21" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S21" s="3">
         <v>1</v>
@@ -54281,13 +54094,13 @@
         <v>3174</v>
       </c>
       <c r="AC21" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD21" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE21" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF21" s="9">
         <v>0</v>
@@ -54317,13 +54130,13 @@
         <v>1</v>
       </c>
       <c r="AO21" s="3" t="s">
-        <v>3241</v>
+        <v>3212</v>
       </c>
       <c r="AP21" s="3" t="s">
-        <v>3190</v>
+        <v>3184</v>
       </c>
       <c r="AQ21" s="3" t="s">
-        <v>3242</v>
+        <v>3213</v>
       </c>
       <c r="AR21" s="3"/>
     </row>
@@ -54371,16 +54184,16 @@
         <v>501</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q22" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S22" s="3">
         <v>1</v>
@@ -54457,16 +54270,16 @@
         <v>506</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q23" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R23" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S23" s="3">
         <v>1</v>
@@ -54499,13 +54312,13 @@
         <v>3174</v>
       </c>
       <c r="AC23" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD23" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE23" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF23" s="9">
         <v>0</v>
@@ -54567,16 +54380,16 @@
         <v>511</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q24" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R24" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S24" s="3">
         <v>1</v>
@@ -54609,13 +54422,13 @@
         <v>3174</v>
       </c>
       <c r="AC24" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD24" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE24" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF24" s="9">
         <v>0</v>
@@ -54677,16 +54490,16 @@
         <v>516</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q25" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R25" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S25" s="3">
         <v>1</v>
@@ -54763,16 +54576,16 @@
         <v>521</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q26" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R26" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S26" s="3">
         <v>1</v>
@@ -54805,13 +54618,13 @@
         <v>3174</v>
       </c>
       <c r="AC26" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD26" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE26" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF26" s="9">
         <v>0</v>
@@ -54873,16 +54686,16 @@
         <v>526</v>
       </c>
       <c r="O27" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q27" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R27" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S27" s="3">
         <v>1</v>
@@ -54915,13 +54728,13 @@
         <v>3174</v>
       </c>
       <c r="AC27" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD27" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE27" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF27" s="9">
         <v>0</v>
@@ -54983,16 +54796,16 @@
         <v>531</v>
       </c>
       <c r="O28" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q28" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R28" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S28" s="3">
         <v>1</v>
@@ -55071,16 +54884,16 @@
         <v>536</v>
       </c>
       <c r="O29" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q29" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R29" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S29" s="3">
         <v>1</v>
@@ -55104,22 +54917,22 @@
         <v>123</v>
       </c>
       <c r="Z29" s="3" t="s">
-        <v>3194</v>
+        <v>3185</v>
       </c>
       <c r="AA29" s="3" t="s">
         <v>3177</v>
       </c>
       <c r="AB29" s="3" t="s">
-        <v>3187</v>
+        <v>3182</v>
       </c>
       <c r="AC29" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD29" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE29" s="8" t="s">
-        <v>3234</v>
+        <v>3205</v>
       </c>
       <c r="AF29" s="9">
         <v>0</v>
@@ -55149,13 +54962,13 @@
         <v>1</v>
       </c>
       <c r="AO29" s="3" t="s">
-        <v>3243</v>
+        <v>3214</v>
       </c>
       <c r="AP29" s="3" t="s">
-        <v>3190</v>
+        <v>3184</v>
       </c>
       <c r="AQ29" s="3" t="s">
-        <v>3244</v>
+        <v>3215</v>
       </c>
       <c r="AR29" s="3"/>
     </row>
@@ -55203,16 +55016,16 @@
         <v>541</v>
       </c>
       <c r="O30" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q30" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R30" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S30" s="3">
         <v>1</v>
@@ -55242,16 +55055,16 @@
         <v>3177</v>
       </c>
       <c r="AB30" s="3" t="s">
-        <v>3187</v>
+        <v>3182</v>
       </c>
       <c r="AC30" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD30" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE30" s="8" t="s">
-        <v>3234</v>
+        <v>3205</v>
       </c>
       <c r="AF30" s="9">
         <v>0</v>
@@ -55281,13 +55094,13 @@
         <v>1</v>
       </c>
       <c r="AO30" s="3" t="s">
-        <v>3245</v>
+        <v>3216</v>
       </c>
       <c r="AP30" s="3" t="s">
-        <v>3190</v>
+        <v>3184</v>
       </c>
       <c r="AQ30" s="3" t="s">
-        <v>3246</v>
+        <v>3217</v>
       </c>
       <c r="AR30" s="3"/>
     </row>
@@ -55335,16 +55148,16 @@
         <v>546</v>
       </c>
       <c r="O31" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q31" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R31" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S31" s="3">
         <v>1</v>
@@ -55427,16 +55240,16 @@
         <v>551</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P32" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q32" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R32" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S32" s="3">
         <v>1</v>
@@ -55469,13 +55282,13 @@
         <v>3174</v>
       </c>
       <c r="AC32" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD32" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE32" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF32" s="9">
         <v>0</v>
@@ -55537,16 +55350,16 @@
         <v>556</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P33" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q33" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R33" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S33" s="3">
         <v>1</v>
@@ -55579,13 +55392,13 @@
         <v>3174</v>
       </c>
       <c r="AC33" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD33" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE33" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF33" s="9">
         <v>0</v>
@@ -55647,16 +55460,16 @@
         <v>561</v>
       </c>
       <c r="O34" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q34" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R34" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S34" s="3">
         <v>1</v>
@@ -55739,16 +55552,16 @@
         <v>566</v>
       </c>
       <c r="O35" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q35" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R35" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S35" s="3">
         <v>1</v>
@@ -55781,13 +55594,13 @@
         <v>3174</v>
       </c>
       <c r="AC35" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD35" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE35" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF35" s="9">
         <v>0</v>
@@ -55849,16 +55662,16 @@
         <v>571</v>
       </c>
       <c r="O36" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q36" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R36" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S36" s="3">
         <v>1</v>
@@ -55891,13 +55704,13 @@
         <v>3174</v>
       </c>
       <c r="AC36" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD36" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE36" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF36" s="9">
         <v>0</v>
@@ -55959,16 +55772,16 @@
         <v>576</v>
       </c>
       <c r="O37" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P37" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q37" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R37" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S37" s="3">
         <v>1</v>
@@ -56051,16 +55864,16 @@
         <v>581</v>
       </c>
       <c r="O38" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P38" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q38" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R38" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S38" s="3">
         <v>1</v>
@@ -56084,7 +55897,7 @@
         <v>214</v>
       </c>
       <c r="Z38" s="3" t="s">
-        <v>3203</v>
+        <v>3186</v>
       </c>
       <c r="AA38" s="3" t="s">
         <v>3177</v>
@@ -56093,13 +55906,13 @@
         <v>3174</v>
       </c>
       <c r="AC38" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD38" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE38" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF38" s="9">
         <v>0</v>
@@ -56111,10 +55924,10 @@
         <v>3180</v>
       </c>
       <c r="AI38" s="3" t="s">
-        <v>3204</v>
+        <v>3187</v>
       </c>
       <c r="AJ38" s="3" t="s">
-        <v>3205</v>
+        <v>3188</v>
       </c>
       <c r="AK38" s="3">
         <v>234234523</v>
@@ -56133,7 +55946,7 @@
         <v>3181</v>
       </c>
       <c r="AQ38" s="3" t="s">
-        <v>3247</v>
+        <v>3218</v>
       </c>
       <c r="AR38" s="3"/>
     </row>
@@ -56181,16 +55994,16 @@
         <v>586</v>
       </c>
       <c r="O39" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P39" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q39" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R39" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S39" s="3">
         <v>1</v>
@@ -56214,7 +56027,7 @@
         <v>214</v>
       </c>
       <c r="Z39" s="3" t="s">
-        <v>3203</v>
+        <v>3186</v>
       </c>
       <c r="AA39" s="3" t="s">
         <v>3177</v>
@@ -56223,13 +56036,13 @@
         <v>3174</v>
       </c>
       <c r="AC39" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD39" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE39" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF39" s="9">
         <v>0</v>
@@ -56241,10 +56054,10 @@
         <v>3180</v>
       </c>
       <c r="AI39" s="3" t="s">
-        <v>3204</v>
+        <v>3187</v>
       </c>
       <c r="AJ39" s="3" t="s">
-        <v>3205</v>
+        <v>3188</v>
       </c>
       <c r="AK39" s="3">
         <v>234234523</v>
@@ -56263,7 +56076,7 @@
         <v>3181</v>
       </c>
       <c r="AQ39" s="3" t="s">
-        <v>3248</v>
+        <v>3219</v>
       </c>
       <c r="AR39" s="3"/>
     </row>
@@ -56311,16 +56124,16 @@
         <v>591</v>
       </c>
       <c r="O40" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P40" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q40" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R40" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S40" s="3">
         <v>1</v>
@@ -56403,16 +56216,16 @@
         <v>596</v>
       </c>
       <c r="O41" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P41" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q41" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R41" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S41" s="3">
         <v>1</v>
@@ -56436,7 +56249,7 @@
         <v>214</v>
       </c>
       <c r="Z41" s="3" t="s">
-        <v>3203</v>
+        <v>3186</v>
       </c>
       <c r="AA41" s="3" t="s">
         <v>3177</v>
@@ -56445,13 +56258,13 @@
         <v>3174</v>
       </c>
       <c r="AC41" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD41" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE41" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF41" s="9">
         <v>0</v>
@@ -56463,10 +56276,10 @@
         <v>3180</v>
       </c>
       <c r="AI41" s="3" t="s">
-        <v>3204</v>
+        <v>3187</v>
       </c>
       <c r="AJ41" s="3" t="s">
-        <v>3205</v>
+        <v>3188</v>
       </c>
       <c r="AK41" s="3">
         <v>234234523</v>
@@ -56529,16 +56342,16 @@
         <v>601</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P42" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q42" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R42" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S42" s="3">
         <v>1</v>
@@ -56562,7 +56375,7 @@
         <v>214</v>
       </c>
       <c r="Z42" s="3" t="s">
-        <v>3203</v>
+        <v>3186</v>
       </c>
       <c r="AA42" s="3" t="s">
         <v>3177</v>
@@ -56571,13 +56384,13 @@
         <v>3174</v>
       </c>
       <c r="AC42" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD42" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE42" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF42" s="9">
         <v>0</v>
@@ -56589,10 +56402,10 @@
         <v>3180</v>
       </c>
       <c r="AI42" s="3" t="s">
-        <v>3204</v>
+        <v>3187</v>
       </c>
       <c r="AJ42" s="3" t="s">
-        <v>3205</v>
+        <v>3188</v>
       </c>
       <c r="AK42" s="3">
         <v>234234523</v>
@@ -56655,16 +56468,16 @@
         <v>606</v>
       </c>
       <c r="O43" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P43" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q43" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R43" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S43" s="3">
         <v>1</v>
@@ -56747,16 +56560,16 @@
         <v>611</v>
       </c>
       <c r="O44" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P44" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q44" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R44" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S44" s="3">
         <v>1</v>
@@ -56789,13 +56602,13 @@
         <v>3174</v>
       </c>
       <c r="AC44" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD44" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE44" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF44" s="9">
         <v>0</v>
@@ -56807,10 +56620,10 @@
         <v>3180</v>
       </c>
       <c r="AI44" s="3" t="s">
-        <v>3204</v>
+        <v>3187</v>
       </c>
       <c r="AJ44" s="3" t="s">
-        <v>3205</v>
+        <v>3188</v>
       </c>
       <c r="AK44" s="3">
         <v>234234523</v>
@@ -56873,16 +56686,16 @@
         <v>616</v>
       </c>
       <c r="O45" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P45" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q45" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R45" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S45" s="3">
         <v>1</v>
@@ -56915,13 +56728,13 @@
         <v>3174</v>
       </c>
       <c r="AC45" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD45" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE45" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF45" s="9">
         <v>0</v>
@@ -56933,10 +56746,10 @@
         <v>3180</v>
       </c>
       <c r="AI45" s="3" t="s">
-        <v>3204</v>
+        <v>3187</v>
       </c>
       <c r="AJ45" s="3" t="s">
-        <v>3205</v>
+        <v>3188</v>
       </c>
       <c r="AK45" s="3">
         <v>234234523</v>
@@ -56999,16 +56812,16 @@
         <v>621</v>
       </c>
       <c r="O46" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P46" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q46" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R46" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S46" s="3">
         <v>1</v>
@@ -57091,16 +56904,16 @@
         <v>626</v>
       </c>
       <c r="O47" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P47" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q47" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R47" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S47" s="3">
         <v>1</v>
@@ -57124,22 +56937,22 @@
         <v>214</v>
       </c>
       <c r="Z47" s="3" t="s">
-        <v>3203</v>
+        <v>3186</v>
       </c>
       <c r="AA47" s="3" t="s">
         <v>3177</v>
       </c>
       <c r="AB47" s="3" t="s">
-        <v>3187</v>
+        <v>3182</v>
       </c>
       <c r="AC47" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD47" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE47" s="8" t="s">
-        <v>3234</v>
+        <v>3205</v>
       </c>
       <c r="AF47" s="9">
         <v>0</v>
@@ -57151,10 +56964,10 @@
         <v>3180</v>
       </c>
       <c r="AI47" s="3" t="s">
-        <v>3204</v>
+        <v>3187</v>
       </c>
       <c r="AJ47" s="3" t="s">
-        <v>3205</v>
+        <v>3188</v>
       </c>
       <c r="AK47" s="3">
         <v>234234523</v>
@@ -57173,7 +56986,7 @@
         <v>3181</v>
       </c>
       <c r="AQ47" s="3" t="s">
-        <v>3249</v>
+        <v>3220</v>
       </c>
       <c r="AR47" s="3"/>
     </row>
@@ -57221,16 +57034,16 @@
         <v>631</v>
       </c>
       <c r="O48" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P48" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q48" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R48" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S48" s="3">
         <v>1</v>
@@ -57254,22 +57067,22 @@
         <v>214</v>
       </c>
       <c r="Z48" s="3" t="s">
-        <v>3203</v>
+        <v>3186</v>
       </c>
       <c r="AA48" s="3" t="s">
         <v>3177</v>
       </c>
       <c r="AB48" s="3" t="s">
-        <v>3187</v>
+        <v>3182</v>
       </c>
       <c r="AC48" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD48" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE48" s="8" t="s">
-        <v>3234</v>
+        <v>3205</v>
       </c>
       <c r="AF48" s="9">
         <v>0</v>
@@ -57281,10 +57094,10 @@
         <v>3180</v>
       </c>
       <c r="AI48" s="3" t="s">
-        <v>3204</v>
+        <v>3187</v>
       </c>
       <c r="AJ48" s="3" t="s">
-        <v>3205</v>
+        <v>3188</v>
       </c>
       <c r="AK48" s="3">
         <v>234234523</v>
@@ -57303,7 +57116,7 @@
         <v>3181</v>
       </c>
       <c r="AQ48" s="3" t="s">
-        <v>3250</v>
+        <v>3221</v>
       </c>
       <c r="AR48" s="3"/>
     </row>
@@ -57351,10 +57164,10 @@
         <v>636</v>
       </c>
       <c r="O49" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P49" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q49" s="3"/>
       <c r="R49" s="3"/>
@@ -57431,16 +57244,16 @@
         <v>641</v>
       </c>
       <c r="O50" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P50" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q50" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R50" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S50" s="3">
         <v>1</v>
@@ -57464,7 +57277,7 @@
         <v>214</v>
       </c>
       <c r="Z50" s="3" t="s">
-        <v>3203</v>
+        <v>3186</v>
       </c>
       <c r="AA50" s="3" t="s">
         <v>3177</v>
@@ -57473,13 +57286,13 @@
         <v>3174</v>
       </c>
       <c r="AC50" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD50" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE50" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF50" s="9">
         <v>0</v>
@@ -57491,10 +57304,10 @@
         <v>3180</v>
       </c>
       <c r="AI50" s="3" t="s">
-        <v>3204</v>
+        <v>3187</v>
       </c>
       <c r="AJ50" s="3" t="s">
-        <v>3205</v>
+        <v>3188</v>
       </c>
       <c r="AK50" s="3">
         <v>234234523</v>
@@ -57557,16 +57370,16 @@
         <v>646</v>
       </c>
       <c r="O51" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P51" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q51" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R51" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S51" s="3">
         <v>1</v>
@@ -57590,7 +57403,7 @@
         <v>214</v>
       </c>
       <c r="Z51" s="3" t="s">
-        <v>3203</v>
+        <v>3186</v>
       </c>
       <c r="AA51" s="3" t="s">
         <v>3177</v>
@@ -57599,13 +57412,13 @@
         <v>3174</v>
       </c>
       <c r="AC51" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD51" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE51" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF51" s="9">
         <v>0</v>
@@ -57617,10 +57430,10 @@
         <v>3180</v>
       </c>
       <c r="AI51" s="3" t="s">
-        <v>3204</v>
+        <v>3187</v>
       </c>
       <c r="AJ51" s="3" t="s">
-        <v>3205</v>
+        <v>3188</v>
       </c>
       <c r="AK51" s="3">
         <v>234234523</v>
@@ -57683,10 +57496,10 @@
         <v>651</v>
       </c>
       <c r="O52" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P52" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q52" s="3"/>
       <c r="R52" s="3"/>
@@ -57763,16 +57576,16 @@
         <v>656</v>
       </c>
       <c r="O53" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P53" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q53" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R53" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S53" s="3">
         <v>1</v>
@@ -57796,7 +57609,7 @@
         <v>214</v>
       </c>
       <c r="Z53" s="3" t="s">
-        <v>3203</v>
+        <v>3186</v>
       </c>
       <c r="AA53" s="3" t="s">
         <v>3177</v>
@@ -57805,13 +57618,13 @@
         <v>3174</v>
       </c>
       <c r="AC53" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD53" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE53" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF53" s="9">
         <v>0</v>
@@ -57823,10 +57636,10 @@
         <v>3180</v>
       </c>
       <c r="AI53" s="3" t="s">
-        <v>3204</v>
+        <v>3187</v>
       </c>
       <c r="AJ53" s="3" t="s">
-        <v>3205</v>
+        <v>3188</v>
       </c>
       <c r="AK53" s="3">
         <v>234234523</v>
@@ -57889,16 +57702,16 @@
         <v>661</v>
       </c>
       <c r="O54" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P54" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q54" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R54" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S54" s="3">
         <v>1</v>
@@ -57922,7 +57735,7 @@
         <v>214</v>
       </c>
       <c r="Z54" s="3" t="s">
-        <v>3203</v>
+        <v>3186</v>
       </c>
       <c r="AA54" s="3" t="s">
         <v>3177</v>
@@ -57931,13 +57744,13 @@
         <v>3174</v>
       </c>
       <c r="AC54" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD54" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE54" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF54" s="9">
         <v>0</v>
@@ -57949,10 +57762,10 @@
         <v>3180</v>
       </c>
       <c r="AI54" s="3" t="s">
-        <v>3204</v>
+        <v>3187</v>
       </c>
       <c r="AJ54" s="3" t="s">
-        <v>3205</v>
+        <v>3188</v>
       </c>
       <c r="AK54" s="3">
         <v>234234523</v>
@@ -58015,10 +57828,10 @@
         <v>666</v>
       </c>
       <c r="O55" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P55" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q55" s="3"/>
       <c r="R55" s="3"/>
@@ -58095,16 +57908,16 @@
         <v>671</v>
       </c>
       <c r="O56" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P56" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q56" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R56" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S56" s="3">
         <v>1</v>
@@ -58125,7 +57938,7 @@
         <v>3174</v>
       </c>
       <c r="Y56" s="3" t="s">
-        <v>3210</v>
+        <v>3189</v>
       </c>
       <c r="Z56" s="3" t="s">
         <v>3176</v>
@@ -58137,13 +57950,13 @@
         <v>3174</v>
       </c>
       <c r="AC56" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD56" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE56" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF56" s="9">
         <v>0</v>
@@ -58173,13 +57986,13 @@
         <v>1</v>
       </c>
       <c r="AO56" s="3" t="s">
-        <v>3251</v>
+        <v>3222</v>
       </c>
       <c r="AP56" s="3" t="s">
-        <v>3190</v>
+        <v>3184</v>
       </c>
       <c r="AQ56" s="3" t="s">
-        <v>3252</v>
+        <v>3223</v>
       </c>
       <c r="AR56" s="3"/>
     </row>
@@ -58227,16 +58040,16 @@
         <v>676</v>
       </c>
       <c r="O57" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P57" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q57" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R57" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S57" s="3">
         <v>1</v>
@@ -58257,7 +58070,7 @@
         <v>3174</v>
       </c>
       <c r="Y57" s="3" t="s">
-        <v>3210</v>
+        <v>3189</v>
       </c>
       <c r="Z57" s="3" t="s">
         <v>3176</v>
@@ -58269,13 +58082,13 @@
         <v>3174</v>
       </c>
       <c r="AC57" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD57" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE57" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF57" s="9">
         <v>0</v>
@@ -58305,13 +58118,13 @@
         <v>1</v>
       </c>
       <c r="AO57" s="3" t="s">
-        <v>3253</v>
+        <v>3224</v>
       </c>
       <c r="AP57" s="3" t="s">
-        <v>3190</v>
+        <v>3184</v>
       </c>
       <c r="AQ57" s="3" t="s">
-        <v>3254</v>
+        <v>3225</v>
       </c>
       <c r="AR57" s="3"/>
     </row>
@@ -58359,10 +58172,10 @@
         <v>681</v>
       </c>
       <c r="O58" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P58" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q58" s="3"/>
       <c r="R58" s="3"/>
@@ -58439,16 +58252,16 @@
         <v>686</v>
       </c>
       <c r="O59" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P59" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q59" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R59" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S59" s="3">
         <v>1</v>
@@ -58469,7 +58282,7 @@
         <v>3174</v>
       </c>
       <c r="Y59" s="3" t="s">
-        <v>3210</v>
+        <v>3189</v>
       </c>
       <c r="Z59" s="3" t="s">
         <v>3176</v>
@@ -58481,13 +58294,13 @@
         <v>3174</v>
       </c>
       <c r="AC59" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD59" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE59" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF59" s="9">
         <v>0</v>
@@ -58565,16 +58378,16 @@
         <v>691</v>
       </c>
       <c r="O60" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P60" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q60" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R60" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S60" s="3">
         <v>1</v>
@@ -58595,7 +58408,7 @@
         <v>3174</v>
       </c>
       <c r="Y60" s="3" t="s">
-        <v>3210</v>
+        <v>3189</v>
       </c>
       <c r="Z60" s="3" t="s">
         <v>3176</v>
@@ -58607,13 +58420,13 @@
         <v>3174</v>
       </c>
       <c r="AC60" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD60" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE60" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF60" s="9">
         <v>0</v>
@@ -58691,10 +58504,10 @@
         <v>696</v>
       </c>
       <c r="O61" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P61" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q61" s="3"/>
       <c r="R61" s="3"/>
@@ -58771,16 +58584,16 @@
         <v>701</v>
       </c>
       <c r="O62" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P62" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q62" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R62" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S62" s="3">
         <v>1</v>
@@ -58801,7 +58614,7 @@
         <v>3174</v>
       </c>
       <c r="Y62" s="3" t="s">
-        <v>3210</v>
+        <v>3189</v>
       </c>
       <c r="Z62" s="3" t="s">
         <v>3176</v>
@@ -58813,13 +58626,13 @@
         <v>3174</v>
       </c>
       <c r="AC62" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD62" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE62" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF62" s="9">
         <v>0</v>
@@ -58897,16 +58710,16 @@
         <v>706</v>
       </c>
       <c r="O63" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P63" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q63" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R63" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S63" s="3">
         <v>1</v>
@@ -58927,7 +58740,7 @@
         <v>3174</v>
       </c>
       <c r="Y63" s="3" t="s">
-        <v>3210</v>
+        <v>3189</v>
       </c>
       <c r="Z63" s="3" t="s">
         <v>3176</v>
@@ -58939,13 +58752,13 @@
         <v>3174</v>
       </c>
       <c r="AC63" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD63" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE63" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AF63" s="9">
         <v>0</v>
@@ -59023,10 +58836,10 @@
         <v>711</v>
       </c>
       <c r="O64" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P64" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q64" s="3"/>
       <c r="R64" s="3"/>
@@ -59103,16 +58916,16 @@
         <v>716</v>
       </c>
       <c r="O65" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P65" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q65" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R65" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S65" s="3">
         <v>1</v>
@@ -59133,7 +58946,7 @@
         <v>3174</v>
       </c>
       <c r="Y65" s="3" t="s">
-        <v>3210</v>
+        <v>3189</v>
       </c>
       <c r="Z65" s="3" t="s">
         <v>3176</v>
@@ -59142,16 +58955,16 @@
         <v>3177</v>
       </c>
       <c r="AB65" s="3" t="s">
-        <v>3187</v>
+        <v>3182</v>
       </c>
       <c r="AC65" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD65" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE65" s="8" t="s">
-        <v>3234</v>
+        <v>3205</v>
       </c>
       <c r="AF65" s="9">
         <v>0</v>
@@ -59181,13 +58994,13 @@
         <v>1</v>
       </c>
       <c r="AO65" s="3" t="s">
-        <v>3255</v>
+        <v>3226</v>
       </c>
       <c r="AP65" s="3" t="s">
-        <v>3190</v>
+        <v>3184</v>
       </c>
       <c r="AQ65" s="3" t="s">
-        <v>3256</v>
+        <v>3227</v>
       </c>
       <c r="AR65" s="3"/>
     </row>
@@ -59235,16 +59048,16 @@
         <v>721</v>
       </c>
       <c r="O66" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P66" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q66" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R66" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S66" s="3">
         <v>1</v>
@@ -59265,7 +59078,7 @@
         <v>3174</v>
       </c>
       <c r="Y66" s="3" t="s">
-        <v>3210</v>
+        <v>3189</v>
       </c>
       <c r="Z66" s="3" t="s">
         <v>3176</v>
@@ -59274,16 +59087,16 @@
         <v>3177</v>
       </c>
       <c r="AB66" s="3" t="s">
-        <v>3187</v>
+        <v>3182</v>
       </c>
       <c r="AC66" s="3" t="s">
-        <v>3229</v>
+        <v>3200</v>
       </c>
       <c r="AD66" s="7" t="s">
         <v>3178</v>
       </c>
       <c r="AE66" s="8" t="s">
-        <v>3234</v>
+        <v>3205</v>
       </c>
       <c r="AF66" s="9">
         <v>0</v>
@@ -59313,13 +59126,13 @@
         <v>1</v>
       </c>
       <c r="AO66" s="3" t="s">
-        <v>3257</v>
+        <v>3228</v>
       </c>
       <c r="AP66" s="3" t="s">
-        <v>3190</v>
+        <v>3184</v>
       </c>
       <c r="AQ66" s="3" t="s">
-        <v>3258</v>
+        <v>3229</v>
       </c>
       <c r="AR66" s="3"/>
     </row>
@@ -59367,7 +59180,7 @@
         <v>726</v>
       </c>
       <c r="O67" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P67" s="3"/>
       <c r="Q67" s="3"/>
@@ -59445,16 +59258,16 @@
         <v>731</v>
       </c>
       <c r="O68" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P68" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q68" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R68" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S68" s="3">
         <v>1</v>
@@ -59539,16 +59352,16 @@
         <v>736</v>
       </c>
       <c r="O69" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P69" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q69" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R69" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S69" s="3">
         <v>1</v>
@@ -59633,7 +59446,7 @@
         <v>741</v>
       </c>
       <c r="O70" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P70" s="3"/>
       <c r="Q70" s="3"/>
@@ -59711,16 +59524,16 @@
         <v>746</v>
       </c>
       <c r="O71" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P71" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q71" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R71" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S71" s="3">
         <v>1</v>
@@ -59805,16 +59618,16 @@
         <v>751</v>
       </c>
       <c r="O72" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P72" s="3" t="s">
-        <v>3227</v>
+        <v>3198</v>
       </c>
       <c r="Q72" s="3" t="s">
         <v>3172</v>
       </c>
       <c r="R72" s="3" t="s">
-        <v>3228</v>
+        <v>3199</v>
       </c>
       <c r="S72" s="3">
         <v>1</v>
@@ -59899,7 +59712,7 @@
         <v>756</v>
       </c>
       <c r="O73" s="3" t="s">
-        <v>3226</v>
+        <v>3197</v>
       </c>
       <c r="P73" s="3"/>
       <c r="Q73" s="3"/>

</xml_diff>

<commit_message>
fix: update variable names for order IDs in CreateOrderDBTests to match Excel sheet references
</commit_message>
<xml_diff>
--- a/data/BigCommerceData/BigC_Ecomm_TestCases_AutomationMasterSheet.xlsx
+++ b/data/BigCommerceData/BigC_Ecomm_TestCases_AutomationMasterSheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DED119-D703-4A7C-B92C-78E9748C8A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92947A8-AF99-4D73-B9C0-213CF866C5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9595,25 +9595,25 @@
     <t>Standard product order for existing customer</t>
   </si>
   <si>
+    <t>2025-09-29T10:00:44.194Z</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>["=== Test Failure Details ===","Failed Step: Proceed to Payment","Error Message: locator.selectOption: Target page, context or browser has been closed\nCall log:\n\u001b[2m  - waiting for locator('#content-iframe').contentFrame().locator('//div[@class=\\'payment-form\\']//select[@id=\\'paymentMethod\\']')\u001b[22m\n\u001b[2m    - locator resolved to &lt;select id=\"paymentMethod\" name=\"paymentMethod\"&gt;…&lt;/select&gt;\u001b[22m\n\u001b[2m  - attempting select option action\u001b[22m\n\u001b[2m    2 × waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m    - waiting 20ms\u001b[22m\n\u001b[2m    2 × waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 100ms\u001b[22m\n\u001b[2m    254 × waiting for element to be visible and enabled\u001b[22m\n\u001b[2m        - did not find some options\u001b[22m\n\u001b[2m      - retrying select option action\u001b[22m\n\u001b[2m        - waiting 500ms\u001b[22m\n\u001b[2m  2 × element was detached from the DOM, retrying\u001b[22m\n\u001b[2m      - locator resolved to &lt;select id=\"paymentMethod\" name=\"paymentMethod\"&gt;…&lt;/select&gt;\u001b[22m\n\u001b[2m    - attempting select option action\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 20ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 100ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 100ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m    2 × waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u</t>
+  </si>
+  <si>
+    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: Invalid object name 'KiboOrder'.","Failure Timestamp: 2025-09-29T10:00:44.050Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-29T10:00:44.194Z","---"]</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-09-27T21:28:57.060Z\nScreenshot: N/A","Status: Passed","Last Updated: 2025-09-27T21:28:57.142Z","---"]</t>
+  </si>
+  <si>
     <t>357028</t>
-  </si>
-  <si>
-    <t>2025-09-29T08:35:01.245Z</t>
-  </si>
-  <si>
-    <t>Failed</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Proceed to Payment","Error Message: locator.selectOption: Target page, context or browser has been closed\nCall log:\n\u001b[2m  - waiting for locator('#content-iframe').contentFrame().locator('//div[@class=\\'payment-form\\']//select[@id=\\'paymentMethod\\']')\u001b[22m\n\u001b[2m    - locator resolved to &lt;select id=\"paymentMethod\" name=\"paymentMethod\"&gt;…&lt;/select&gt;\u001b[22m\n\u001b[2m  - attempting select option action\u001b[22m\n\u001b[2m    2 × waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m    - waiting 20ms\u001b[22m\n\u001b[2m    2 × waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 100ms\u001b[22m\n\u001b[2m    254 × waiting for element to be visible and enabled\u001b[22m\n\u001b[2m        - did not find some options\u001b[22m\n\u001b[2m      - retrying select option action\u001b[22m\n\u001b[2m        - waiting 500ms\u001b[22m\n\u001b[2m  2 × element was detached from the DOM, retrying\u001b[22m\n\u001b[2m      - locator resolved to &lt;select id=\"paymentMethod\" name=\"paymentMethod\"&gt;…&lt;/select&gt;\u001b[22m\n\u001b[2m    - attempting select option action\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 20ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 100ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 100ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m    2 × waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u001b[22m\n\u001b[2m      - waiting for element to be visible and enabled\u001b[22m\n\u001b[2m      - did not find some options\u001b[22m\n\u001b[2m    - retrying select option action\u001b[22m\n\u001b[2m      - waiting 500ms\u</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: \u001b[2mexpect(\u001b[22m\u001b[31mreceived\u001b[39m\u001b[2m).\u001b[22mtoBe\u001b[2m(\u001b[22m\u001b[32mexpected\u001b[39m\u001b[2m) // Object.is equality\u001b[22m\n\nExpected: \u001b[32m\"357028\"\u001b[39m\nReceived: \u001b[31m357566\u001b[39m","Failure Timestamp: 2025-09-29T08:35:01.138Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-29T08:35:01.245Z","---"]</t>
-  </si>
-  <si>
-    <t>Passed</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-27T21:28:57.060Z\nScreenshot: N/A","Status: Passed","Last Updated: 2025-09-27T21:28:57.142Z","---"]</t>
   </si>
   <si>
     <t>USD $20.00</t>
@@ -47352,8 +47352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AV73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="AR2" sqref="AR2"/>
+    <sheetView tabSelected="1" topLeftCell="AO1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="AR11" sqref="AR11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -47399,10 +47399,10 @@
     <col min="40" max="40" width="13.77734375" style="3" customWidth="1"/>
     <col min="41" max="41" width="27" style="3" customWidth="1"/>
     <col min="42" max="42" width="21.88671875" customWidth="1"/>
-    <col min="43" max="43" width="26.33203125" style="3" customWidth="1"/>
-    <col min="44" max="44" width="31.5546875" style="3" customWidth="1"/>
-    <col min="45" max="45" width="39.77734375" style="3" customWidth="1"/>
-    <col min="46" max="46" width="60.109375" style="3" customWidth="1"/>
+    <col min="43" max="43" width="19.88671875" style="3" customWidth="1"/>
+    <col min="44" max="44" width="63.88671875" style="3" customWidth="1"/>
+    <col min="45" max="45" width="18.6640625" style="3" customWidth="1"/>
+    <col min="46" max="46" width="69.77734375" style="3" customWidth="1"/>
     <col min="47" max="47" width="27.88671875" style="3" customWidth="1"/>
     <col min="48" max="48" width="26.109375" style="3" customWidth="1"/>
     <col min="49" max="51" width="18.33203125" style="3" customWidth="1"/>
@@ -47410,7 +47410,7 @@
     <col min="53" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" s="4" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:48" s="4" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -47675,25 +47675,25 @@
         <v>358102</v>
       </c>
       <c r="AP2" t="s">
+        <v>3189</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
         <v>3190</v>
       </c>
-      <c r="AQ2" s="3" t="s">
+      <c r="AR2" s="3" t="s">
         <v>3191</v>
       </c>
-      <c r="AR2" s="3" t="s">
+      <c r="AS2" s="3" t="s">
+        <v>3190</v>
+      </c>
+      <c r="AT2" s="3" t="s">
         <v>3192</v>
       </c>
-      <c r="AS2" s="3" t="s">
-        <v>3191</v>
-      </c>
-      <c r="AT2" s="3" t="s">
+      <c r="AU2" s="3" t="s">
         <v>3193</v>
       </c>
-      <c r="AU2" s="3" t="s">
+      <c r="AV2" s="3" t="s">
         <v>3194</v>
-      </c>
-      <c r="AV2" s="3" t="s">
-        <v>3195</v>
       </c>
     </row>
     <row r="3" spans="1:48" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -47809,7 +47809,7 @@
         <v>1</v>
       </c>
       <c r="AM3" s="3" t="s">
-        <v>3189</v>
+        <v>3195</v>
       </c>
     </row>
     <row r="4" spans="1:48" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -48260,7 +48260,7 @@
         <v>3199</v>
       </c>
       <c r="AQ11" s="3" t="s">
-        <v>3194</v>
+        <v>3193</v>
       </c>
       <c r="AR11" s="3" t="s">
         <v>3200</v>
@@ -49450,7 +49450,7 @@
         <v>3202</v>
       </c>
       <c r="AS30" s="3" t="s">
-        <v>3191</v>
+        <v>3190</v>
       </c>
       <c r="AT30" s="3" t="s">
         <v>3203</v>
@@ -49880,7 +49880,7 @@
         <v>3207</v>
       </c>
       <c r="AQ38" s="3" t="s">
-        <v>3191</v>
+        <v>3190</v>
       </c>
       <c r="AR38" s="3" t="s">
         <v>3208</v>
@@ -50423,13 +50423,13 @@
         <v>3209</v>
       </c>
       <c r="AQ47" s="3" t="s">
-        <v>3191</v>
+        <v>3190</v>
       </c>
       <c r="AR47" s="3" t="s">
         <v>3210</v>
       </c>
       <c r="AS47" s="3" t="s">
-        <v>3191</v>
+        <v>3190</v>
       </c>
       <c r="AT47" s="3" t="s">
         <v>3211</v>
@@ -50975,7 +50975,7 @@
         <v>3214</v>
       </c>
       <c r="AQ56" s="3" t="s">
-        <v>3194</v>
+        <v>3193</v>
       </c>
       <c r="AR56" s="3" t="s">
         <v>3215</v>
@@ -51521,7 +51521,7 @@
         <v>3217</v>
       </c>
       <c r="AQ65" s="3" t="s">
-        <v>3194</v>
+        <v>3193</v>
       </c>
       <c r="AR65" s="3" t="s">
         <v>3218</v>
@@ -51643,7 +51643,7 @@
         <v>3219</v>
       </c>
       <c r="AS66" s="3" t="s">
-        <v>3191</v>
+        <v>3190</v>
       </c>
       <c r="AT66" s="3" t="s">
         <v>3220</v>
@@ -51960,7 +51960,7 @@
   </sheetData>
   <autoFilter ref="A1:AO73" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
@@ -52274,7 +52274,7 @@
         <v>3233</v>
       </c>
       <c r="AP2" s="3" t="s">
-        <v>3194</v>
+        <v>3193</v>
       </c>
       <c r="AQ2" s="3" t="s">
         <v>3234</v>
@@ -52406,7 +52406,7 @@
         <v>3235</v>
       </c>
       <c r="AP3" s="3" t="s">
-        <v>3194</v>
+        <v>3193</v>
       </c>
       <c r="AQ3" s="3" t="s">
         <v>3236</v>
@@ -53236,7 +53236,7 @@
         <v>3238</v>
       </c>
       <c r="AP11" s="3" t="s">
-        <v>3194</v>
+        <v>3193</v>
       </c>
       <c r="AQ11" s="3" t="s">
         <v>3239</v>
@@ -53368,7 +53368,7 @@
         <v>3240</v>
       </c>
       <c r="AP12" s="3" t="s">
-        <v>3194</v>
+        <v>3193</v>
       </c>
       <c r="AQ12" s="3" t="s">
         <v>3241</v>
@@ -54200,7 +54200,7 @@
         <v>3242</v>
       </c>
       <c r="AP20" s="3" t="s">
-        <v>3194</v>
+        <v>3193</v>
       </c>
       <c r="AQ20" s="3" t="s">
         <v>3243</v>
@@ -54332,7 +54332,7 @@
         <v>3244</v>
       </c>
       <c r="AP21" s="3" t="s">
-        <v>3194</v>
+        <v>3193</v>
       </c>
       <c r="AQ21" s="3" t="s">
         <v>3245</v>
@@ -55164,7 +55164,7 @@
         <v>3246</v>
       </c>
       <c r="AP29" s="3" t="s">
-        <v>3194</v>
+        <v>3193</v>
       </c>
       <c r="AQ29" s="3" t="s">
         <v>3247</v>
@@ -55296,7 +55296,7 @@
         <v>3248</v>
       </c>
       <c r="AP30" s="3" t="s">
-        <v>3194</v>
+        <v>3193</v>
       </c>
       <c r="AQ30" s="3" t="s">
         <v>3249</v>
@@ -56142,7 +56142,7 @@
       </c>
       <c r="AO38" s="3"/>
       <c r="AP38" s="3" t="s">
-        <v>3191</v>
+        <v>3190</v>
       </c>
       <c r="AQ38" s="3" t="s">
         <v>3250</v>
@@ -56272,7 +56272,7 @@
       </c>
       <c r="AO39" s="3"/>
       <c r="AP39" s="3" t="s">
-        <v>3191</v>
+        <v>3190</v>
       </c>
       <c r="AQ39" s="3" t="s">
         <v>3251</v>
@@ -57182,7 +57182,7 @@
       </c>
       <c r="AO47" s="3"/>
       <c r="AP47" s="3" t="s">
-        <v>3191</v>
+        <v>3190</v>
       </c>
       <c r="AQ47" s="3" t="s">
         <v>3252</v>
@@ -57312,7 +57312,7 @@
       </c>
       <c r="AO48" s="3"/>
       <c r="AP48" s="3" t="s">
-        <v>3191</v>
+        <v>3190</v>
       </c>
       <c r="AQ48" s="3" t="s">
         <v>3253</v>
@@ -58188,7 +58188,7 @@
         <v>3254</v>
       </c>
       <c r="AP56" s="3" t="s">
-        <v>3191</v>
+        <v>3190</v>
       </c>
       <c r="AQ56" s="3" t="s">
         <v>3255</v>
@@ -58320,7 +58320,7 @@
         <v>3256</v>
       </c>
       <c r="AP57" s="3" t="s">
-        <v>3194</v>
+        <v>3193</v>
       </c>
       <c r="AQ57" s="3" t="s">
         <v>3257</v>
@@ -59196,7 +59196,7 @@
         <v>3258</v>
       </c>
       <c r="AP65" s="3" t="s">
-        <v>3194</v>
+        <v>3193</v>
       </c>
       <c r="AQ65" s="3" t="s">
         <v>3259</v>
@@ -59328,7 +59328,7 @@
         <v>3260</v>
       </c>
       <c r="AP66" s="3" t="s">
-        <v>3191</v>
+        <v>3190</v>
       </c>
       <c r="AQ66" s="3" t="s">
         <v>3261</v>

</xml_diff>

<commit_message>
fix: add validation and logging for test execution scenarios in CreateOrderDBTests
</commit_message>
<xml_diff>
--- a/data/BigCommerceData/BigC_Ecomm_TestCases_AutomationMasterSheet.xlsx
+++ b/data/BigCommerceData/BigC_Ecomm_TestCases_AutomationMasterSheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A227E67-EE2A-4412-97B3-DB2DD82282CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510AC19C-B87F-4BA8-9C2B-6D1CE2E49AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20373" uniqueCount="3286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20372" uniqueCount="3285">
   <si>
     <t>Global Test Case ID</t>
   </si>
@@ -9639,9 +9639,6 @@
   </si>
   <si>
     <t>USD $132.15</t>
-  </si>
-  <si>
-    <t>357036</t>
   </si>
   <si>
     <t>2025-09-30T09:34:37.828Z</t>
@@ -47423,10 +47420,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AW73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="AN12" sqref="AN12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -47912,7 +47910,7 @@
         <v>3201</v>
       </c>
     </row>
-    <row r="4" spans="1:49" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:49" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>35</v>
       </c>
@@ -47962,7 +47960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:49" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:49" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>42</v>
       </c>
@@ -48012,7 +48010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:49" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:49" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>48</v>
       </c>
@@ -48062,7 +48060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:49" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:49" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>53</v>
       </c>
@@ -48112,7 +48110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:49" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:49" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>58</v>
       </c>
@@ -48162,7 +48160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:49" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:49" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>64</v>
       </c>
@@ -48212,7 +48210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:49" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:49" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>69</v>
       </c>
@@ -48377,23 +48375,26 @@
       <c r="AL11" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="AM11" s="3" t="s">
+      <c r="AM11" s="3">
+        <v>434397</v>
+      </c>
+      <c r="AN11" s="3">
+        <v>434398</v>
+      </c>
+      <c r="AQ11" t="s">
         <v>3204</v>
-      </c>
-      <c r="AQ11" t="s">
-        <v>3205</v>
       </c>
       <c r="AR11" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AS11" s="3" t="s">
-        <v>3206</v>
+        <v>3205</v>
       </c>
       <c r="AT11" s="3" t="s">
         <v>3194</v>
       </c>
       <c r="AU11" s="3" t="s">
-        <v>3207</v>
+        <v>3206</v>
       </c>
     </row>
     <row r="12" spans="1:49" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -48512,19 +48513,19 @@
         <v>0</v>
       </c>
       <c r="AM12" s="3" t="s">
+        <v>3207</v>
+      </c>
+      <c r="AQ12" t="s">
         <v>3208</v>
-      </c>
-      <c r="AQ12" t="s">
-        <v>3209</v>
       </c>
       <c r="AR12" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AS12" s="3" t="s">
-        <v>3210</v>
-      </c>
-    </row>
-    <row r="13" spans="1:49" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3209</v>
+      </c>
+    </row>
+    <row r="13" spans="1:49" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>85</v>
       </c>
@@ -48571,7 +48572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:49" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:49" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>90</v>
       </c>
@@ -48618,7 +48619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:49" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:49" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>95</v>
       </c>
@@ -48665,7 +48666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:49" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:49" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>100</v>
       </c>
@@ -48712,7 +48713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>105</v>
       </c>
@@ -48759,7 +48760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>110</v>
       </c>
@@ -48806,7 +48807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>115</v>
       </c>
@@ -48921,7 +48922,7 @@
         <v>123</v>
       </c>
       <c r="W20" s="3" t="s">
-        <v>3211</v>
+        <v>3210</v>
       </c>
       <c r="X20" s="3" t="s">
         <v>3186</v>
@@ -48969,13 +48970,13 @@
         <v>0</v>
       </c>
       <c r="AQ20" t="s">
-        <v>3212</v>
+        <v>3211</v>
       </c>
       <c r="AT20" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AU20" s="3" t="s">
-        <v>3213</v>
+        <v>3212</v>
       </c>
     </row>
     <row r="21" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -49094,7 +49095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>131</v>
       </c>
@@ -49141,7 +49142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>136</v>
       </c>
@@ -49188,7 +49189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>141</v>
       </c>
@@ -49235,7 +49236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>146</v>
       </c>
@@ -49282,7 +49283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>151</v>
       </c>
@@ -49329,7 +49330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>156</v>
       </c>
@@ -49376,7 +49377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>161</v>
       </c>
@@ -49491,7 +49492,7 @@
         <v>123</v>
       </c>
       <c r="W29" s="3" t="s">
-        <v>3211</v>
+        <v>3210</v>
       </c>
       <c r="X29" s="3" t="s">
         <v>3186</v>
@@ -49539,13 +49540,13 @@
         <v>0</v>
       </c>
       <c r="AQ29" t="s">
-        <v>3214</v>
+        <v>3213</v>
       </c>
       <c r="AT29" s="3" t="s">
         <v>3194</v>
       </c>
       <c r="AU29" s="3" t="s">
-        <v>3215</v>
+        <v>3214</v>
       </c>
     </row>
     <row r="30" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -49664,16 +49665,16 @@
         <v>0</v>
       </c>
       <c r="AQ30" t="s">
-        <v>3216</v>
+        <v>3215</v>
       </c>
       <c r="AT30" s="3" t="s">
         <v>3194</v>
       </c>
       <c r="AU30" s="3" t="s">
-        <v>3217</v>
-      </c>
-    </row>
-    <row r="31" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3216</v>
+      </c>
+    </row>
+    <row r="31" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>176</v>
       </c>
@@ -49720,7 +49721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>181</v>
       </c>
@@ -49767,7 +49768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>186</v>
       </c>
@@ -49814,7 +49815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>191</v>
       </c>
@@ -49861,7 +49862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>196</v>
       </c>
@@ -49908,7 +49909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>201</v>
       </c>
@@ -49955,7 +49956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>206</v>
       </c>
@@ -50070,7 +50071,7 @@
         <v>214</v>
       </c>
       <c r="W38" s="3" t="s">
-        <v>3218</v>
+        <v>3217</v>
       </c>
       <c r="X38" s="3" t="s">
         <v>3186</v>
@@ -50097,10 +50098,10 @@
         <v>3189</v>
       </c>
       <c r="AF38" s="3" t="s">
+        <v>3218</v>
+      </c>
+      <c r="AG38" s="3" t="s">
         <v>3219</v>
-      </c>
-      <c r="AG38" s="3" t="s">
-        <v>3220</v>
       </c>
       <c r="AH38" s="3">
         <v>234234523</v>
@@ -50118,19 +50119,19 @@
         <v>0</v>
       </c>
       <c r="AQ38" t="s">
-        <v>3221</v>
+        <v>3220</v>
       </c>
       <c r="AR38" s="3" t="s">
         <v>3194</v>
       </c>
       <c r="AS38" s="3" t="s">
-        <v>3222</v>
+        <v>3221</v>
       </c>
       <c r="AT38" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AU38" s="3" t="s">
-        <v>3223</v>
+        <v>3222</v>
       </c>
     </row>
     <row r="39" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -50228,10 +50229,10 @@
         <v>3189</v>
       </c>
       <c r="AF39" s="3" t="s">
+        <v>3218</v>
+      </c>
+      <c r="AG39" s="3" t="s">
         <v>3219</v>
-      </c>
-      <c r="AG39" s="3" t="s">
-        <v>3220</v>
       </c>
       <c r="AH39" s="3">
         <v>234234523</v>
@@ -50249,16 +50250,16 @@
         <v>0</v>
       </c>
       <c r="AQ39" t="s">
-        <v>3224</v>
+        <v>3223</v>
       </c>
       <c r="AR39" s="3" t="s">
         <v>3194</v>
       </c>
       <c r="AS39" s="3" t="s">
-        <v>3225</v>
-      </c>
-    </row>
-    <row r="40" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3224</v>
+      </c>
+    </row>
+    <row r="40" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>222</v>
       </c>
@@ -50305,7 +50306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>227</v>
       </c>
@@ -50352,7 +50353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>232</v>
       </c>
@@ -50399,7 +50400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>237</v>
       </c>
@@ -50446,7 +50447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>242</v>
       </c>
@@ -50493,7 +50494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>247</v>
       </c>
@@ -50540,7 +50541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>252</v>
       </c>
@@ -50655,7 +50656,7 @@
         <v>214</v>
       </c>
       <c r="W47" s="3" t="s">
-        <v>3218</v>
+        <v>3217</v>
       </c>
       <c r="X47" s="3" t="s">
         <v>3186</v>
@@ -50682,10 +50683,10 @@
         <v>3189</v>
       </c>
       <c r="AF47" s="3" t="s">
+        <v>3218</v>
+      </c>
+      <c r="AG47" s="3" t="s">
         <v>3219</v>
-      </c>
-      <c r="AG47" s="3" t="s">
-        <v>3220</v>
       </c>
       <c r="AH47" s="3">
         <v>234234523</v>
@@ -50703,19 +50704,19 @@
         <v>0</v>
       </c>
       <c r="AQ47" t="s">
-        <v>3226</v>
+        <v>3225</v>
       </c>
       <c r="AR47" s="3" t="s">
         <v>3194</v>
       </c>
       <c r="AS47" s="3" t="s">
-        <v>3227</v>
+        <v>3226</v>
       </c>
       <c r="AT47" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AU47" s="3" t="s">
-        <v>3228</v>
+        <v>3227</v>
       </c>
     </row>
     <row r="48" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -50813,10 +50814,10 @@
         <v>3189</v>
       </c>
       <c r="AF48" s="3" t="s">
+        <v>3218</v>
+      </c>
+      <c r="AG48" s="3" t="s">
         <v>3219</v>
-      </c>
-      <c r="AG48" s="3" t="s">
-        <v>3220</v>
       </c>
       <c r="AH48" s="3">
         <v>234234523</v>
@@ -50834,7 +50835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>267</v>
       </c>
@@ -50881,7 +50882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>272</v>
       </c>
@@ -50928,7 +50929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>277</v>
       </c>
@@ -50975,7 +50976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>282</v>
       </c>
@@ -51022,7 +51023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>287</v>
       </c>
@@ -51069,7 +51070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>292</v>
       </c>
@@ -51116,7 +51117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>297</v>
       </c>
@@ -51228,7 +51229,7 @@
         <v>3182</v>
       </c>
       <c r="V56" s="3" t="s">
-        <v>3229</v>
+        <v>3228</v>
       </c>
       <c r="W56" s="3" t="s">
         <v>3185</v>
@@ -51279,22 +51280,22 @@
         <v>0</v>
       </c>
       <c r="AM56" s="3" t="s">
+        <v>3229</v>
+      </c>
+      <c r="AQ56" t="s">
         <v>3230</v>
-      </c>
-      <c r="AQ56" t="s">
-        <v>3231</v>
       </c>
       <c r="AR56" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AS56" s="3" t="s">
-        <v>3232</v>
+        <v>3231</v>
       </c>
       <c r="AT56" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AU56" s="3" t="s">
-        <v>3233</v>
+        <v>3232</v>
       </c>
     </row>
     <row r="57" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -51362,7 +51363,7 @@
         <v>3182</v>
       </c>
       <c r="V57" s="3" t="s">
-        <v>3229</v>
+        <v>3228</v>
       </c>
       <c r="W57" s="3" t="s">
         <v>3185</v>
@@ -51413,19 +51414,19 @@
         <v>0</v>
       </c>
       <c r="AM57" s="3" t="s">
+        <v>3233</v>
+      </c>
+      <c r="AQ57" t="s">
         <v>3234</v>
-      </c>
-      <c r="AQ57" t="s">
-        <v>3235</v>
       </c>
       <c r="AR57" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AS57" s="3" t="s">
-        <v>3236</v>
-      </c>
-    </row>
-    <row r="58" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3235</v>
+      </c>
+    </row>
+    <row r="58" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>313</v>
       </c>
@@ -51472,7 +51473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>318</v>
       </c>
@@ -51519,7 +51520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>323</v>
       </c>
@@ -51566,7 +51567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>328</v>
       </c>
@@ -51613,7 +51614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>333</v>
       </c>
@@ -51660,7 +51661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>338</v>
       </c>
@@ -51707,7 +51708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>343</v>
       </c>
@@ -51819,7 +51820,7 @@
         <v>3182</v>
       </c>
       <c r="V65" s="3" t="s">
-        <v>3229</v>
+        <v>3228</v>
       </c>
       <c r="W65" s="3" t="s">
         <v>3185</v>
@@ -51870,22 +51871,22 @@
         <v>0</v>
       </c>
       <c r="AM65" s="3" t="s">
+        <v>3236</v>
+      </c>
+      <c r="AQ65" t="s">
         <v>3237</v>
-      </c>
-      <c r="AQ65" t="s">
-        <v>3238</v>
       </c>
       <c r="AR65" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AS65" s="3" t="s">
-        <v>3239</v>
+        <v>3238</v>
       </c>
       <c r="AT65" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AU65" s="3" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="66" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -51953,7 +51954,7 @@
         <v>3182</v>
       </c>
       <c r="V66" s="3" t="s">
-        <v>3229</v>
+        <v>3228</v>
       </c>
       <c r="W66" s="3" t="s">
         <v>3185</v>
@@ -52004,25 +52005,25 @@
         <v>0</v>
       </c>
       <c r="AM66" s="3" t="s">
+        <v>3240</v>
+      </c>
+      <c r="AQ66" t="s">
         <v>3241</v>
-      </c>
-      <c r="AQ66" t="s">
-        <v>3242</v>
       </c>
       <c r="AR66" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AS66" s="3" t="s">
-        <v>3243</v>
+        <v>3242</v>
       </c>
       <c r="AT66" s="3" t="s">
         <v>3194</v>
       </c>
       <c r="AU66" s="3" t="s">
-        <v>3244</v>
-      </c>
-    </row>
-    <row r="67" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3243</v>
+      </c>
+    </row>
+    <row r="67" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>358</v>
       </c>
@@ -52066,7 +52067,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="68" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>363</v>
       </c>
@@ -52110,7 +52111,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="69" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>368</v>
       </c>
@@ -52154,7 +52155,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="70" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>373</v>
       </c>
@@ -52198,7 +52199,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="71" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>378</v>
       </c>
@@ -52242,7 +52243,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="72" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>383</v>
       </c>
@@ -52286,7 +52287,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="73" spans="1:47" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:47" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>388</v>
       </c>
@@ -52331,7 +52332,19 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AP73" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <autoFilter ref="A1:AP73" xr:uid="{00000000-0009-0000-0000-000002000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Order with Standard product - Fulfillment using Billing Address"/>
+        <filter val="Order with Standard product - Fulfillment using New Single Address"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="8">
+      <filters>
+        <filter val="No Coupon"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
@@ -52434,25 +52447,25 @@
         <v>13</v>
       </c>
       <c r="O1" s="4" t="s">
+        <v>3244</v>
+      </c>
+      <c r="P1" s="4" t="s">
         <v>3245</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>3246</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>3247</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>3248</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>3249</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>3250</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>3251</v>
       </c>
       <c r="V1" s="4" t="s">
         <v>3149</v>
@@ -52512,7 +52525,7 @@
         <v>3167</v>
       </c>
       <c r="AO1" s="4" t="s">
-        <v>3252</v>
+        <v>3251</v>
       </c>
       <c r="AP1" s="4" t="s">
         <v>3171</v>
@@ -52566,16 +52579,16 @@
         <v>399</v>
       </c>
       <c r="O2" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S2" s="3">
         <v>1</v>
@@ -52608,13 +52621,13 @@
         <v>3182</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD2" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF2" s="9">
         <v>0</v>
@@ -52644,13 +52657,13 @@
         <v>1</v>
       </c>
       <c r="AO2" s="3" t="s">
-        <v>3257</v>
+        <v>3256</v>
       </c>
       <c r="AP2" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AQ2" s="3" t="s">
-        <v>3258</v>
+        <v>3257</v>
       </c>
       <c r="AR2" s="3"/>
     </row>
@@ -52698,16 +52711,16 @@
         <v>405</v>
       </c>
       <c r="O3" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S3" s="3">
         <v>1</v>
@@ -52740,13 +52753,13 @@
         <v>3182</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD3" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE3" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF3" s="9">
         <v>0</v>
@@ -52776,13 +52789,13 @@
         <v>1</v>
       </c>
       <c r="AO3" s="3" t="s">
-        <v>3259</v>
+        <v>3258</v>
       </c>
       <c r="AP3" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AQ3" s="3" t="s">
-        <v>3260</v>
+        <v>3259</v>
       </c>
       <c r="AR3" s="3"/>
     </row>
@@ -52830,16 +52843,16 @@
         <v>411</v>
       </c>
       <c r="O4" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P4" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S4" s="3">
         <v>1</v>
@@ -52916,16 +52929,16 @@
         <v>416</v>
       </c>
       <c r="O5" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P5" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q5" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S5" s="3">
         <v>1</v>
@@ -52958,13 +52971,13 @@
         <v>3182</v>
       </c>
       <c r="AC5" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD5" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE5" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF5" s="9">
         <v>0</v>
@@ -53026,16 +53039,16 @@
         <v>421</v>
       </c>
       <c r="O6" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P6" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q6" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S6" s="3">
         <v>1</v>
@@ -53068,13 +53081,13 @@
         <v>3182</v>
       </c>
       <c r="AC6" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD6" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE6" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF6" s="9">
         <v>0</v>
@@ -53136,16 +53149,16 @@
         <v>426</v>
       </c>
       <c r="O7" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P7" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q7" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S7" s="3">
         <v>1</v>
@@ -53222,16 +53235,16 @@
         <v>431</v>
       </c>
       <c r="O8" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P8" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q8" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S8" s="3">
         <v>1</v>
@@ -53264,13 +53277,13 @@
         <v>3182</v>
       </c>
       <c r="AC8" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD8" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE8" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF8" s="9">
         <v>0</v>
@@ -53332,16 +53345,16 @@
         <v>436</v>
       </c>
       <c r="O9" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P9" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q9" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S9" s="3">
         <v>1</v>
@@ -53374,13 +53387,13 @@
         <v>3182</v>
       </c>
       <c r="AC9" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD9" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE9" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF9" s="9">
         <v>0</v>
@@ -53442,16 +53455,16 @@
         <v>441</v>
       </c>
       <c r="O10" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P10" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q10" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S10" s="3">
         <v>1</v>
@@ -53528,16 +53541,16 @@
         <v>446</v>
       </c>
       <c r="O11" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P11" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q11" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S11" s="3">
         <v>1</v>
@@ -53570,13 +53583,13 @@
         <v>3202</v>
       </c>
       <c r="AC11" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD11" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE11" s="8" t="s">
-        <v>3261</v>
+        <v>3260</v>
       </c>
       <c r="AF11" s="9">
         <v>0</v>
@@ -53606,13 +53619,13 @@
         <v>1</v>
       </c>
       <c r="AO11" s="3" t="s">
-        <v>3262</v>
+        <v>3261</v>
       </c>
       <c r="AP11" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AQ11" s="3" t="s">
-        <v>3263</v>
+        <v>3262</v>
       </c>
       <c r="AR11" s="3"/>
     </row>
@@ -53660,16 +53673,16 @@
         <v>451</v>
       </c>
       <c r="O12" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P12" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q12" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S12" s="3">
         <v>1</v>
@@ -53702,13 +53715,13 @@
         <v>3202</v>
       </c>
       <c r="AC12" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD12" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE12" s="8" t="s">
-        <v>3261</v>
+        <v>3260</v>
       </c>
       <c r="AF12" s="9">
         <v>0</v>
@@ -53738,13 +53751,13 @@
         <v>1</v>
       </c>
       <c r="AO12" s="3" t="s">
-        <v>3264</v>
+        <v>3263</v>
       </c>
       <c r="AP12" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AQ12" s="3" t="s">
-        <v>3265</v>
+        <v>3264</v>
       </c>
       <c r="AR12" s="3"/>
     </row>
@@ -53792,16 +53805,16 @@
         <v>456</v>
       </c>
       <c r="O13" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P13" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q13" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S13" s="3">
         <v>1</v>
@@ -53878,16 +53891,16 @@
         <v>461</v>
       </c>
       <c r="O14" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P14" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P14" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q14" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S14" s="3">
         <v>1</v>
@@ -53920,13 +53933,13 @@
         <v>3182</v>
       </c>
       <c r="AC14" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD14" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE14" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF14" s="9">
         <v>0</v>
@@ -53988,16 +54001,16 @@
         <v>466</v>
       </c>
       <c r="O15" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P15" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P15" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q15" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S15" s="3">
         <v>1</v>
@@ -54030,13 +54043,13 @@
         <v>3182</v>
       </c>
       <c r="AC15" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD15" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE15" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF15" s="9">
         <v>0</v>
@@ -54098,16 +54111,16 @@
         <v>471</v>
       </c>
       <c r="O16" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P16" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P16" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q16" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R16" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S16" s="3">
         <v>1</v>
@@ -54184,16 +54197,16 @@
         <v>476</v>
       </c>
       <c r="O17" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P17" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P17" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q17" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S17" s="3">
         <v>1</v>
@@ -54226,13 +54239,13 @@
         <v>3182</v>
       </c>
       <c r="AC17" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD17" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE17" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF17" s="9">
         <v>0</v>
@@ -54294,16 +54307,16 @@
         <v>481</v>
       </c>
       <c r="O18" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P18" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P18" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q18" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S18" s="3">
         <v>1</v>
@@ -54336,13 +54349,13 @@
         <v>3182</v>
       </c>
       <c r="AC18" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD18" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE18" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF18" s="9">
         <v>0</v>
@@ -54404,16 +54417,16 @@
         <v>486</v>
       </c>
       <c r="O19" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P19" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P19" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q19" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S19" s="3">
         <v>1</v>
@@ -54492,16 +54505,16 @@
         <v>491</v>
       </c>
       <c r="O20" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P20" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P20" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q20" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S20" s="3">
         <v>1</v>
@@ -54525,7 +54538,7 @@
         <v>123</v>
       </c>
       <c r="Z20" s="3" t="s">
-        <v>3211</v>
+        <v>3210</v>
       </c>
       <c r="AA20" s="3" t="s">
         <v>3186</v>
@@ -54534,13 +54547,13 @@
         <v>3182</v>
       </c>
       <c r="AC20" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD20" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE20" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF20" s="9">
         <v>0</v>
@@ -54570,13 +54583,13 @@
         <v>1</v>
       </c>
       <c r="AO20" s="3" t="s">
-        <v>3266</v>
+        <v>3265</v>
       </c>
       <c r="AP20" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AQ20" s="3" t="s">
-        <v>3267</v>
+        <v>3266</v>
       </c>
       <c r="AR20" s="3"/>
     </row>
@@ -54624,16 +54637,16 @@
         <v>496</v>
       </c>
       <c r="O21" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P21" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P21" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q21" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S21" s="3">
         <v>1</v>
@@ -54666,13 +54679,13 @@
         <v>3182</v>
       </c>
       <c r="AC21" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD21" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE21" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF21" s="9">
         <v>0</v>
@@ -54702,13 +54715,13 @@
         <v>1</v>
       </c>
       <c r="AO21" s="3" t="s">
-        <v>3268</v>
+        <v>3267</v>
       </c>
       <c r="AP21" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AQ21" s="3" t="s">
-        <v>3269</v>
+        <v>3268</v>
       </c>
       <c r="AR21" s="3"/>
     </row>
@@ -54756,16 +54769,16 @@
         <v>501</v>
       </c>
       <c r="O22" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P22" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P22" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q22" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S22" s="3">
         <v>1</v>
@@ -54842,16 +54855,16 @@
         <v>506</v>
       </c>
       <c r="O23" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P23" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P23" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q23" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R23" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S23" s="3">
         <v>1</v>
@@ -54884,13 +54897,13 @@
         <v>3182</v>
       </c>
       <c r="AC23" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD23" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE23" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF23" s="9">
         <v>0</v>
@@ -54952,16 +54965,16 @@
         <v>511</v>
       </c>
       <c r="O24" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P24" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P24" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q24" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R24" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S24" s="3">
         <v>1</v>
@@ -54994,13 +55007,13 @@
         <v>3182</v>
       </c>
       <c r="AC24" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD24" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE24" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF24" s="9">
         <v>0</v>
@@ -55062,16 +55075,16 @@
         <v>516</v>
       </c>
       <c r="O25" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P25" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P25" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q25" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R25" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S25" s="3">
         <v>1</v>
@@ -55148,16 +55161,16 @@
         <v>521</v>
       </c>
       <c r="O26" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P26" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P26" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q26" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R26" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S26" s="3">
         <v>1</v>
@@ -55190,13 +55203,13 @@
         <v>3182</v>
       </c>
       <c r="AC26" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD26" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE26" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF26" s="9">
         <v>0</v>
@@ -55258,16 +55271,16 @@
         <v>526</v>
       </c>
       <c r="O27" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P27" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P27" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q27" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R27" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S27" s="3">
         <v>1</v>
@@ -55300,13 +55313,13 @@
         <v>3182</v>
       </c>
       <c r="AC27" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD27" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE27" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF27" s="9">
         <v>0</v>
@@ -55368,16 +55381,16 @@
         <v>531</v>
       </c>
       <c r="O28" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P28" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P28" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q28" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R28" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S28" s="3">
         <v>1</v>
@@ -55456,16 +55469,16 @@
         <v>536</v>
       </c>
       <c r="O29" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P29" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P29" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q29" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R29" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S29" s="3">
         <v>1</v>
@@ -55489,7 +55502,7 @@
         <v>123</v>
       </c>
       <c r="Z29" s="3" t="s">
-        <v>3211</v>
+        <v>3210</v>
       </c>
       <c r="AA29" s="3" t="s">
         <v>3186</v>
@@ -55498,13 +55511,13 @@
         <v>3202</v>
       </c>
       <c r="AC29" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD29" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE29" s="8" t="s">
-        <v>3261</v>
+        <v>3260</v>
       </c>
       <c r="AF29" s="9">
         <v>0</v>
@@ -55534,13 +55547,13 @@
         <v>1</v>
       </c>
       <c r="AO29" s="3" t="s">
-        <v>3270</v>
+        <v>3269</v>
       </c>
       <c r="AP29" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AQ29" s="3" t="s">
-        <v>3271</v>
+        <v>3270</v>
       </c>
       <c r="AR29" s="3"/>
     </row>
@@ -55588,16 +55601,16 @@
         <v>541</v>
       </c>
       <c r="O30" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P30" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P30" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q30" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R30" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S30" s="3">
         <v>1</v>
@@ -55630,13 +55643,13 @@
         <v>3202</v>
       </c>
       <c r="AC30" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD30" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE30" s="8" t="s">
-        <v>3261</v>
+        <v>3260</v>
       </c>
       <c r="AF30" s="9">
         <v>0</v>
@@ -55666,13 +55679,13 @@
         <v>1</v>
       </c>
       <c r="AO30" s="3" t="s">
-        <v>3272</v>
+        <v>3271</v>
       </c>
       <c r="AP30" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AQ30" s="3" t="s">
-        <v>3273</v>
+        <v>3272</v>
       </c>
       <c r="AR30" s="3"/>
     </row>
@@ -55720,16 +55733,16 @@
         <v>546</v>
       </c>
       <c r="O31" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P31" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P31" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q31" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R31" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S31" s="3">
         <v>1</v>
@@ -55812,16 +55825,16 @@
         <v>551</v>
       </c>
       <c r="O32" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P32" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P32" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q32" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R32" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S32" s="3">
         <v>1</v>
@@ -55854,13 +55867,13 @@
         <v>3182</v>
       </c>
       <c r="AC32" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD32" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE32" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF32" s="9">
         <v>0</v>
@@ -55922,16 +55935,16 @@
         <v>556</v>
       </c>
       <c r="O33" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P33" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P33" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q33" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R33" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S33" s="3">
         <v>1</v>
@@ -55964,13 +55977,13 @@
         <v>3182</v>
       </c>
       <c r="AC33" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD33" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE33" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF33" s="9">
         <v>0</v>
@@ -56032,16 +56045,16 @@
         <v>561</v>
       </c>
       <c r="O34" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P34" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P34" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q34" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R34" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S34" s="3">
         <v>1</v>
@@ -56124,16 +56137,16 @@
         <v>566</v>
       </c>
       <c r="O35" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P35" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P35" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q35" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R35" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S35" s="3">
         <v>1</v>
@@ -56166,13 +56179,13 @@
         <v>3182</v>
       </c>
       <c r="AC35" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD35" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE35" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF35" s="9">
         <v>0</v>
@@ -56234,16 +56247,16 @@
         <v>571</v>
       </c>
       <c r="O36" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P36" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P36" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q36" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R36" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S36" s="3">
         <v>1</v>
@@ -56276,13 +56289,13 @@
         <v>3182</v>
       </c>
       <c r="AC36" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD36" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE36" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF36" s="9">
         <v>0</v>
@@ -56344,16 +56357,16 @@
         <v>576</v>
       </c>
       <c r="O37" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P37" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P37" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q37" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R37" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S37" s="3">
         <v>1</v>
@@ -56436,16 +56449,16 @@
         <v>581</v>
       </c>
       <c r="O38" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P38" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P38" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q38" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R38" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S38" s="3">
         <v>1</v>
@@ -56469,7 +56482,7 @@
         <v>214</v>
       </c>
       <c r="Z38" s="3" t="s">
-        <v>3218</v>
+        <v>3217</v>
       </c>
       <c r="AA38" s="3" t="s">
         <v>3186</v>
@@ -56478,13 +56491,13 @@
         <v>3182</v>
       </c>
       <c r="AC38" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD38" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE38" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF38" s="9">
         <v>0</v>
@@ -56496,10 +56509,10 @@
         <v>3189</v>
       </c>
       <c r="AI38" s="3" t="s">
+        <v>3218</v>
+      </c>
+      <c r="AJ38" s="3" t="s">
         <v>3219</v>
-      </c>
-      <c r="AJ38" s="3" t="s">
-        <v>3220</v>
       </c>
       <c r="AK38" s="3">
         <v>234234523</v>
@@ -56518,7 +56531,7 @@
         <v>3194</v>
       </c>
       <c r="AQ38" s="3" t="s">
-        <v>3274</v>
+        <v>3273</v>
       </c>
       <c r="AR38" s="3"/>
     </row>
@@ -56566,16 +56579,16 @@
         <v>586</v>
       </c>
       <c r="O39" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P39" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P39" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q39" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R39" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S39" s="3">
         <v>1</v>
@@ -56599,7 +56612,7 @@
         <v>214</v>
       </c>
       <c r="Z39" s="3" t="s">
-        <v>3218</v>
+        <v>3217</v>
       </c>
       <c r="AA39" s="3" t="s">
         <v>3186</v>
@@ -56608,13 +56621,13 @@
         <v>3182</v>
       </c>
       <c r="AC39" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD39" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE39" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF39" s="9">
         <v>0</v>
@@ -56626,10 +56639,10 @@
         <v>3189</v>
       </c>
       <c r="AI39" s="3" t="s">
+        <v>3218</v>
+      </c>
+      <c r="AJ39" s="3" t="s">
         <v>3219</v>
-      </c>
-      <c r="AJ39" s="3" t="s">
-        <v>3220</v>
       </c>
       <c r="AK39" s="3">
         <v>234234523</v>
@@ -56648,7 +56661,7 @@
         <v>3194</v>
       </c>
       <c r="AQ39" s="3" t="s">
-        <v>3275</v>
+        <v>3274</v>
       </c>
       <c r="AR39" s="3"/>
     </row>
@@ -56696,16 +56709,16 @@
         <v>591</v>
       </c>
       <c r="O40" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P40" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P40" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q40" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R40" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S40" s="3">
         <v>1</v>
@@ -56788,16 +56801,16 @@
         <v>596</v>
       </c>
       <c r="O41" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P41" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P41" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q41" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R41" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S41" s="3">
         <v>1</v>
@@ -56821,7 +56834,7 @@
         <v>214</v>
       </c>
       <c r="Z41" s="3" t="s">
-        <v>3218</v>
+        <v>3217</v>
       </c>
       <c r="AA41" s="3" t="s">
         <v>3186</v>
@@ -56830,13 +56843,13 @@
         <v>3182</v>
       </c>
       <c r="AC41" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD41" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE41" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF41" s="9">
         <v>0</v>
@@ -56848,10 +56861,10 @@
         <v>3189</v>
       </c>
       <c r="AI41" s="3" t="s">
+        <v>3218</v>
+      </c>
+      <c r="AJ41" s="3" t="s">
         <v>3219</v>
-      </c>
-      <c r="AJ41" s="3" t="s">
-        <v>3220</v>
       </c>
       <c r="AK41" s="3">
         <v>234234523</v>
@@ -56914,16 +56927,16 @@
         <v>601</v>
       </c>
       <c r="O42" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P42" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P42" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q42" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R42" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S42" s="3">
         <v>1</v>
@@ -56947,7 +56960,7 @@
         <v>214</v>
       </c>
       <c r="Z42" s="3" t="s">
-        <v>3218</v>
+        <v>3217</v>
       </c>
       <c r="AA42" s="3" t="s">
         <v>3186</v>
@@ -56956,13 +56969,13 @@
         <v>3182</v>
       </c>
       <c r="AC42" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD42" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE42" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF42" s="9">
         <v>0</v>
@@ -56974,10 +56987,10 @@
         <v>3189</v>
       </c>
       <c r="AI42" s="3" t="s">
+        <v>3218</v>
+      </c>
+      <c r="AJ42" s="3" t="s">
         <v>3219</v>
-      </c>
-      <c r="AJ42" s="3" t="s">
-        <v>3220</v>
       </c>
       <c r="AK42" s="3">
         <v>234234523</v>
@@ -57040,16 +57053,16 @@
         <v>606</v>
       </c>
       <c r="O43" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P43" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P43" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q43" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R43" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S43" s="3">
         <v>1</v>
@@ -57132,16 +57145,16 @@
         <v>611</v>
       </c>
       <c r="O44" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P44" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P44" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q44" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R44" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S44" s="3">
         <v>1</v>
@@ -57174,13 +57187,13 @@
         <v>3182</v>
       </c>
       <c r="AC44" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD44" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE44" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF44" s="9">
         <v>0</v>
@@ -57192,10 +57205,10 @@
         <v>3189</v>
       </c>
       <c r="AI44" s="3" t="s">
+        <v>3218</v>
+      </c>
+      <c r="AJ44" s="3" t="s">
         <v>3219</v>
-      </c>
-      <c r="AJ44" s="3" t="s">
-        <v>3220</v>
       </c>
       <c r="AK44" s="3">
         <v>234234523</v>
@@ -57258,16 +57271,16 @@
         <v>616</v>
       </c>
       <c r="O45" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P45" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P45" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q45" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R45" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S45" s="3">
         <v>1</v>
@@ -57300,13 +57313,13 @@
         <v>3182</v>
       </c>
       <c r="AC45" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD45" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE45" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF45" s="9">
         <v>0</v>
@@ -57318,10 +57331,10 @@
         <v>3189</v>
       </c>
       <c r="AI45" s="3" t="s">
+        <v>3218</v>
+      </c>
+      <c r="AJ45" s="3" t="s">
         <v>3219</v>
-      </c>
-      <c r="AJ45" s="3" t="s">
-        <v>3220</v>
       </c>
       <c r="AK45" s="3">
         <v>234234523</v>
@@ -57384,16 +57397,16 @@
         <v>621</v>
       </c>
       <c r="O46" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P46" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P46" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q46" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R46" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S46" s="3">
         <v>1</v>
@@ -57476,16 +57489,16 @@
         <v>626</v>
       </c>
       <c r="O47" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P47" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P47" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q47" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R47" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S47" s="3">
         <v>1</v>
@@ -57509,7 +57522,7 @@
         <v>214</v>
       </c>
       <c r="Z47" s="3" t="s">
-        <v>3218</v>
+        <v>3217</v>
       </c>
       <c r="AA47" s="3" t="s">
         <v>3186</v>
@@ -57518,13 +57531,13 @@
         <v>3202</v>
       </c>
       <c r="AC47" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD47" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE47" s="8" t="s">
-        <v>3261</v>
+        <v>3260</v>
       </c>
       <c r="AF47" s="9">
         <v>0</v>
@@ -57536,10 +57549,10 @@
         <v>3189</v>
       </c>
       <c r="AI47" s="3" t="s">
+        <v>3218</v>
+      </c>
+      <c r="AJ47" s="3" t="s">
         <v>3219</v>
-      </c>
-      <c r="AJ47" s="3" t="s">
-        <v>3220</v>
       </c>
       <c r="AK47" s="3">
         <v>234234523</v>
@@ -57558,7 +57571,7 @@
         <v>3194</v>
       </c>
       <c r="AQ47" s="3" t="s">
-        <v>3276</v>
+        <v>3275</v>
       </c>
       <c r="AR47" s="3"/>
     </row>
@@ -57606,16 +57619,16 @@
         <v>631</v>
       </c>
       <c r="O48" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P48" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P48" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q48" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R48" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S48" s="3">
         <v>1</v>
@@ -57639,7 +57652,7 @@
         <v>214</v>
       </c>
       <c r="Z48" s="3" t="s">
-        <v>3218</v>
+        <v>3217</v>
       </c>
       <c r="AA48" s="3" t="s">
         <v>3186</v>
@@ -57648,13 +57661,13 @@
         <v>3202</v>
       </c>
       <c r="AC48" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD48" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE48" s="8" t="s">
-        <v>3261</v>
+        <v>3260</v>
       </c>
       <c r="AF48" s="9">
         <v>0</v>
@@ -57666,10 +57679,10 @@
         <v>3189</v>
       </c>
       <c r="AI48" s="3" t="s">
+        <v>3218</v>
+      </c>
+      <c r="AJ48" s="3" t="s">
         <v>3219</v>
-      </c>
-      <c r="AJ48" s="3" t="s">
-        <v>3220</v>
       </c>
       <c r="AK48" s="3">
         <v>234234523</v>
@@ -57688,7 +57701,7 @@
         <v>3194</v>
       </c>
       <c r="AQ48" s="3" t="s">
-        <v>3277</v>
+        <v>3276</v>
       </c>
       <c r="AR48" s="3"/>
     </row>
@@ -57736,10 +57749,10 @@
         <v>636</v>
       </c>
       <c r="O49" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P49" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P49" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q49" s="3"/>
       <c r="R49" s="3"/>
@@ -57816,16 +57829,16 @@
         <v>641</v>
       </c>
       <c r="O50" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P50" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P50" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q50" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R50" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S50" s="3">
         <v>1</v>
@@ -57849,7 +57862,7 @@
         <v>214</v>
       </c>
       <c r="Z50" s="3" t="s">
-        <v>3218</v>
+        <v>3217</v>
       </c>
       <c r="AA50" s="3" t="s">
         <v>3186</v>
@@ -57858,13 +57871,13 @@
         <v>3182</v>
       </c>
       <c r="AC50" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD50" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE50" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF50" s="9">
         <v>0</v>
@@ -57876,10 +57889,10 @@
         <v>3189</v>
       </c>
       <c r="AI50" s="3" t="s">
+        <v>3218</v>
+      </c>
+      <c r="AJ50" s="3" t="s">
         <v>3219</v>
-      </c>
-      <c r="AJ50" s="3" t="s">
-        <v>3220</v>
       </c>
       <c r="AK50" s="3">
         <v>234234523</v>
@@ -57942,16 +57955,16 @@
         <v>646</v>
       </c>
       <c r="O51" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P51" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P51" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q51" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R51" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S51" s="3">
         <v>1</v>
@@ -57975,7 +57988,7 @@
         <v>214</v>
       </c>
       <c r="Z51" s="3" t="s">
-        <v>3218</v>
+        <v>3217</v>
       </c>
       <c r="AA51" s="3" t="s">
         <v>3186</v>
@@ -57984,13 +57997,13 @@
         <v>3182</v>
       </c>
       <c r="AC51" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD51" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE51" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF51" s="9">
         <v>0</v>
@@ -58002,10 +58015,10 @@
         <v>3189</v>
       </c>
       <c r="AI51" s="3" t="s">
+        <v>3218</v>
+      </c>
+      <c r="AJ51" s="3" t="s">
         <v>3219</v>
-      </c>
-      <c r="AJ51" s="3" t="s">
-        <v>3220</v>
       </c>
       <c r="AK51" s="3">
         <v>234234523</v>
@@ -58068,10 +58081,10 @@
         <v>651</v>
       </c>
       <c r="O52" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P52" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P52" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q52" s="3"/>
       <c r="R52" s="3"/>
@@ -58148,16 +58161,16 @@
         <v>656</v>
       </c>
       <c r="O53" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P53" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P53" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q53" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R53" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S53" s="3">
         <v>1</v>
@@ -58181,7 +58194,7 @@
         <v>214</v>
       </c>
       <c r="Z53" s="3" t="s">
-        <v>3218</v>
+        <v>3217</v>
       </c>
       <c r="AA53" s="3" t="s">
         <v>3186</v>
@@ -58190,13 +58203,13 @@
         <v>3182</v>
       </c>
       <c r="AC53" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD53" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE53" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF53" s="9">
         <v>0</v>
@@ -58208,10 +58221,10 @@
         <v>3189</v>
       </c>
       <c r="AI53" s="3" t="s">
+        <v>3218</v>
+      </c>
+      <c r="AJ53" s="3" t="s">
         <v>3219</v>
-      </c>
-      <c r="AJ53" s="3" t="s">
-        <v>3220</v>
       </c>
       <c r="AK53" s="3">
         <v>234234523</v>
@@ -58274,16 +58287,16 @@
         <v>661</v>
       </c>
       <c r="O54" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P54" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P54" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q54" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R54" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S54" s="3">
         <v>1</v>
@@ -58307,7 +58320,7 @@
         <v>214</v>
       </c>
       <c r="Z54" s="3" t="s">
-        <v>3218</v>
+        <v>3217</v>
       </c>
       <c r="AA54" s="3" t="s">
         <v>3186</v>
@@ -58316,13 +58329,13 @@
         <v>3182</v>
       </c>
       <c r="AC54" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD54" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE54" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF54" s="9">
         <v>0</v>
@@ -58334,10 +58347,10 @@
         <v>3189</v>
       </c>
       <c r="AI54" s="3" t="s">
+        <v>3218</v>
+      </c>
+      <c r="AJ54" s="3" t="s">
         <v>3219</v>
-      </c>
-      <c r="AJ54" s="3" t="s">
-        <v>3220</v>
       </c>
       <c r="AK54" s="3">
         <v>234234523</v>
@@ -58400,10 +58413,10 @@
         <v>666</v>
       </c>
       <c r="O55" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P55" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P55" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q55" s="3"/>
       <c r="R55" s="3"/>
@@ -58480,16 +58493,16 @@
         <v>671</v>
       </c>
       <c r="O56" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P56" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P56" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q56" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R56" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S56" s="3">
         <v>1</v>
@@ -58510,7 +58523,7 @@
         <v>3182</v>
       </c>
       <c r="Y56" s="3" t="s">
-        <v>3229</v>
+        <v>3228</v>
       </c>
       <c r="Z56" s="3" t="s">
         <v>3185</v>
@@ -58522,13 +58535,13 @@
         <v>3182</v>
       </c>
       <c r="AC56" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD56" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE56" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF56" s="9">
         <v>0</v>
@@ -58558,13 +58571,13 @@
         <v>1</v>
       </c>
       <c r="AO56" s="3" t="s">
-        <v>3278</v>
+        <v>3277</v>
       </c>
       <c r="AP56" s="3" t="s">
         <v>3194</v>
       </c>
       <c r="AQ56" s="3" t="s">
-        <v>3279</v>
+        <v>3278</v>
       </c>
       <c r="AR56" s="3"/>
     </row>
@@ -58612,16 +58625,16 @@
         <v>676</v>
       </c>
       <c r="O57" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P57" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P57" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q57" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R57" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S57" s="3">
         <v>1</v>
@@ -58642,7 +58655,7 @@
         <v>3182</v>
       </c>
       <c r="Y57" s="3" t="s">
-        <v>3229</v>
+        <v>3228</v>
       </c>
       <c r="Z57" s="3" t="s">
         <v>3185</v>
@@ -58654,13 +58667,13 @@
         <v>3182</v>
       </c>
       <c r="AC57" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD57" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE57" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF57" s="9">
         <v>0</v>
@@ -58690,13 +58703,13 @@
         <v>1</v>
       </c>
       <c r="AO57" s="3" t="s">
-        <v>3280</v>
+        <v>3279</v>
       </c>
       <c r="AP57" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AQ57" s="3" t="s">
-        <v>3281</v>
+        <v>3280</v>
       </c>
       <c r="AR57" s="3"/>
     </row>
@@ -58744,10 +58757,10 @@
         <v>681</v>
       </c>
       <c r="O58" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P58" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P58" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q58" s="3"/>
       <c r="R58" s="3"/>
@@ -58824,16 +58837,16 @@
         <v>686</v>
       </c>
       <c r="O59" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P59" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P59" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q59" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R59" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S59" s="3">
         <v>1</v>
@@ -58854,7 +58867,7 @@
         <v>3182</v>
       </c>
       <c r="Y59" s="3" t="s">
-        <v>3229</v>
+        <v>3228</v>
       </c>
       <c r="Z59" s="3" t="s">
         <v>3185</v>
@@ -58866,13 +58879,13 @@
         <v>3182</v>
       </c>
       <c r="AC59" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD59" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE59" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF59" s="9">
         <v>0</v>
@@ -58950,16 +58963,16 @@
         <v>691</v>
       </c>
       <c r="O60" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P60" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P60" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q60" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R60" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S60" s="3">
         <v>1</v>
@@ -58980,7 +58993,7 @@
         <v>3182</v>
       </c>
       <c r="Y60" s="3" t="s">
-        <v>3229</v>
+        <v>3228</v>
       </c>
       <c r="Z60" s="3" t="s">
         <v>3185</v>
@@ -58992,13 +59005,13 @@
         <v>3182</v>
       </c>
       <c r="AC60" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD60" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE60" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF60" s="9">
         <v>0</v>
@@ -59076,10 +59089,10 @@
         <v>696</v>
       </c>
       <c r="O61" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P61" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P61" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q61" s="3"/>
       <c r="R61" s="3"/>
@@ -59156,16 +59169,16 @@
         <v>701</v>
       </c>
       <c r="O62" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P62" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P62" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q62" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R62" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S62" s="3">
         <v>1</v>
@@ -59186,7 +59199,7 @@
         <v>3182</v>
       </c>
       <c r="Y62" s="3" t="s">
-        <v>3229</v>
+        <v>3228</v>
       </c>
       <c r="Z62" s="3" t="s">
         <v>3185</v>
@@ -59198,13 +59211,13 @@
         <v>3182</v>
       </c>
       <c r="AC62" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD62" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE62" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF62" s="9">
         <v>0</v>
@@ -59282,16 +59295,16 @@
         <v>706</v>
       </c>
       <c r="O63" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P63" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P63" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q63" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R63" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S63" s="3">
         <v>1</v>
@@ -59312,7 +59325,7 @@
         <v>3182</v>
       </c>
       <c r="Y63" s="3" t="s">
-        <v>3229</v>
+        <v>3228</v>
       </c>
       <c r="Z63" s="3" t="s">
         <v>3185</v>
@@ -59324,13 +59337,13 @@
         <v>3182</v>
       </c>
       <c r="AC63" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD63" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE63" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AF63" s="9">
         <v>0</v>
@@ -59408,10 +59421,10 @@
         <v>711</v>
       </c>
       <c r="O64" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P64" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P64" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q64" s="3"/>
       <c r="R64" s="3"/>
@@ -59488,16 +59501,16 @@
         <v>716</v>
       </c>
       <c r="O65" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P65" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P65" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q65" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R65" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S65" s="3">
         <v>1</v>
@@ -59518,7 +59531,7 @@
         <v>3182</v>
       </c>
       <c r="Y65" s="3" t="s">
-        <v>3229</v>
+        <v>3228</v>
       </c>
       <c r="Z65" s="3" t="s">
         <v>3185</v>
@@ -59530,13 +59543,13 @@
         <v>3202</v>
       </c>
       <c r="AC65" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD65" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE65" s="8" t="s">
-        <v>3261</v>
+        <v>3260</v>
       </c>
       <c r="AF65" s="9">
         <v>0</v>
@@ -59566,13 +59579,13 @@
         <v>1</v>
       </c>
       <c r="AO65" s="3" t="s">
-        <v>3282</v>
+        <v>3281</v>
       </c>
       <c r="AP65" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AQ65" s="3" t="s">
-        <v>3283</v>
+        <v>3282</v>
       </c>
       <c r="AR65" s="3"/>
     </row>
@@ -59620,16 +59633,16 @@
         <v>721</v>
       </c>
       <c r="O66" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P66" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P66" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q66" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R66" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S66" s="3">
         <v>1</v>
@@ -59650,7 +59663,7 @@
         <v>3182</v>
       </c>
       <c r="Y66" s="3" t="s">
-        <v>3229</v>
+        <v>3228</v>
       </c>
       <c r="Z66" s="3" t="s">
         <v>3185</v>
@@ -59662,13 +59675,13 @@
         <v>3202</v>
       </c>
       <c r="AC66" s="3" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="AD66" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE66" s="8" t="s">
-        <v>3261</v>
+        <v>3260</v>
       </c>
       <c r="AF66" s="9">
         <v>0</v>
@@ -59698,13 +59711,13 @@
         <v>1</v>
       </c>
       <c r="AO66" s="3" t="s">
-        <v>3284</v>
+        <v>3283</v>
       </c>
       <c r="AP66" s="3" t="s">
         <v>3194</v>
       </c>
       <c r="AQ66" s="3" t="s">
-        <v>3285</v>
+        <v>3284</v>
       </c>
       <c r="AR66" s="3"/>
     </row>
@@ -59752,7 +59765,7 @@
         <v>726</v>
       </c>
       <c r="O67" s="3" t="s">
-        <v>3253</v>
+        <v>3252</v>
       </c>
       <c r="P67" s="3"/>
       <c r="Q67" s="3"/>
@@ -59830,16 +59843,16 @@
         <v>731</v>
       </c>
       <c r="O68" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P68" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P68" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q68" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R68" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S68" s="3">
         <v>1</v>
@@ -59924,16 +59937,16 @@
         <v>736</v>
       </c>
       <c r="O69" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P69" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P69" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q69" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R69" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S69" s="3">
         <v>1</v>
@@ -60018,7 +60031,7 @@
         <v>741</v>
       </c>
       <c r="O70" s="3" t="s">
-        <v>3253</v>
+        <v>3252</v>
       </c>
       <c r="P70" s="3"/>
       <c r="Q70" s="3"/>
@@ -60096,16 +60109,16 @@
         <v>746</v>
       </c>
       <c r="O71" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P71" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P71" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q71" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R71" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S71" s="3">
         <v>1</v>
@@ -60190,16 +60203,16 @@
         <v>751</v>
       </c>
       <c r="O72" s="3" t="s">
+        <v>3252</v>
+      </c>
+      <c r="P72" s="3" t="s">
         <v>3253</v>
-      </c>
-      <c r="P72" s="3" t="s">
-        <v>3254</v>
       </c>
       <c r="Q72" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R72" s="3" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="S72" s="3">
         <v>1</v>
@@ -60284,7 +60297,7 @@
         <v>756</v>
       </c>
       <c r="O73" s="3" t="s">
-        <v>3253</v>
+        <v>3252</v>
       </c>
       <c r="P73" s="3"/>
       <c r="Q73" s="3"/>

</xml_diff>

<commit_message>
fix: update BigC_Ecomm_TestCases_AutomationMasterSheet.xlsx to improve test case automation
</commit_message>
<xml_diff>
--- a/data/BigCommerceData/BigC_Ecomm_TestCases_AutomationMasterSheet.xlsx
+++ b/data/BigCommerceData/BigC_Ecomm_TestCases_AutomationMasterSheet.xlsx
@@ -9639,13 +9639,13 @@
     <t>USD $132.15</t>
   </si>
   <si>
-    <t>2025-09-30T12:25:19.193Z</t>
+    <t>2025-10-01T12:27:07.945Z</t>
   </si>
   <si>
     <t>["All steps completed successfully\nExecution Time: 2025-09-29T15:58:39.464Z\nScreenshot: test-results/screenshots/TC0202.png","Status: Passed","Last Updated: 2025-09-29T15:58:39.606Z","---"]</t>
   </si>
   <si>
-    <t>["=== Test Failure Details ===","Failed Step: Comparison","Error Message: Order data mismatch for BigC Order 434397 vs Kibo Order 434398. 11/13 key fields matched. Differences: OrderNumber: BigC=434397, Kibo=434398; EntityOrderId: BigC=443779, Kibo=443780","Failure Timestamp: 2025-09-30T12:25:19.037Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Comparison\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-30T12:25:19.193Z","---"]</t>
+    <t>["All steps completed successfully\nExecution Time: 2025-10-01T12:27:07.799Z\nScreenshot: N/A","Status: Passed","Last Updated: 2025-10-01T12:27:07.945Z","---"]</t>
   </si>
   <si>
     <t>["All steps completed successfully\nExecution Time: 2025-09-30T12:21:53.025Z\nScreenshot: N/A","Status: Passed","Last Updated: 2025-09-30T12:21:53.111Z","---"]</t>
@@ -48380,7 +48380,7 @@
         <v>3205</v>
       </c>
       <c r="AT11" s="3" t="s">
-        <v>3194</v>
+        <v>3192</v>
       </c>
       <c r="AU11" s="3" t="s">
         <v>3206</v>

</xml_diff>

<commit_message>
fix: enhance SettlementReportPage with no data message and filterAndSearch method for improved order comparison
</commit_message>
<xml_diff>
--- a/data/BigCommerceData/BigC_Ecomm_TestCases_AutomationMasterSheet.xlsx
+++ b/data/BigCommerceData/BigC_Ecomm_TestCases_AutomationMasterSheet.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20374" uniqueCount="3286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20375" uniqueCount="3287">
   <si>
     <t>Global Test Case ID</t>
   </si>
@@ -9597,16 +9597,16 @@
     <t>Standard product order for existing customer</t>
   </si>
   <si>
-    <t>357043</t>
-  </si>
-  <si>
-    <t>2025-09-30T12:29:29.937Z</t>
+    <t>357052</t>
+  </si>
+  <si>
+    <t>2025-10-06T22:04:39.219Z</t>
   </si>
   <si>
     <t>Passed</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-30T07:28:24.806Z\nScreenshot: test-results/screenshots/TC0193.png","Status: Passed","Last Updated: 2025-09-30T07:28:25.822Z","---"]</t>
+    <t>["All steps completed successfully\nExecution Time: 2025-10-06T11:15:50.527Z\nScreenshot: test-results/screenshots/TC0193.png","Status: Passed","Last Updated: 2025-10-06T11:15:50.636Z","---"]</t>
   </si>
   <si>
     <t>Failed</t>
@@ -9615,22 +9615,22 @@
     <t>["=== Test Failure Details ===","Failed Step: Comparison","Error Message: Order data mismatch for BigC Order 357043 vs Kibo Order 358102. 3/13 key fields matched. Differences: OrderNumber: BigC=357043, Kibo=358102; EntityOrderId: BigC=356510, Kibo=357566; Total: BigC=0, Kibo=11000; Status: BigC=Completed, Kibo=Abandoned; PaymentStatus: BigC=Paid, Kibo=Unpaid; FulfillmentStatus: BigC=Fulfilled, Kibo=NotFulfilled; SubTotal: BigC=14.99, Kibo=11000; CustomerAccountId: BigC=517693, Kibo=null; Email: BigC=main-OrderStatusTest20240619785-99d1-ec8f6a0898f0@ged.com, Kibo=null; SiteId: BigC=40996, Kibo=57983","Failure Timestamp: 2025-09-30T12:29:29.759Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Comparison\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-30T12:29:29.937Z","---"]</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-30T12:21:48.377Z\nScreenshot: N/A","Status: Passed","Last Updated: 2025-09-30T12:21:48.523Z","---"]</t>
-  </si>
-  <si>
-    <t>357039</t>
+    <t>["All steps completed successfully\nExecution Time: 2025-10-06T22:04:39.145Z\nScreenshot: N/A","Status: Passed","Last Updated: 2025-10-06T22:04:39.219Z","---"]</t>
+  </si>
+  <si>
+    <t>357056</t>
   </si>
   <si>
     <t>357028</t>
   </si>
   <si>
-    <t>2025-09-30T12:21:50.938Z</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-29T16:04:43.806Z\nScreenshot: test-results/screenshots/TC0194.png","Status: Passed","Last Updated: 2025-09-29T16:04:43.938Z","---"]</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-30T12:21:50.842Z\nScreenshot: N/A","Status: Passed","Last Updated: 2025-09-30T12:21:50.938Z","---"]</t>
+    <t>2025-10-06T22:04:45.083Z</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-10-06T11:22:51.813Z\nScreenshot: test-results/screenshots/TC0194.png","Status: Passed","Last Updated: 2025-10-06T11:22:52.200Z","---"]</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-10-06T22:04:44.961Z\nScreenshot: N/A","Status: Passed","Last Updated: 2025-10-06T22:04:45.083Z","---"]</t>
   </si>
   <si>
     <t>USD $20.00</t>
@@ -9639,25 +9639,28 @@
     <t>USD $132.15</t>
   </si>
   <si>
-    <t>2025-10-01T12:27:07.945Z</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-29T15:58:39.464Z\nScreenshot: test-results/screenshots/TC0202.png","Status: Passed","Last Updated: 2025-09-29T15:58:39.606Z","---"]</t>
+    <t>357053</t>
+  </si>
+  <si>
+    <t>2025-10-06T22:04:50.644Z</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-10-06T11:16:37.336Z\nScreenshot: test-results/screenshots/TC0202.png","Status: Passed","Last Updated: 2025-10-06T11:16:37.469Z","---"]</t>
   </si>
   <si>
     <t>["All steps completed successfully\nExecution Time: 2025-10-01T12:27:07.799Z\nScreenshot: N/A","Status: Passed","Last Updated: 2025-10-01T12:27:07.945Z","---"]</t>
   </si>
   <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-30T12:21:53.025Z\nScreenshot: N/A","Status: Passed","Last Updated: 2025-09-30T12:21:53.111Z","---"]</t>
-  </si>
-  <si>
-    <t>357040</t>
-  </si>
-  <si>
-    <t>2025-09-29T16:05:38.057Z</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-29T16:05:37.959Z\nScreenshot: test-results/screenshots/TC0203.png","Status: Passed","Last Updated: 2025-09-29T16:05:38.057Z","---"]</t>
+    <t>["All steps completed successfully\nExecution Time: 2025-10-06T22:04:50.559Z\nScreenshot: N/A","Status: Passed","Last Updated: 2025-10-06T22:04:50.644Z","---"]</t>
+  </si>
+  <si>
+    <t>357057</t>
+  </si>
+  <si>
+    <t>2025-10-06T11:23:49.542Z</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-10-06T11:23:49.425Z\nScreenshot: test-results/screenshots/TC0203.png","Status: Passed","Last Updated: 2025-10-06T11:23:49.542Z","---"]</t>
   </si>
   <si>
     <t>Customer transfers money directly to the seller's bank account.</t>
@@ -9690,25 +9693,25 @@
     <t>American Express</t>
   </si>
   <si>
-    <t>2025-09-30T09:06:05.086Z</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Verify Order Creation in All Orders Page","Error Message: locator.waitFor: Timeout 10000ms exceeded.\nCall log:\n\u001b[2m  - waiting for locator('#content-iframe').contentFrame().locator('//div[@id=\"orderStatus\"]//p') to be visible\u001b[22m\n","Failure Timestamp: 2025-09-29T16:01:32.282Z","Failure Screenshot: test-results/screenshots/failure_TC0229_1759161691942.png","","=== Additional Notes ===","Test failed during: Verify Order Creation in All Orders Page\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-29T16:01:32.460Z","---"]</t>
+    <t>2025-10-06T11:19:31.206Z</t>
+  </si>
+  <si>
+    <t>["=== Test Failure Details ===","Failed Step: Verify Order Creation in All Orders Page","Error Message: locator.waitFor: Timeout 10000ms exceeded.\nCall log:\n\u001b[2m  - waiting for locator('#content-iframe').contentFrame().locator('//div[@id=\"orderStatus\"]//p') to be visible\u001b[22m\n","Failure Timestamp: 2025-10-06T11:19:31.022Z","Failure Screenshot: test-results/screenshots/failure_TC0229_1759749570704.png","","=== Additional Notes ===","Test failed during: Verify Order Creation in All Orders Page\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-10-06T11:19:31.206Z","---"]</t>
   </si>
   <si>
     <t>["All steps completed successfully\nExecution Time: 2025-09-30T09:06:04.906Z\nScreenshot: N/A","Status: Passed","Last Updated: 2025-09-30T09:06:05.086Z","---"]</t>
   </si>
   <si>
-    <t>2025-09-29T16:08:36.099Z</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Verify Order Creation in All Orders Page","Error Message: locator.waitFor: Timeout 10000ms exceeded.\nCall log:\n\u001b[2m  - waiting for locator('#content-iframe').contentFrame().locator('//div[@id=\"orderStatus\"]//p') to be visible\u001b[22m\n","Failure Timestamp: 2025-09-29T16:08:35.919Z","Failure Screenshot: test-results/screenshots/failure_TC0230_1759162115355.png","","=== Additional Notes ===","Test failed during: Verify Order Creation in All Orders Page\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-29T16:08:36.099Z","---"]</t>
-  </si>
-  <si>
-    <t>2025-09-30T09:06:12.928Z</t>
-  </si>
-  <si>
-    <t>["=== Test Failure Details ===","Failed Step: Verify Order Creation in All Orders Page","Error Message: locator.waitFor: Timeout 10000ms exceeded.\nCall log:\n\u001b[2m  - waiting for locator('#content-iframe').contentFrame().locator('//div[@id=\"orderStatus\"]//p') to be visible\u001b[22m\n","Failure Timestamp: 2025-09-29T16:02:27.739Z","Failure Screenshot: test-results/screenshots/failure_TC0238_1759161747337.png","","=== Additional Notes ===","Test failed during: Verify Order Creation in All Orders Page\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-29T16:02:27.988Z","---"]</t>
+    <t>2025-10-06T11:26:49.271Z</t>
+  </si>
+  <si>
+    <t>["=== Test Failure Details ===","Failed Step: Verify Order Creation in All Orders Page","Error Message: locator.waitFor: Timeout 10000ms exceeded.\nCall log:\n\u001b[2m  - waiting for locator('#content-iframe').contentFrame().locator('//div[@id=\"orderStatus\"]//p') to be visible\u001b[22m\n","Failure Timestamp: 2025-10-06T11:26:49.100Z","Failure Screenshot: test-results/screenshots/failure_TC0230_1759750008755.png","","=== Additional Notes ===","Test failed during: Verify Order Creation in All Orders Page\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-10-06T11:26:49.271Z","---"]</t>
+  </si>
+  <si>
+    <t>2025-10-06T11:20:27.504Z</t>
+  </si>
+  <si>
+    <t>["=== Test Failure Details ===","Failed Step: Verify Order Creation in All Orders Page","Error Message: locator.waitFor: Timeout 10000ms exceeded.\nCall log:\n\u001b[2m  - waiting for locator('#content-iframe').contentFrame().locator('//div[@id=\"orderStatus\"]//p') to be visible\u001b[22m\n","Failure Timestamp: 2025-10-06T11:20:27.341Z","Failure Screenshot: test-results/screenshots/failure_TC0238_1759749627052.png","","=== Additional Notes ===","Test failed during: Verify Order Creation in All Orders Page\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-10-06T11:20:27.504Z","---"]</t>
   </si>
   <si>
     <t>["All steps completed successfully\nExecution Time: 2025-09-30T09:06:12.734Z\nScreenshot: N/A","Status: Passed","Last Updated: 2025-09-30T09:06:12.928Z","---"]</t>
@@ -9717,46 +9720,46 @@
     <t>Manual payment</t>
   </si>
   <si>
-    <t>357037</t>
-  </si>
-  <si>
-    <t>2025-09-30T09:06:20.778Z</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-29T16:03:10.238Z\nScreenshot: test-results/screenshots/TC0247.png","Status: Passed","Last Updated: 2025-09-29T16:03:10.357Z","---"]</t>
+    <t>357054</t>
+  </si>
+  <si>
+    <t>2025-10-06T11:21:10.966Z</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-10-06T11:21:10.860Z\nScreenshot: test-results/screenshots/TC0247.png","Status: Passed","Last Updated: 2025-10-06T11:21:10.966Z","---"]</t>
   </si>
   <si>
     <t>["All steps completed successfully\nExecution Time: 2025-09-30T09:06:20.598Z\nScreenshot: N/A","Status: Passed","Last Updated: 2025-09-30T09:06:20.778Z","---"]</t>
   </si>
   <si>
-    <t>357041</t>
-  </si>
-  <si>
-    <t>2025-09-29T16:10:28.308Z</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-29T16:10:27.789Z\nScreenshot: test-results/screenshots/TC0248.png","Status: Passed","Last Updated: 2025-09-29T16:10:28.308Z","---"]</t>
-  </si>
-  <si>
-    <t>357038</t>
-  </si>
-  <si>
-    <t>2025-09-30T09:06:56.734Z</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-29T16:03:56.955Z\nScreenshot: test-results/screenshots/TC0256.png","Status: Passed","Last Updated: 2025-09-29T16:03:57.056Z","---"]</t>
+    <t>357058</t>
+  </si>
+  <si>
+    <t>2025-10-06T11:28:41.573Z</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-10-06T11:28:41.420Z\nScreenshot: test-results/screenshots/TC0248.png","Status: Passed","Last Updated: 2025-10-06T11:28:41.573Z","---"]</t>
+  </si>
+  <si>
+    <t>357055</t>
+  </si>
+  <si>
+    <t>2025-10-06T11:21:56.858Z</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-10-06T11:21:56.759Z\nScreenshot: test-results/screenshots/TC0256.png","Status: Passed","Last Updated: 2025-10-06T11:21:56.858Z","---"]</t>
   </si>
   <si>
     <t>["All steps completed successfully\nExecution Time: 2025-09-30T09:06:56.529Z\nScreenshot: N/A","Status: Passed","Last Updated: 2025-09-30T09:06:56.734Z","---"]</t>
   </si>
   <si>
-    <t>357042</t>
-  </si>
-  <si>
-    <t>2025-09-29T16:11:21.246Z</t>
-  </si>
-  <si>
-    <t>["All steps completed successfully\nExecution Time: 2025-09-29T16:11:20.834Z\nScreenshot: test-results/screenshots/TC0257.png","Status: Passed","Last Updated: 2025-09-29T16:11:21.246Z","---"]</t>
+    <t>357059</t>
+  </si>
+  <si>
+    <t>2025-10-06T11:29:38.915Z</t>
+  </si>
+  <si>
+    <t>["All steps completed successfully\nExecution Time: 2025-10-06T11:29:38.791Z\nScreenshot: test-results/screenshots/TC0257.png","Status: Passed","Last Updated: 2025-10-06T11:29:38.915Z","---"]</t>
   </si>
   <si>
     <t>["=== Test Failure Details ===","Failed Step: Database Verification","Error Message: BigC_OrderId not found in Excel sheet. Ensure the order has been created first.","Failure Timestamp: 2025-09-29T08:54:57.743Z","Failure Screenshot: Not available","","=== Additional Notes ===","Test failed during: Database Verification\nPrevious successful steps:\n1. Navigate to Add Order page\n2. Select Existing Customer\n3. Add Products\n4. Proceed to Fulfillment\n5. Proceed to Payment\n6. Verify Summary and Add Comments","","Status: Failed","Last Updated: 2025-09-29T08:54:58.095Z","---"]</t>
@@ -48364,32 +48367,32 @@
       <c r="AL11" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="AM11" s="3">
-        <v>434397</v>
+      <c r="AM11" s="3" t="s">
+        <v>3204</v>
       </c>
       <c r="AN11" s="3">
         <v>434398</v>
       </c>
       <c r="AQ11" t="s">
-        <v>3204</v>
+        <v>3205</v>
       </c>
       <c r="AR11" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AS11" s="3" t="s">
-        <v>3205</v>
+        <v>3206</v>
       </c>
       <c r="AT11" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AU11" s="3" t="s">
-        <v>3206</v>
+        <v>3207</v>
       </c>
       <c r="AV11" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AW11" s="3" t="s">
-        <v>3207</v>
+        <v>3208</v>
       </c>
     </row>
     <row r="12" ht="43.2" customHeight="1" spans="1:45" x14ac:dyDescent="0.25">
@@ -48508,16 +48511,16 @@
         <v>0</v>
       </c>
       <c r="AM12" s="3" t="s">
-        <v>3208</v>
+        <v>3209</v>
       </c>
       <c r="AQ12" t="s">
-        <v>3209</v>
+        <v>3210</v>
       </c>
       <c r="AR12" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AS12" s="3" t="s">
-        <v>3210</v>
+        <v>3211</v>
       </c>
     </row>
     <row r="13" ht="43.2" customHeight="1" hidden="1" spans="1:38" x14ac:dyDescent="0.25">
@@ -48917,7 +48920,7 @@
         <v>123</v>
       </c>
       <c r="W20" s="3" t="s">
-        <v>3211</v>
+        <v>3212</v>
       </c>
       <c r="X20" s="3" t="s">
         <v>3186</v>
@@ -48965,13 +48968,13 @@
         <v>0</v>
       </c>
       <c r="AQ20" t="s">
-        <v>3212</v>
+        <v>3213</v>
       </c>
       <c r="AT20" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AU20" s="3" t="s">
-        <v>3213</v>
+        <v>3214</v>
       </c>
     </row>
     <row r="21" ht="43.2" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
@@ -49487,7 +49490,7 @@
         <v>123</v>
       </c>
       <c r="W29" s="3" t="s">
-        <v>3211</v>
+        <v>3212</v>
       </c>
       <c r="X29" s="3" t="s">
         <v>3186</v>
@@ -49535,13 +49538,13 @@
         <v>0</v>
       </c>
       <c r="AQ29" t="s">
-        <v>3214</v>
+        <v>3215</v>
       </c>
       <c r="AT29" s="3" t="s">
         <v>3194</v>
       </c>
       <c r="AU29" s="3" t="s">
-        <v>3215</v>
+        <v>3216</v>
       </c>
     </row>
     <row r="30" ht="43.2" customHeight="1" spans="1:47" x14ac:dyDescent="0.25">
@@ -49660,13 +49663,13 @@
         <v>0</v>
       </c>
       <c r="AQ30" t="s">
-        <v>3216</v>
+        <v>3217</v>
       </c>
       <c r="AT30" s="3" t="s">
         <v>3194</v>
       </c>
       <c r="AU30" s="3" t="s">
-        <v>3217</v>
+        <v>3218</v>
       </c>
     </row>
     <row r="31" ht="43.2" customHeight="1" hidden="1" spans="1:38" x14ac:dyDescent="0.25">
@@ -50066,7 +50069,7 @@
         <v>214</v>
       </c>
       <c r="W38" s="3" t="s">
-        <v>3218</v>
+        <v>3219</v>
       </c>
       <c r="X38" s="3" t="s">
         <v>3186</v>
@@ -50093,10 +50096,10 @@
         <v>3189</v>
       </c>
       <c r="AF38" s="3" t="s">
-        <v>3219</v>
+        <v>3220</v>
       </c>
       <c r="AG38" s="3" t="s">
-        <v>3220</v>
+        <v>3221</v>
       </c>
       <c r="AH38" s="3">
         <v>234234523</v>
@@ -50114,19 +50117,19 @@
         <v>0</v>
       </c>
       <c r="AQ38" t="s">
-        <v>3221</v>
+        <v>3222</v>
       </c>
       <c r="AR38" s="3" t="s">
         <v>3194</v>
       </c>
       <c r="AS38" s="3" t="s">
-        <v>3222</v>
+        <v>3223</v>
       </c>
       <c r="AT38" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AU38" s="3" t="s">
-        <v>3223</v>
+        <v>3224</v>
       </c>
     </row>
     <row r="39" ht="43.2" customHeight="1" spans="1:45" x14ac:dyDescent="0.25">
@@ -50224,10 +50227,10 @@
         <v>3189</v>
       </c>
       <c r="AF39" s="3" t="s">
-        <v>3219</v>
+        <v>3220</v>
       </c>
       <c r="AG39" s="3" t="s">
-        <v>3220</v>
+        <v>3221</v>
       </c>
       <c r="AH39" s="3">
         <v>234234523</v>
@@ -50245,13 +50248,13 @@
         <v>0</v>
       </c>
       <c r="AQ39" t="s">
-        <v>3224</v>
+        <v>3225</v>
       </c>
       <c r="AR39" s="3" t="s">
         <v>3194</v>
       </c>
       <c r="AS39" s="3" t="s">
-        <v>3225</v>
+        <v>3226</v>
       </c>
     </row>
     <row r="40" ht="43.2" customHeight="1" hidden="1" spans="1:38" x14ac:dyDescent="0.25">
@@ -50651,7 +50654,7 @@
         <v>214</v>
       </c>
       <c r="W47" s="3" t="s">
-        <v>3218</v>
+        <v>3219</v>
       </c>
       <c r="X47" s="3" t="s">
         <v>3186</v>
@@ -50678,10 +50681,10 @@
         <v>3189</v>
       </c>
       <c r="AF47" s="3" t="s">
-        <v>3219</v>
+        <v>3220</v>
       </c>
       <c r="AG47" s="3" t="s">
-        <v>3220</v>
+        <v>3221</v>
       </c>
       <c r="AH47" s="3">
         <v>234234523</v>
@@ -50699,19 +50702,19 @@
         <v>0</v>
       </c>
       <c r="AQ47" t="s">
-        <v>3226</v>
+        <v>3227</v>
       </c>
       <c r="AR47" s="3" t="s">
         <v>3194</v>
       </c>
       <c r="AS47" s="3" t="s">
-        <v>3227</v>
+        <v>3228</v>
       </c>
       <c r="AT47" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AU47" s="3" t="s">
-        <v>3228</v>
+        <v>3229</v>
       </c>
     </row>
     <row r="48" ht="43.2" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
@@ -50809,10 +50812,10 @@
         <v>3189</v>
       </c>
       <c r="AF48" s="3" t="s">
-        <v>3219</v>
+        <v>3220</v>
       </c>
       <c r="AG48" s="3" t="s">
-        <v>3220</v>
+        <v>3221</v>
       </c>
       <c r="AH48" s="3">
         <v>234234523</v>
@@ -51224,7 +51227,7 @@
         <v>3182</v>
       </c>
       <c r="V56" s="3" t="s">
-        <v>3229</v>
+        <v>3230</v>
       </c>
       <c r="W56" s="3" t="s">
         <v>3185</v>
@@ -51275,22 +51278,22 @@
         <v>0</v>
       </c>
       <c r="AM56" s="3" t="s">
-        <v>3230</v>
+        <v>3231</v>
       </c>
       <c r="AQ56" t="s">
-        <v>3231</v>
+        <v>3232</v>
       </c>
       <c r="AR56" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AS56" s="3" t="s">
-        <v>3232</v>
+        <v>3233</v>
       </c>
       <c r="AT56" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AU56" s="3" t="s">
-        <v>3233</v>
+        <v>3234</v>
       </c>
     </row>
     <row r="57" ht="43.2" customHeight="1" spans="1:45" x14ac:dyDescent="0.25">
@@ -51358,7 +51361,7 @@
         <v>3182</v>
       </c>
       <c r="V57" s="3" t="s">
-        <v>3229</v>
+        <v>3230</v>
       </c>
       <c r="W57" s="3" t="s">
         <v>3185</v>
@@ -51409,16 +51412,16 @@
         <v>0</v>
       </c>
       <c r="AM57" s="3" t="s">
-        <v>3234</v>
+        <v>3235</v>
       </c>
       <c r="AQ57" t="s">
-        <v>3235</v>
+        <v>3236</v>
       </c>
       <c r="AR57" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AS57" s="3" t="s">
-        <v>3236</v>
+        <v>3237</v>
       </c>
     </row>
     <row r="58" ht="43.2" customHeight="1" hidden="1" spans="1:38" x14ac:dyDescent="0.25">
@@ -51815,7 +51818,7 @@
         <v>3182</v>
       </c>
       <c r="V65" s="3" t="s">
-        <v>3229</v>
+        <v>3230</v>
       </c>
       <c r="W65" s="3" t="s">
         <v>3185</v>
@@ -51866,22 +51869,22 @@
         <v>0</v>
       </c>
       <c r="AM65" s="3" t="s">
-        <v>3237</v>
+        <v>3238</v>
       </c>
       <c r="AQ65" t="s">
-        <v>3238</v>
+        <v>3239</v>
       </c>
       <c r="AR65" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AS65" s="3" t="s">
-        <v>3239</v>
+        <v>3240</v>
       </c>
       <c r="AT65" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AU65" s="3" t="s">
-        <v>3240</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="66" ht="43.2" customHeight="1" spans="1:47" x14ac:dyDescent="0.25">
@@ -51949,7 +51952,7 @@
         <v>3182</v>
       </c>
       <c r="V66" s="3" t="s">
-        <v>3229</v>
+        <v>3230</v>
       </c>
       <c r="W66" s="3" t="s">
         <v>3185</v>
@@ -52000,22 +52003,22 @@
         <v>0</v>
       </c>
       <c r="AM66" s="3" t="s">
-        <v>3241</v>
+        <v>3242</v>
       </c>
       <c r="AQ66" t="s">
-        <v>3242</v>
+        <v>3243</v>
       </c>
       <c r="AR66" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AS66" s="3" t="s">
-        <v>3243</v>
+        <v>3244</v>
       </c>
       <c r="AT66" s="3" t="s">
         <v>3194</v>
       </c>
       <c r="AU66" s="3" t="s">
-        <v>3244</v>
+        <v>3245</v>
       </c>
     </row>
     <row r="67" ht="43.2" customHeight="1" hidden="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -52429,25 +52432,25 @@
         <v>13</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>3245</v>
+        <v>3246</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>3246</v>
+        <v>3247</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>3247</v>
+        <v>3248</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>3248</v>
+        <v>3249</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>3249</v>
+        <v>3250</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>3250</v>
+        <v>3251</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>3251</v>
+        <v>3252</v>
       </c>
       <c r="V1" s="4" t="s">
         <v>3149</v>
@@ -52507,7 +52510,7 @@
         <v>3167</v>
       </c>
       <c r="AO1" s="4" t="s">
-        <v>3252</v>
+        <v>3253</v>
       </c>
       <c r="AP1" s="4" t="s">
         <v>3171</v>
@@ -52561,16 +52564,16 @@
         <v>399</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S2" s="3">
         <v>1</v>
@@ -52603,13 +52606,13 @@
         <v>3182</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD2" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF2" s="9">
         <v>0</v>
@@ -52639,13 +52642,13 @@
         <v>1</v>
       </c>
       <c r="AO2" s="3" t="s">
-        <v>3257</v>
+        <v>3258</v>
       </c>
       <c r="AP2" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AQ2" s="3" t="s">
-        <v>3258</v>
+        <v>3259</v>
       </c>
       <c r="AR2" s="3"/>
     </row>
@@ -52693,16 +52696,16 @@
         <v>405</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S3" s="3">
         <v>1</v>
@@ -52735,13 +52738,13 @@
         <v>3182</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD3" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE3" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF3" s="9">
         <v>0</v>
@@ -52771,13 +52774,13 @@
         <v>1</v>
       </c>
       <c r="AO3" s="3" t="s">
-        <v>3259</v>
+        <v>3260</v>
       </c>
       <c r="AP3" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AQ3" s="3" t="s">
-        <v>3260</v>
+        <v>3261</v>
       </c>
       <c r="AR3" s="3"/>
     </row>
@@ -52825,16 +52828,16 @@
         <v>411</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S4" s="3">
         <v>1</v>
@@ -52911,16 +52914,16 @@
         <v>416</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q5" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S5" s="3">
         <v>1</v>
@@ -52953,13 +52956,13 @@
         <v>3182</v>
       </c>
       <c r="AC5" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD5" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE5" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF5" s="9">
         <v>0</v>
@@ -53021,16 +53024,16 @@
         <v>421</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q6" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S6" s="3">
         <v>1</v>
@@ -53063,13 +53066,13 @@
         <v>3182</v>
       </c>
       <c r="AC6" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD6" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE6" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF6" s="9">
         <v>0</v>
@@ -53131,16 +53134,16 @@
         <v>426</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q7" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S7" s="3">
         <v>1</v>
@@ -53217,16 +53220,16 @@
         <v>431</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q8" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S8" s="3">
         <v>1</v>
@@ -53259,13 +53262,13 @@
         <v>3182</v>
       </c>
       <c r="AC8" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD8" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE8" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF8" s="9">
         <v>0</v>
@@ -53327,16 +53330,16 @@
         <v>436</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q9" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S9" s="3">
         <v>1</v>
@@ -53369,13 +53372,13 @@
         <v>3182</v>
       </c>
       <c r="AC9" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD9" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE9" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF9" s="9">
         <v>0</v>
@@ -53437,16 +53440,16 @@
         <v>441</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q10" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S10" s="3">
         <v>1</v>
@@ -53523,16 +53526,16 @@
         <v>446</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q11" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S11" s="3">
         <v>1</v>
@@ -53565,13 +53568,13 @@
         <v>3202</v>
       </c>
       <c r="AC11" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD11" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE11" s="8" t="s">
-        <v>3261</v>
+        <v>3262</v>
       </c>
       <c r="AF11" s="9">
         <v>0</v>
@@ -53601,13 +53604,13 @@
         <v>1</v>
       </c>
       <c r="AO11" s="3" t="s">
-        <v>3262</v>
+        <v>3263</v>
       </c>
       <c r="AP11" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AQ11" s="3" t="s">
-        <v>3263</v>
+        <v>3264</v>
       </c>
       <c r="AR11" s="3"/>
     </row>
@@ -53655,16 +53658,16 @@
         <v>451</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q12" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S12" s="3">
         <v>1</v>
@@ -53697,13 +53700,13 @@
         <v>3202</v>
       </c>
       <c r="AC12" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD12" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE12" s="8" t="s">
-        <v>3261</v>
+        <v>3262</v>
       </c>
       <c r="AF12" s="9">
         <v>0</v>
@@ -53733,13 +53736,13 @@
         <v>1</v>
       </c>
       <c r="AO12" s="3" t="s">
-        <v>3264</v>
+        <v>3265</v>
       </c>
       <c r="AP12" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AQ12" s="3" t="s">
-        <v>3265</v>
+        <v>3266</v>
       </c>
       <c r="AR12" s="3"/>
     </row>
@@ -53787,16 +53790,16 @@
         <v>456</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q13" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S13" s="3">
         <v>1</v>
@@ -53873,16 +53876,16 @@
         <v>461</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q14" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S14" s="3">
         <v>1</v>
@@ -53915,13 +53918,13 @@
         <v>3182</v>
       </c>
       <c r="AC14" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD14" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE14" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF14" s="9">
         <v>0</v>
@@ -53983,16 +53986,16 @@
         <v>466</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q15" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S15" s="3">
         <v>1</v>
@@ -54025,13 +54028,13 @@
         <v>3182</v>
       </c>
       <c r="AC15" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD15" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE15" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF15" s="9">
         <v>0</v>
@@ -54093,16 +54096,16 @@
         <v>471</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q16" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R16" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S16" s="3">
         <v>1</v>
@@ -54179,16 +54182,16 @@
         <v>476</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q17" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S17" s="3">
         <v>1</v>
@@ -54221,13 +54224,13 @@
         <v>3182</v>
       </c>
       <c r="AC17" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD17" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE17" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF17" s="9">
         <v>0</v>
@@ -54289,16 +54292,16 @@
         <v>481</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q18" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S18" s="3">
         <v>1</v>
@@ -54331,13 +54334,13 @@
         <v>3182</v>
       </c>
       <c r="AC18" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD18" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE18" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF18" s="9">
         <v>0</v>
@@ -54399,16 +54402,16 @@
         <v>486</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q19" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S19" s="3">
         <v>1</v>
@@ -54487,16 +54490,16 @@
         <v>491</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q20" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S20" s="3">
         <v>1</v>
@@ -54520,7 +54523,7 @@
         <v>123</v>
       </c>
       <c r="Z20" s="3" t="s">
-        <v>3211</v>
+        <v>3212</v>
       </c>
       <c r="AA20" s="3" t="s">
         <v>3186</v>
@@ -54529,13 +54532,13 @@
         <v>3182</v>
       </c>
       <c r="AC20" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD20" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE20" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF20" s="9">
         <v>0</v>
@@ -54565,13 +54568,13 @@
         <v>1</v>
       </c>
       <c r="AO20" s="3" t="s">
-        <v>3266</v>
+        <v>3267</v>
       </c>
       <c r="AP20" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AQ20" s="3" t="s">
-        <v>3267</v>
+        <v>3268</v>
       </c>
       <c r="AR20" s="3"/>
     </row>
@@ -54619,16 +54622,16 @@
         <v>496</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q21" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S21" s="3">
         <v>1</v>
@@ -54661,13 +54664,13 @@
         <v>3182</v>
       </c>
       <c r="AC21" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD21" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE21" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF21" s="9">
         <v>0</v>
@@ -54697,13 +54700,13 @@
         <v>1</v>
       </c>
       <c r="AO21" s="3" t="s">
-        <v>3268</v>
+        <v>3269</v>
       </c>
       <c r="AP21" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AQ21" s="3" t="s">
-        <v>3269</v>
+        <v>3270</v>
       </c>
       <c r="AR21" s="3"/>
     </row>
@@ -54751,16 +54754,16 @@
         <v>501</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q22" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S22" s="3">
         <v>1</v>
@@ -54837,16 +54840,16 @@
         <v>506</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q23" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R23" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S23" s="3">
         <v>1</v>
@@ -54879,13 +54882,13 @@
         <v>3182</v>
       </c>
       <c r="AC23" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD23" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE23" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF23" s="9">
         <v>0</v>
@@ -54947,16 +54950,16 @@
         <v>511</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q24" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R24" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S24" s="3">
         <v>1</v>
@@ -54989,13 +54992,13 @@
         <v>3182</v>
       </c>
       <c r="AC24" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD24" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE24" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF24" s="9">
         <v>0</v>
@@ -55057,16 +55060,16 @@
         <v>516</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q25" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R25" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S25" s="3">
         <v>1</v>
@@ -55143,16 +55146,16 @@
         <v>521</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q26" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R26" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S26" s="3">
         <v>1</v>
@@ -55185,13 +55188,13 @@
         <v>3182</v>
       </c>
       <c r="AC26" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD26" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE26" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF26" s="9">
         <v>0</v>
@@ -55253,16 +55256,16 @@
         <v>526</v>
       </c>
       <c r="O27" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q27" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R27" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S27" s="3">
         <v>1</v>
@@ -55295,13 +55298,13 @@
         <v>3182</v>
       </c>
       <c r="AC27" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD27" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE27" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF27" s="9">
         <v>0</v>
@@ -55363,16 +55366,16 @@
         <v>531</v>
       </c>
       <c r="O28" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q28" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R28" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S28" s="3">
         <v>1</v>
@@ -55451,16 +55454,16 @@
         <v>536</v>
       </c>
       <c r="O29" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q29" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R29" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S29" s="3">
         <v>1</v>
@@ -55484,7 +55487,7 @@
         <v>123</v>
       </c>
       <c r="Z29" s="3" t="s">
-        <v>3211</v>
+        <v>3212</v>
       </c>
       <c r="AA29" s="3" t="s">
         <v>3186</v>
@@ -55493,13 +55496,13 @@
         <v>3202</v>
       </c>
       <c r="AC29" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD29" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE29" s="8" t="s">
-        <v>3261</v>
+        <v>3262</v>
       </c>
       <c r="AF29" s="9">
         <v>0</v>
@@ -55529,13 +55532,13 @@
         <v>1</v>
       </c>
       <c r="AO29" s="3" t="s">
-        <v>3270</v>
+        <v>3271</v>
       </c>
       <c r="AP29" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AQ29" s="3" t="s">
-        <v>3271</v>
+        <v>3272</v>
       </c>
       <c r="AR29" s="3"/>
     </row>
@@ -55583,16 +55586,16 @@
         <v>541</v>
       </c>
       <c r="O30" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q30" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R30" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S30" s="3">
         <v>1</v>
@@ -55625,13 +55628,13 @@
         <v>3202</v>
       </c>
       <c r="AC30" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD30" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE30" s="8" t="s">
-        <v>3261</v>
+        <v>3262</v>
       </c>
       <c r="AF30" s="9">
         <v>0</v>
@@ -55661,13 +55664,13 @@
         <v>1</v>
       </c>
       <c r="AO30" s="3" t="s">
-        <v>3272</v>
+        <v>3273</v>
       </c>
       <c r="AP30" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AQ30" s="3" t="s">
-        <v>3273</v>
+        <v>3274</v>
       </c>
       <c r="AR30" s="3"/>
     </row>
@@ -55715,16 +55718,16 @@
         <v>546</v>
       </c>
       <c r="O31" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q31" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R31" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S31" s="3">
         <v>1</v>
@@ -55807,16 +55810,16 @@
         <v>551</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P32" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q32" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R32" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S32" s="3">
         <v>1</v>
@@ -55849,13 +55852,13 @@
         <v>3182</v>
       </c>
       <c r="AC32" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD32" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE32" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF32" s="9">
         <v>0</v>
@@ -55917,16 +55920,16 @@
         <v>556</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P33" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q33" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R33" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S33" s="3">
         <v>1</v>
@@ -55959,13 +55962,13 @@
         <v>3182</v>
       </c>
       <c r="AC33" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD33" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE33" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF33" s="9">
         <v>0</v>
@@ -56027,16 +56030,16 @@
         <v>561</v>
       </c>
       <c r="O34" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q34" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R34" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S34" s="3">
         <v>1</v>
@@ -56119,16 +56122,16 @@
         <v>566</v>
       </c>
       <c r="O35" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q35" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R35" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S35" s="3">
         <v>1</v>
@@ -56161,13 +56164,13 @@
         <v>3182</v>
       </c>
       <c r="AC35" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD35" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE35" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF35" s="9">
         <v>0</v>
@@ -56229,16 +56232,16 @@
         <v>571</v>
       </c>
       <c r="O36" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q36" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R36" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S36" s="3">
         <v>1</v>
@@ -56271,13 +56274,13 @@
         <v>3182</v>
       </c>
       <c r="AC36" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD36" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE36" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF36" s="9">
         <v>0</v>
@@ -56339,16 +56342,16 @@
         <v>576</v>
       </c>
       <c r="O37" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P37" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q37" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R37" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S37" s="3">
         <v>1</v>
@@ -56431,16 +56434,16 @@
         <v>581</v>
       </c>
       <c r="O38" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P38" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q38" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R38" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S38" s="3">
         <v>1</v>
@@ -56464,7 +56467,7 @@
         <v>214</v>
       </c>
       <c r="Z38" s="3" t="s">
-        <v>3218</v>
+        <v>3219</v>
       </c>
       <c r="AA38" s="3" t="s">
         <v>3186</v>
@@ -56473,13 +56476,13 @@
         <v>3182</v>
       </c>
       <c r="AC38" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD38" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE38" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF38" s="9">
         <v>0</v>
@@ -56491,10 +56494,10 @@
         <v>3189</v>
       </c>
       <c r="AI38" s="3" t="s">
-        <v>3219</v>
+        <v>3220</v>
       </c>
       <c r="AJ38" s="3" t="s">
-        <v>3220</v>
+        <v>3221</v>
       </c>
       <c r="AK38" s="3">
         <v>234234523</v>
@@ -56513,7 +56516,7 @@
         <v>3194</v>
       </c>
       <c r="AQ38" s="3" t="s">
-        <v>3274</v>
+        <v>3275</v>
       </c>
       <c r="AR38" s="3"/>
     </row>
@@ -56561,16 +56564,16 @@
         <v>586</v>
       </c>
       <c r="O39" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P39" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q39" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R39" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S39" s="3">
         <v>1</v>
@@ -56594,7 +56597,7 @@
         <v>214</v>
       </c>
       <c r="Z39" s="3" t="s">
-        <v>3218</v>
+        <v>3219</v>
       </c>
       <c r="AA39" s="3" t="s">
         <v>3186</v>
@@ -56603,13 +56606,13 @@
         <v>3182</v>
       </c>
       <c r="AC39" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD39" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE39" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF39" s="9">
         <v>0</v>
@@ -56621,10 +56624,10 @@
         <v>3189</v>
       </c>
       <c r="AI39" s="3" t="s">
-        <v>3219</v>
+        <v>3220</v>
       </c>
       <c r="AJ39" s="3" t="s">
-        <v>3220</v>
+        <v>3221</v>
       </c>
       <c r="AK39" s="3">
         <v>234234523</v>
@@ -56643,7 +56646,7 @@
         <v>3194</v>
       </c>
       <c r="AQ39" s="3" t="s">
-        <v>3275</v>
+        <v>3276</v>
       </c>
       <c r="AR39" s="3"/>
     </row>
@@ -56691,16 +56694,16 @@
         <v>591</v>
       </c>
       <c r="O40" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P40" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q40" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R40" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S40" s="3">
         <v>1</v>
@@ -56783,16 +56786,16 @@
         <v>596</v>
       </c>
       <c r="O41" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P41" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q41" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R41" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S41" s="3">
         <v>1</v>
@@ -56816,7 +56819,7 @@
         <v>214</v>
       </c>
       <c r="Z41" s="3" t="s">
-        <v>3218</v>
+        <v>3219</v>
       </c>
       <c r="AA41" s="3" t="s">
         <v>3186</v>
@@ -56825,13 +56828,13 @@
         <v>3182</v>
       </c>
       <c r="AC41" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD41" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE41" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF41" s="9">
         <v>0</v>
@@ -56843,10 +56846,10 @@
         <v>3189</v>
       </c>
       <c r="AI41" s="3" t="s">
-        <v>3219</v>
+        <v>3220</v>
       </c>
       <c r="AJ41" s="3" t="s">
-        <v>3220</v>
+        <v>3221</v>
       </c>
       <c r="AK41" s="3">
         <v>234234523</v>
@@ -56909,16 +56912,16 @@
         <v>601</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P42" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q42" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R42" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S42" s="3">
         <v>1</v>
@@ -56942,7 +56945,7 @@
         <v>214</v>
       </c>
       <c r="Z42" s="3" t="s">
-        <v>3218</v>
+        <v>3219</v>
       </c>
       <c r="AA42" s="3" t="s">
         <v>3186</v>
@@ -56951,13 +56954,13 @@
         <v>3182</v>
       </c>
       <c r="AC42" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD42" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE42" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF42" s="9">
         <v>0</v>
@@ -56969,10 +56972,10 @@
         <v>3189</v>
       </c>
       <c r="AI42" s="3" t="s">
-        <v>3219</v>
+        <v>3220</v>
       </c>
       <c r="AJ42" s="3" t="s">
-        <v>3220</v>
+        <v>3221</v>
       </c>
       <c r="AK42" s="3">
         <v>234234523</v>
@@ -57035,16 +57038,16 @@
         <v>606</v>
       </c>
       <c r="O43" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P43" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q43" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R43" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S43" s="3">
         <v>1</v>
@@ -57127,16 +57130,16 @@
         <v>611</v>
       </c>
       <c r="O44" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P44" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q44" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R44" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S44" s="3">
         <v>1</v>
@@ -57169,13 +57172,13 @@
         <v>3182</v>
       </c>
       <c r="AC44" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD44" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE44" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF44" s="9">
         <v>0</v>
@@ -57187,10 +57190,10 @@
         <v>3189</v>
       </c>
       <c r="AI44" s="3" t="s">
-        <v>3219</v>
+        <v>3220</v>
       </c>
       <c r="AJ44" s="3" t="s">
-        <v>3220</v>
+        <v>3221</v>
       </c>
       <c r="AK44" s="3">
         <v>234234523</v>
@@ -57253,16 +57256,16 @@
         <v>616</v>
       </c>
       <c r="O45" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P45" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q45" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R45" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S45" s="3">
         <v>1</v>
@@ -57295,13 +57298,13 @@
         <v>3182</v>
       </c>
       <c r="AC45" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD45" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE45" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF45" s="9">
         <v>0</v>
@@ -57313,10 +57316,10 @@
         <v>3189</v>
       </c>
       <c r="AI45" s="3" t="s">
-        <v>3219</v>
+        <v>3220</v>
       </c>
       <c r="AJ45" s="3" t="s">
-        <v>3220</v>
+        <v>3221</v>
       </c>
       <c r="AK45" s="3">
         <v>234234523</v>
@@ -57379,16 +57382,16 @@
         <v>621</v>
       </c>
       <c r="O46" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P46" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q46" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R46" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S46" s="3">
         <v>1</v>
@@ -57471,16 +57474,16 @@
         <v>626</v>
       </c>
       <c r="O47" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P47" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q47" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R47" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S47" s="3">
         <v>1</v>
@@ -57504,7 +57507,7 @@
         <v>214</v>
       </c>
       <c r="Z47" s="3" t="s">
-        <v>3218</v>
+        <v>3219</v>
       </c>
       <c r="AA47" s="3" t="s">
         <v>3186</v>
@@ -57513,13 +57516,13 @@
         <v>3202</v>
       </c>
       <c r="AC47" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD47" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE47" s="8" t="s">
-        <v>3261</v>
+        <v>3262</v>
       </c>
       <c r="AF47" s="9">
         <v>0</v>
@@ -57531,10 +57534,10 @@
         <v>3189</v>
       </c>
       <c r="AI47" s="3" t="s">
-        <v>3219</v>
+        <v>3220</v>
       </c>
       <c r="AJ47" s="3" t="s">
-        <v>3220</v>
+        <v>3221</v>
       </c>
       <c r="AK47" s="3">
         <v>234234523</v>
@@ -57553,7 +57556,7 @@
         <v>3194</v>
       </c>
       <c r="AQ47" s="3" t="s">
-        <v>3276</v>
+        <v>3277</v>
       </c>
       <c r="AR47" s="3"/>
     </row>
@@ -57601,16 +57604,16 @@
         <v>631</v>
       </c>
       <c r="O48" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P48" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q48" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R48" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S48" s="3">
         <v>1</v>
@@ -57634,7 +57637,7 @@
         <v>214</v>
       </c>
       <c r="Z48" s="3" t="s">
-        <v>3218</v>
+        <v>3219</v>
       </c>
       <c r="AA48" s="3" t="s">
         <v>3186</v>
@@ -57643,13 +57646,13 @@
         <v>3202</v>
       </c>
       <c r="AC48" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD48" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE48" s="8" t="s">
-        <v>3261</v>
+        <v>3262</v>
       </c>
       <c r="AF48" s="9">
         <v>0</v>
@@ -57661,10 +57664,10 @@
         <v>3189</v>
       </c>
       <c r="AI48" s="3" t="s">
-        <v>3219</v>
+        <v>3220</v>
       </c>
       <c r="AJ48" s="3" t="s">
-        <v>3220</v>
+        <v>3221</v>
       </c>
       <c r="AK48" s="3">
         <v>234234523</v>
@@ -57683,7 +57686,7 @@
         <v>3194</v>
       </c>
       <c r="AQ48" s="3" t="s">
-        <v>3277</v>
+        <v>3278</v>
       </c>
       <c r="AR48" s="3"/>
     </row>
@@ -57731,10 +57734,10 @@
         <v>636</v>
       </c>
       <c r="O49" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P49" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q49" s="3"/>
       <c r="R49" s="3"/>
@@ -57811,16 +57814,16 @@
         <v>641</v>
       </c>
       <c r="O50" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P50" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q50" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R50" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S50" s="3">
         <v>1</v>
@@ -57844,7 +57847,7 @@
         <v>214</v>
       </c>
       <c r="Z50" s="3" t="s">
-        <v>3218</v>
+        <v>3219</v>
       </c>
       <c r="AA50" s="3" t="s">
         <v>3186</v>
@@ -57853,13 +57856,13 @@
         <v>3182</v>
       </c>
       <c r="AC50" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD50" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE50" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF50" s="9">
         <v>0</v>
@@ -57871,10 +57874,10 @@
         <v>3189</v>
       </c>
       <c r="AI50" s="3" t="s">
-        <v>3219</v>
+        <v>3220</v>
       </c>
       <c r="AJ50" s="3" t="s">
-        <v>3220</v>
+        <v>3221</v>
       </c>
       <c r="AK50" s="3">
         <v>234234523</v>
@@ -57937,16 +57940,16 @@
         <v>646</v>
       </c>
       <c r="O51" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P51" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q51" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R51" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S51" s="3">
         <v>1</v>
@@ -57970,7 +57973,7 @@
         <v>214</v>
       </c>
       <c r="Z51" s="3" t="s">
-        <v>3218</v>
+        <v>3219</v>
       </c>
       <c r="AA51" s="3" t="s">
         <v>3186</v>
@@ -57979,13 +57982,13 @@
         <v>3182</v>
       </c>
       <c r="AC51" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD51" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE51" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF51" s="9">
         <v>0</v>
@@ -57997,10 +58000,10 @@
         <v>3189</v>
       </c>
       <c r="AI51" s="3" t="s">
-        <v>3219</v>
+        <v>3220</v>
       </c>
       <c r="AJ51" s="3" t="s">
-        <v>3220</v>
+        <v>3221</v>
       </c>
       <c r="AK51" s="3">
         <v>234234523</v>
@@ -58063,10 +58066,10 @@
         <v>651</v>
       </c>
       <c r="O52" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P52" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q52" s="3"/>
       <c r="R52" s="3"/>
@@ -58143,16 +58146,16 @@
         <v>656</v>
       </c>
       <c r="O53" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P53" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q53" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R53" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S53" s="3">
         <v>1</v>
@@ -58176,7 +58179,7 @@
         <v>214</v>
       </c>
       <c r="Z53" s="3" t="s">
-        <v>3218</v>
+        <v>3219</v>
       </c>
       <c r="AA53" s="3" t="s">
         <v>3186</v>
@@ -58185,13 +58188,13 @@
         <v>3182</v>
       </c>
       <c r="AC53" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD53" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE53" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF53" s="9">
         <v>0</v>
@@ -58203,10 +58206,10 @@
         <v>3189</v>
       </c>
       <c r="AI53" s="3" t="s">
-        <v>3219</v>
+        <v>3220</v>
       </c>
       <c r="AJ53" s="3" t="s">
-        <v>3220</v>
+        <v>3221</v>
       </c>
       <c r="AK53" s="3">
         <v>234234523</v>
@@ -58269,16 +58272,16 @@
         <v>661</v>
       </c>
       <c r="O54" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P54" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q54" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R54" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S54" s="3">
         <v>1</v>
@@ -58302,7 +58305,7 @@
         <v>214</v>
       </c>
       <c r="Z54" s="3" t="s">
-        <v>3218</v>
+        <v>3219</v>
       </c>
       <c r="AA54" s="3" t="s">
         <v>3186</v>
@@ -58311,13 +58314,13 @@
         <v>3182</v>
       </c>
       <c r="AC54" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD54" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE54" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF54" s="9">
         <v>0</v>
@@ -58329,10 +58332,10 @@
         <v>3189</v>
       </c>
       <c r="AI54" s="3" t="s">
-        <v>3219</v>
+        <v>3220</v>
       </c>
       <c r="AJ54" s="3" t="s">
-        <v>3220</v>
+        <v>3221</v>
       </c>
       <c r="AK54" s="3">
         <v>234234523</v>
@@ -58395,10 +58398,10 @@
         <v>666</v>
       </c>
       <c r="O55" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P55" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q55" s="3"/>
       <c r="R55" s="3"/>
@@ -58475,16 +58478,16 @@
         <v>671</v>
       </c>
       <c r="O56" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P56" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q56" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R56" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S56" s="3">
         <v>1</v>
@@ -58505,7 +58508,7 @@
         <v>3182</v>
       </c>
       <c r="Y56" s="3" t="s">
-        <v>3229</v>
+        <v>3230</v>
       </c>
       <c r="Z56" s="3" t="s">
         <v>3185</v>
@@ -58517,13 +58520,13 @@
         <v>3182</v>
       </c>
       <c r="AC56" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD56" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE56" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF56" s="9">
         <v>0</v>
@@ -58553,13 +58556,13 @@
         <v>1</v>
       </c>
       <c r="AO56" s="3" t="s">
-        <v>3278</v>
+        <v>3279</v>
       </c>
       <c r="AP56" s="3" t="s">
         <v>3194</v>
       </c>
       <c r="AQ56" s="3" t="s">
-        <v>3279</v>
+        <v>3280</v>
       </c>
       <c r="AR56" s="3"/>
     </row>
@@ -58607,16 +58610,16 @@
         <v>676</v>
       </c>
       <c r="O57" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P57" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q57" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R57" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S57" s="3">
         <v>1</v>
@@ -58637,7 +58640,7 @@
         <v>3182</v>
       </c>
       <c r="Y57" s="3" t="s">
-        <v>3229</v>
+        <v>3230</v>
       </c>
       <c r="Z57" s="3" t="s">
         <v>3185</v>
@@ -58649,13 +58652,13 @@
         <v>3182</v>
       </c>
       <c r="AC57" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD57" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE57" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF57" s="9">
         <v>0</v>
@@ -58685,13 +58688,13 @@
         <v>1</v>
       </c>
       <c r="AO57" s="3" t="s">
-        <v>3280</v>
+        <v>3281</v>
       </c>
       <c r="AP57" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AQ57" s="3" t="s">
-        <v>3281</v>
+        <v>3282</v>
       </c>
       <c r="AR57" s="3"/>
     </row>
@@ -58739,10 +58742,10 @@
         <v>681</v>
       </c>
       <c r="O58" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P58" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q58" s="3"/>
       <c r="R58" s="3"/>
@@ -58819,16 +58822,16 @@
         <v>686</v>
       </c>
       <c r="O59" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P59" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q59" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R59" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S59" s="3">
         <v>1</v>
@@ -58849,7 +58852,7 @@
         <v>3182</v>
       </c>
       <c r="Y59" s="3" t="s">
-        <v>3229</v>
+        <v>3230</v>
       </c>
       <c r="Z59" s="3" t="s">
         <v>3185</v>
@@ -58861,13 +58864,13 @@
         <v>3182</v>
       </c>
       <c r="AC59" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD59" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE59" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF59" s="9">
         <v>0</v>
@@ -58945,16 +58948,16 @@
         <v>691</v>
       </c>
       <c r="O60" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P60" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q60" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R60" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S60" s="3">
         <v>1</v>
@@ -58975,7 +58978,7 @@
         <v>3182</v>
       </c>
       <c r="Y60" s="3" t="s">
-        <v>3229</v>
+        <v>3230</v>
       </c>
       <c r="Z60" s="3" t="s">
         <v>3185</v>
@@ -58987,13 +58990,13 @@
         <v>3182</v>
       </c>
       <c r="AC60" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD60" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE60" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF60" s="9">
         <v>0</v>
@@ -59071,10 +59074,10 @@
         <v>696</v>
       </c>
       <c r="O61" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P61" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q61" s="3"/>
       <c r="R61" s="3"/>
@@ -59151,16 +59154,16 @@
         <v>701</v>
       </c>
       <c r="O62" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P62" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q62" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R62" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S62" s="3">
         <v>1</v>
@@ -59181,7 +59184,7 @@
         <v>3182</v>
       </c>
       <c r="Y62" s="3" t="s">
-        <v>3229</v>
+        <v>3230</v>
       </c>
       <c r="Z62" s="3" t="s">
         <v>3185</v>
@@ -59193,13 +59196,13 @@
         <v>3182</v>
       </c>
       <c r="AC62" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD62" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE62" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF62" s="9">
         <v>0</v>
@@ -59277,16 +59280,16 @@
         <v>706</v>
       </c>
       <c r="O63" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P63" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q63" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R63" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S63" s="3">
         <v>1</v>
@@ -59307,7 +59310,7 @@
         <v>3182</v>
       </c>
       <c r="Y63" s="3" t="s">
-        <v>3229</v>
+        <v>3230</v>
       </c>
       <c r="Z63" s="3" t="s">
         <v>3185</v>
@@ -59319,13 +59322,13 @@
         <v>3182</v>
       </c>
       <c r="AC63" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD63" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE63" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AF63" s="9">
         <v>0</v>
@@ -59403,10 +59406,10 @@
         <v>711</v>
       </c>
       <c r="O64" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P64" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q64" s="3"/>
       <c r="R64" s="3"/>
@@ -59483,16 +59486,16 @@
         <v>716</v>
       </c>
       <c r="O65" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P65" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q65" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R65" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S65" s="3">
         <v>1</v>
@@ -59513,7 +59516,7 @@
         <v>3182</v>
       </c>
       <c r="Y65" s="3" t="s">
-        <v>3229</v>
+        <v>3230</v>
       </c>
       <c r="Z65" s="3" t="s">
         <v>3185</v>
@@ -59525,13 +59528,13 @@
         <v>3202</v>
       </c>
       <c r="AC65" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD65" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE65" s="8" t="s">
-        <v>3261</v>
+        <v>3262</v>
       </c>
       <c r="AF65" s="9">
         <v>0</v>
@@ -59561,13 +59564,13 @@
         <v>1</v>
       </c>
       <c r="AO65" s="3" t="s">
-        <v>3282</v>
+        <v>3283</v>
       </c>
       <c r="AP65" s="3" t="s">
         <v>3192</v>
       </c>
       <c r="AQ65" s="3" t="s">
-        <v>3283</v>
+        <v>3284</v>
       </c>
       <c r="AR65" s="3"/>
     </row>
@@ -59615,16 +59618,16 @@
         <v>721</v>
       </c>
       <c r="O66" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P66" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q66" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R66" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S66" s="3">
         <v>1</v>
@@ -59645,7 +59648,7 @@
         <v>3182</v>
       </c>
       <c r="Y66" s="3" t="s">
-        <v>3229</v>
+        <v>3230</v>
       </c>
       <c r="Z66" s="3" t="s">
         <v>3185</v>
@@ -59657,13 +59660,13 @@
         <v>3202</v>
       </c>
       <c r="AC66" s="3" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AD66" s="7" t="s">
         <v>3187</v>
       </c>
       <c r="AE66" s="8" t="s">
-        <v>3261</v>
+        <v>3262</v>
       </c>
       <c r="AF66" s="9">
         <v>0</v>
@@ -59693,13 +59696,13 @@
         <v>1</v>
       </c>
       <c r="AO66" s="3" t="s">
-        <v>3284</v>
+        <v>3285</v>
       </c>
       <c r="AP66" s="3" t="s">
         <v>3194</v>
       </c>
       <c r="AQ66" s="3" t="s">
-        <v>3285</v>
+        <v>3286</v>
       </c>
       <c r="AR66" s="3"/>
     </row>
@@ -59747,7 +59750,7 @@
         <v>726</v>
       </c>
       <c r="O67" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P67" s="3"/>
       <c r="Q67" s="3"/>
@@ -59825,16 +59828,16 @@
         <v>731</v>
       </c>
       <c r="O68" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P68" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q68" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R68" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S68" s="3">
         <v>1</v>
@@ -59919,16 +59922,16 @@
         <v>736</v>
       </c>
       <c r="O69" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P69" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q69" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R69" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S69" s="3">
         <v>1</v>
@@ -60013,7 +60016,7 @@
         <v>741</v>
       </c>
       <c r="O70" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P70" s="3"/>
       <c r="Q70" s="3"/>
@@ -60091,16 +60094,16 @@
         <v>746</v>
       </c>
       <c r="O71" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P71" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q71" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R71" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S71" s="3">
         <v>1</v>
@@ -60185,16 +60188,16 @@
         <v>751</v>
       </c>
       <c r="O72" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P72" s="3" t="s">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="Q72" s="3" t="s">
         <v>3180</v>
       </c>
       <c r="R72" s="3" t="s">
-        <v>3255</v>
+        <v>3256</v>
       </c>
       <c r="S72" s="3">
         <v>1</v>
@@ -60279,7 +60282,7 @@
         <v>756</v>
       </c>
       <c r="O73" s="3" t="s">
-        <v>3253</v>
+        <v>3254</v>
       </c>
       <c r="P73" s="3"/>
       <c r="Q73" s="3"/>

</xml_diff>